<commit_message>
fleshed out elemental affinities, and started to add descriptions to materials.
</commit_message>
<xml_diff>
--- a/Tags and Affinities.xlsx
+++ b/Tags and Affinities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CK.DESKTOP-BR5NVLN\Documents\Git Repositories\Creative\materials_and_crafting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44FDD01-17B7-4442-9FE9-41C948F51F82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53031307-48AE-491C-B43C-0FAAEC6B96E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{8FD76562-234B-40A6-8AC6-52675E21BBDC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{8FD76562-234B-40A6-8AC6-52675E21BBDC}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPONENT TAGS" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="366">
   <si>
     <t>This component's weapon can be wound up in preparation for a powerful strike, however its strikes take a while to rewind.</t>
   </si>
@@ -1837,6 +1837,81 @@
   </si>
   <si>
     <t>This material increases the emission radius of enchantment spells that conduct through it by a number of inches equal to its nyxian affinity.</t>
+  </si>
+  <si>
+    <t>Movement causes tremors</t>
+  </si>
+  <si>
+    <t>Flask stores soul</t>
+  </si>
+  <si>
+    <t>Random movement size</t>
+  </si>
+  <si>
+    <t>Random AC</t>
+  </si>
+  <si>
+    <t>This helmet thrashes with volatile elemental energy. Whenever you roll damage on a breath weapon while wearing this helmet, roll a 1d10 for each damage type in this list.
+1 / Acid
+2 / Cold
+3 / Fire
+4 / Force
+5 / Lightning
+6 / Poison
+7 / Psychic
+8 / Thunder
+9 / Radiant
+10 / Necrotic
+Replace each of your damage types with the types you obtained from their rolls.</t>
+  </si>
+  <si>
+    <t>When you make an attack with this weapon, you can charge your weapon with radiant energy, firing a blasting wave of light that illuminates all things.
+The space you target is the origin of the wave, which must be directed away from you (when applicable). You choose the form of the wave’s area from the following options:
+ • A 5-foot-wide line with a length of 10 feet per luthian affinity.
+ • A cone of size 5 feet per luthian affinity.
+ • A radius-area 10 feet per 3 luthian affinity centered on the point of impact.
+All creatures (except you) within the affected area must succeed on a Constitution saving throw equal to 10 + (2 * luthian affinity) or take 2d10 points of radiant damage per luthian affinity, bathed in an illuminating light. A successful saving throw halves the damage and prevents the illumination. This illuminating light forces disadvantage on Stealth checks to hide, and nullifies invisibility.
+Once this ability has been used, it can no longer be used until the weapon has spent a long rest bathed in the energies of a holy site.</t>
+  </si>
+  <si>
+    <t>As a reaction when you take damage or when you die, you may explode in blazing wings of phoenix flame.
+Each creature within a radius 10 times this cloak's ignan affinity must make a Dexterity saving throw equal to 10 + (2 * ignan affinity) or take 1d10 fire damage per ignan affinity and be set aflame at a grade equal to the cloak's ignan affinity.
+The explosion reduces you to 0 hit points if you are not dead, and incases you in an glowing obsidian egg, granting you total cover from all effects outside of it. The egg is resistant to all damage,  has hit points equal to 10 times the cloak's ignan affinity, and has an AC of 8 + ignan affinity. While you are incased in this egg, you regain hit points equal to the cloak's ignan affinity at the start of each of your turns.
+Once this ability has been used, it can no longer be used until the weapon has spent a long rest bathed in magma.</t>
+  </si>
+  <si>
+    <t>When ingested, this potion grants resistance to radiant damage.</t>
+  </si>
+  <si>
+    <t>When ingested, this potion grants resistance to lightning damage.</t>
+  </si>
+  <si>
+    <t>When ingested, this potion grants resistance to poison and acid damage.</t>
+  </si>
+  <si>
+    <t>When ingested, this potion grants resistance to cold damage.</t>
+  </si>
+  <si>
+    <t>When ingested, this potion grants resistance to fire damage.</t>
+  </si>
+  <si>
+    <t>When ingested, this potion grants resistance to necrotic damage.</t>
+  </si>
+  <si>
+    <t>When ingested, this potion grants resistance to psychic damage.</t>
+  </si>
+  <si>
+    <t>When ingested, this potion grants resistance to force damage.</t>
+  </si>
+  <si>
+    <t>While you wear this helmet, you have truesight at a radius equal to 10 times its auran affinity.</t>
+  </si>
+  <si>
+    <t>While you wear these boots, you gain the ability to step from one shadow into another.
+When you are in dim light or darkness, as a bonus action you can teleport out to a radius equal to 20 times these boots' erebian affinity to an unoccupied space you can see that is also in dim light or darkness.</t>
+  </si>
+  <si>
+    <t>As an action while you wield this staff, you may conjure a large wave of water that pushes all creatures in a line.</t>
   </si>
 </sst>
 </file>
@@ -1886,7 +1961,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="71">
+  <borders count="72">
     <border>
       <left/>
       <right/>
@@ -2749,8 +2824,27 @@
       <left style="thin">
         <color theme="0" tint="-0.34998626667073579"/>
       </left>
-      <right/>
-      <top/>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -2760,7 +2854,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3025,9 +3119,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3060,15 +3151,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="70" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3078,6 +3169,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3086,6 +3213,117 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -3099,214 +3337,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="70" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="71" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="70" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3628,7 +3743,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3950,7 +4065,7 @@
       <c r="J16" s="44"/>
     </row>
     <row r="17" spans="1:10" s="73" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="93" t="s">
+      <c r="A17" s="92" t="s">
         <v>234</v>
       </c>
       <c r="B17" s="23" t="s">
@@ -3976,15 +4091,15 @@
       <c r="B18" s="77" t="s">
         <v>318</v>
       </c>
-      <c r="C18" s="110" t="s">
+      <c r="C18" s="109" t="s">
         <v>319</v>
       </c>
-      <c r="D18" s="111"/>
-      <c r="E18" s="111"/>
-      <c r="F18" s="111"/>
-      <c r="G18" s="111"/>
-      <c r="H18" s="111"/>
-      <c r="I18" s="112"/>
+      <c r="D18" s="110"/>
+      <c r="E18" s="110"/>
+      <c r="F18" s="110"/>
+      <c r="G18" s="110"/>
+      <c r="H18" s="110"/>
+      <c r="I18" s="111"/>
       <c r="J18" s="35"/>
     </row>
   </sheetData>
@@ -4001,10 +4116,10 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4:G4"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4056,47 +4171,47 @@
       <c r="B2" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="C2" s="153" t="s">
+      <c r="C2" s="134" t="s">
         <v>185</v>
       </c>
-      <c r="D2" s="154"/>
-      <c r="E2" s="154"/>
-      <c r="F2" s="154"/>
-      <c r="G2" s="154"/>
-      <c r="H2" s="154"/>
-      <c r="I2" s="155"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="136"/>
       <c r="J2" s="78"/>
     </row>
     <row r="3" spans="1:10" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="116" t="s">
+      <c r="A3" s="164" t="s">
         <v>184</v>
       </c>
-      <c r="B3" s="118" t="s">
+      <c r="B3" s="166" t="s">
         <v>260</v>
       </c>
-      <c r="C3" s="113" t="s">
+      <c r="C3" s="124" t="s">
         <v>320</v>
       </c>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="115"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="126"/>
     </row>
     <row r="4" spans="1:10" s="18" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A4" s="117"/>
-      <c r="B4" s="119"/>
+      <c r="A4" s="165"/>
+      <c r="B4" s="167"/>
       <c r="C4" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="D4" s="141" t="s">
+      <c r="D4" s="147" t="s">
         <v>182</v>
       </c>
-      <c r="E4" s="141"/>
-      <c r="F4" s="141"/>
-      <c r="G4" s="141"/>
+      <c r="E4" s="147"/>
+      <c r="F4" s="147"/>
+      <c r="G4" s="147"/>
       <c r="H4" s="54" t="s">
         <v>181</v>
       </c>
@@ -4112,15 +4227,15 @@
       <c r="B5" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C5" s="113" t="s">
+      <c r="C5" s="124" t="s">
         <v>178</v>
       </c>
-      <c r="D5" s="114"/>
-      <c r="E5" s="114"/>
-      <c r="F5" s="114"/>
-      <c r="G5" s="114"/>
-      <c r="H5" s="114"/>
-      <c r="I5" s="115"/>
+      <c r="D5" s="125"/>
+      <c r="E5" s="125"/>
+      <c r="F5" s="125"/>
+      <c r="G5" s="125"/>
+      <c r="H5" s="125"/>
+      <c r="I5" s="126"/>
       <c r="J5" s="80"/>
     </row>
     <row r="6" spans="1:10" s="18" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -4131,12 +4246,12 @@
         <v>259</v>
       </c>
       <c r="C6" s="31"/>
-      <c r="D6" s="141" t="s">
+      <c r="D6" s="147" t="s">
         <v>177</v>
       </c>
-      <c r="E6" s="141"/>
-      <c r="F6" s="141"/>
-      <c r="G6" s="141"/>
+      <c r="E6" s="147"/>
+      <c r="F6" s="147"/>
+      <c r="G6" s="147"/>
       <c r="H6" s="54" t="s">
         <v>176</v>
       </c>
@@ -4152,15 +4267,15 @@
       <c r="B7" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C7" s="113" t="s">
+      <c r="C7" s="124" t="s">
         <v>173</v>
       </c>
-      <c r="D7" s="114"/>
-      <c r="E7" s="114"/>
-      <c r="F7" s="114"/>
-      <c r="G7" s="114"/>
-      <c r="H7" s="114"/>
-      <c r="I7" s="115"/>
+      <c r="D7" s="125"/>
+      <c r="E7" s="125"/>
+      <c r="F7" s="125"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="126"/>
       <c r="J7" s="80"/>
     </row>
     <row r="8" spans="1:10" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -4170,16 +4285,16 @@
       <c r="B8" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="C8" s="113" t="s">
+      <c r="C8" s="124" t="s">
         <v>171</v>
       </c>
-      <c r="D8" s="114"/>
-      <c r="E8" s="114"/>
-      <c r="F8" s="114"/>
-      <c r="G8" s="114"/>
-      <c r="H8" s="114"/>
-      <c r="I8" s="114"/>
-      <c r="J8" s="115"/>
+      <c r="D8" s="125"/>
+      <c r="E8" s="125"/>
+      <c r="F8" s="125"/>
+      <c r="G8" s="125"/>
+      <c r="H8" s="125"/>
+      <c r="I8" s="125"/>
+      <c r="J8" s="126"/>
     </row>
     <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="42" t="s">
@@ -4188,15 +4303,15 @@
       <c r="B9" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="C9" s="113" t="s">
+      <c r="C9" s="124" t="s">
         <v>169</v>
       </c>
-      <c r="D9" s="114"/>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
-      <c r="G9" s="114"/>
-      <c r="H9" s="114"/>
-      <c r="I9" s="115"/>
+      <c r="D9" s="125"/>
+      <c r="E9" s="125"/>
+      <c r="F9" s="125"/>
+      <c r="G9" s="125"/>
+      <c r="H9" s="125"/>
+      <c r="I9" s="126"/>
       <c r="J9" s="59"/>
     </row>
     <row r="10" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -4206,14 +4321,14 @@
       <c r="B10" s="69" t="s">
         <v>261</v>
       </c>
-      <c r="C10" s="113" t="s">
+      <c r="C10" s="124" t="s">
         <v>263</v>
       </c>
-      <c r="D10" s="114"/>
-      <c r="E10" s="114"/>
-      <c r="F10" s="114"/>
-      <c r="G10" s="114"/>
-      <c r="H10" s="115"/>
+      <c r="D10" s="125"/>
+      <c r="E10" s="125"/>
+      <c r="F10" s="125"/>
+      <c r="G10" s="125"/>
+      <c r="H10" s="126"/>
       <c r="I10" s="4"/>
       <c r="J10" s="70" t="s">
         <v>262</v>
@@ -4243,7 +4358,7 @@
       <c r="I11" s="61" t="s">
         <v>246</v>
       </c>
-      <c r="J11" s="120"/>
+      <c r="J11" s="127"/>
     </row>
     <row r="12" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
@@ -4255,15 +4370,15 @@
       <c r="C12" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="D12" s="126"/>
-      <c r="E12" s="127"/>
-      <c r="F12" s="128"/>
-      <c r="G12" s="128"/>
-      <c r="H12" s="128"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="158"/>
+      <c r="G12" s="158"/>
+      <c r="H12" s="158"/>
       <c r="I12" s="61" t="s">
         <v>294</v>
       </c>
-      <c r="J12" s="121"/>
+      <c r="J12" s="162"/>
     </row>
     <row r="13" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
@@ -4291,20 +4406,20 @@
       <c r="I13" s="60" t="s">
         <v>241</v>
       </c>
-      <c r="J13" s="121"/>
+      <c r="J13" s="162"/>
     </row>
     <row r="14" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="142" t="s">
+      <c r="A14" s="168" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="143" t="s">
+      <c r="B14" s="154" t="s">
         <v>157</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="D14" s="126"/>
-      <c r="E14" s="137"/>
+      <c r="D14" s="112"/>
+      <c r="E14" s="113"/>
       <c r="F14" s="32" t="s">
         <v>238</v>
       </c>
@@ -4315,34 +4430,34 @@
       <c r="I14" s="63" t="s">
         <v>243</v>
       </c>
-      <c r="J14" s="121"/>
+      <c r="J14" s="162"/>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="142"/>
-      <c r="B15" s="143"/>
-      <c r="C15" s="156" t="s">
+      <c r="A15" s="168"/>
+      <c r="B15" s="154"/>
+      <c r="C15" s="143" t="s">
         <v>155</v>
       </c>
-      <c r="D15" s="157"/>
-      <c r="E15" s="157"/>
-      <c r="F15" s="157"/>
-      <c r="G15" s="157"/>
-      <c r="H15" s="157"/>
-      <c r="I15" s="158"/>
-      <c r="J15" s="121"/>
+      <c r="D15" s="144"/>
+      <c r="E15" s="144"/>
+      <c r="F15" s="144"/>
+      <c r="G15" s="144"/>
+      <c r="H15" s="144"/>
+      <c r="I15" s="145"/>
+      <c r="J15" s="162"/>
     </row>
     <row r="16" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="168" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="143" t="s">
+      <c r="B16" s="154" t="s">
         <v>154</v>
       </c>
       <c r="C16" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="D16" s="129"/>
-      <c r="E16" s="130"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="142"/>
       <c r="F16" s="60" t="s">
         <v>152</v>
       </c>
@@ -4353,21 +4468,21 @@
       <c r="I16" s="64" t="s">
         <v>244</v>
       </c>
-      <c r="J16" s="121"/>
+      <c r="J16" s="162"/>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="142"/>
-      <c r="B17" s="144"/>
-      <c r="C17" s="159" t="s">
+      <c r="A17" s="168"/>
+      <c r="B17" s="169"/>
+      <c r="C17" s="146" t="s">
         <v>151</v>
       </c>
-      <c r="D17" s="141"/>
-      <c r="E17" s="141"/>
-      <c r="F17" s="141"/>
-      <c r="G17" s="141"/>
-      <c r="H17" s="141"/>
-      <c r="I17" s="141"/>
-      <c r="J17" s="122"/>
+      <c r="D17" s="147"/>
+      <c r="E17" s="147"/>
+      <c r="F17" s="147"/>
+      <c r="G17" s="147"/>
+      <c r="H17" s="147"/>
+      <c r="I17" s="147"/>
+      <c r="J17" s="128"/>
     </row>
     <row r="18" spans="1:10" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="90" t="s">
@@ -4376,13 +4491,13 @@
       <c r="B18" s="91" t="s">
         <v>315</v>
       </c>
-      <c r="C18" s="131"/>
-      <c r="D18" s="132"/>
-      <c r="E18" s="132"/>
-      <c r="F18" s="132"/>
-      <c r="G18" s="132"/>
-      <c r="H18" s="132"/>
-      <c r="I18" s="130"/>
+      <c r="C18" s="163"/>
+      <c r="D18" s="141"/>
+      <c r="E18" s="141"/>
+      <c r="F18" s="141"/>
+      <c r="G18" s="141"/>
+      <c r="H18" s="141"/>
+      <c r="I18" s="142"/>
       <c r="J18" s="46" t="s">
         <v>313</v>
       </c>
@@ -4394,14 +4509,14 @@
       <c r="B19" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="C19" s="113" t="s">
+      <c r="C19" s="124" t="s">
         <v>279</v>
       </c>
-      <c r="D19" s="114"/>
-      <c r="E19" s="114"/>
-      <c r="F19" s="114"/>
-      <c r="G19" s="114"/>
-      <c r="H19" s="115"/>
+      <c r="D19" s="125"/>
+      <c r="E19" s="125"/>
+      <c r="F19" s="125"/>
+      <c r="G19" s="125"/>
+      <c r="H19" s="126"/>
       <c r="I19" s="81"/>
       <c r="J19" s="62" t="s">
         <v>280</v>
@@ -4414,16 +4529,16 @@
       <c r="B20" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C20" s="123" t="s">
+      <c r="C20" s="114" t="s">
         <v>146</v>
       </c>
-      <c r="D20" s="124"/>
-      <c r="E20" s="124"/>
-      <c r="F20" s="124"/>
-      <c r="G20" s="124"/>
-      <c r="H20" s="124"/>
-      <c r="I20" s="124"/>
-      <c r="J20" s="125"/>
+      <c r="D20" s="115"/>
+      <c r="E20" s="115"/>
+      <c r="F20" s="115"/>
+      <c r="G20" s="115"/>
+      <c r="H20" s="115"/>
+      <c r="I20" s="115"/>
+      <c r="J20" s="116"/>
     </row>
     <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
@@ -4432,16 +4547,16 @@
       <c r="B21" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="C21" s="123" t="s">
+      <c r="C21" s="114" t="s">
         <v>143</v>
       </c>
-      <c r="D21" s="124"/>
-      <c r="E21" s="124"/>
-      <c r="F21" s="124"/>
-      <c r="G21" s="124"/>
-      <c r="H21" s="124"/>
-      <c r="I21" s="124"/>
-      <c r="J21" s="125"/>
+      <c r="D21" s="115"/>
+      <c r="E21" s="115"/>
+      <c r="F21" s="115"/>
+      <c r="G21" s="115"/>
+      <c r="H21" s="115"/>
+      <c r="I21" s="115"/>
+      <c r="J21" s="116"/>
     </row>
     <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
@@ -4450,16 +4565,16 @@
       <c r="B22" s="40" t="s">
         <v>200</v>
       </c>
-      <c r="C22" s="123" t="s">
+      <c r="C22" s="114" t="s">
         <v>201</v>
       </c>
-      <c r="D22" s="124"/>
-      <c r="E22" s="124"/>
-      <c r="F22" s="124"/>
-      <c r="G22" s="124"/>
-      <c r="H22" s="124"/>
-      <c r="I22" s="124"/>
-      <c r="J22" s="125"/>
+      <c r="D22" s="115"/>
+      <c r="E22" s="115"/>
+      <c r="F22" s="115"/>
+      <c r="G22" s="115"/>
+      <c r="H22" s="115"/>
+      <c r="I22" s="115"/>
+      <c r="J22" s="116"/>
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
@@ -4468,16 +4583,16 @@
       <c r="B23" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="C23" s="123" t="s">
+      <c r="C23" s="114" t="s">
         <v>140</v>
       </c>
-      <c r="D23" s="124"/>
-      <c r="E23" s="124"/>
-      <c r="F23" s="124"/>
-      <c r="G23" s="124"/>
-      <c r="H23" s="124"/>
-      <c r="I23" s="124"/>
-      <c r="J23" s="125"/>
+      <c r="D23" s="115"/>
+      <c r="E23" s="115"/>
+      <c r="F23" s="115"/>
+      <c r="G23" s="115"/>
+      <c r="H23" s="115"/>
+      <c r="I23" s="115"/>
+      <c r="J23" s="116"/>
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
@@ -4486,16 +4601,16 @@
       <c r="B24" s="40" t="s">
         <v>203</v>
       </c>
-      <c r="C24" s="123" t="s">
+      <c r="C24" s="114" t="s">
         <v>204</v>
       </c>
-      <c r="D24" s="124"/>
-      <c r="E24" s="124"/>
-      <c r="F24" s="124"/>
-      <c r="G24" s="124"/>
-      <c r="H24" s="124"/>
-      <c r="I24" s="124"/>
-      <c r="J24" s="125"/>
+      <c r="D24" s="115"/>
+      <c r="E24" s="115"/>
+      <c r="F24" s="115"/>
+      <c r="G24" s="115"/>
+      <c r="H24" s="115"/>
+      <c r="I24" s="115"/>
+      <c r="J24" s="116"/>
     </row>
     <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
@@ -4504,16 +4619,16 @@
       <c r="B25" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="C25" s="123" t="s">
+      <c r="C25" s="114" t="s">
         <v>137</v>
       </c>
-      <c r="D25" s="124"/>
-      <c r="E25" s="124"/>
-      <c r="F25" s="124"/>
-      <c r="G25" s="124"/>
-      <c r="H25" s="124"/>
-      <c r="I25" s="124"/>
-      <c r="J25" s="125"/>
+      <c r="D25" s="115"/>
+      <c r="E25" s="115"/>
+      <c r="F25" s="115"/>
+      <c r="G25" s="115"/>
+      <c r="H25" s="115"/>
+      <c r="I25" s="115"/>
+      <c r="J25" s="116"/>
     </row>
     <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
@@ -4522,16 +4637,16 @@
       <c r="B26" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="C26" s="123" t="s">
+      <c r="C26" s="114" t="s">
         <v>134</v>
       </c>
-      <c r="D26" s="124"/>
-      <c r="E26" s="124"/>
-      <c r="F26" s="124"/>
-      <c r="G26" s="124"/>
-      <c r="H26" s="124"/>
-      <c r="I26" s="124"/>
-      <c r="J26" s="125"/>
+      <c r="D26" s="115"/>
+      <c r="E26" s="115"/>
+      <c r="F26" s="115"/>
+      <c r="G26" s="115"/>
+      <c r="H26" s="115"/>
+      <c r="I26" s="115"/>
+      <c r="J26" s="116"/>
     </row>
     <row r="27" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="39" t="s">
@@ -4550,8 +4665,8 @@
       <c r="F27" s="45" t="s">
         <v>208</v>
       </c>
-      <c r="G27" s="151"/>
-      <c r="H27" s="152"/>
+      <c r="G27" s="156"/>
+      <c r="H27" s="157"/>
       <c r="I27" s="36" t="s">
         <v>295</v>
       </c>
@@ -4566,16 +4681,16 @@
       <c r="B28" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="C28" s="138" t="s">
+      <c r="C28" s="159" t="s">
         <v>128</v>
       </c>
-      <c r="D28" s="139"/>
-      <c r="E28" s="139"/>
-      <c r="F28" s="139"/>
-      <c r="G28" s="139"/>
-      <c r="H28" s="139"/>
-      <c r="I28" s="139"/>
-      <c r="J28" s="140"/>
+      <c r="D28" s="160"/>
+      <c r="E28" s="160"/>
+      <c r="F28" s="160"/>
+      <c r="G28" s="160"/>
+      <c r="H28" s="160"/>
+      <c r="I28" s="160"/>
+      <c r="J28" s="161"/>
     </row>
     <row r="29" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
@@ -4584,16 +4699,16 @@
       <c r="B29" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="C29" s="145" t="s">
+      <c r="C29" s="139" t="s">
         <v>125</v>
       </c>
-      <c r="D29" s="146"/>
-      <c r="E29" s="146"/>
-      <c r="F29" s="146"/>
-      <c r="G29" s="146"/>
-      <c r="H29" s="146"/>
-      <c r="I29" s="147"/>
-      <c r="J29" s="120"/>
+      <c r="D29" s="152"/>
+      <c r="E29" s="152"/>
+      <c r="F29" s="152"/>
+      <c r="G29" s="152"/>
+      <c r="H29" s="152"/>
+      <c r="I29" s="153"/>
+      <c r="J29" s="127"/>
     </row>
     <row r="30" spans="1:10" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="34" t="s">
@@ -4605,19 +4720,19 @@
       <c r="C30" s="53" t="s">
         <v>122</v>
       </c>
-      <c r="D30" s="149"/>
-      <c r="E30" s="150"/>
+      <c r="D30" s="132"/>
+      <c r="E30" s="133"/>
       <c r="F30" s="41" t="s">
         <v>121</v>
       </c>
       <c r="G30" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="H30" s="129"/>
+      <c r="H30" s="155"/>
       <c r="I30" s="61" t="s">
         <v>248</v>
       </c>
-      <c r="J30" s="121"/>
+      <c r="J30" s="162"/>
     </row>
     <row r="31" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
@@ -4641,11 +4756,11 @@
       <c r="G31" s="60" t="s">
         <v>113</v>
       </c>
-      <c r="H31" s="148"/>
+      <c r="H31" s="122"/>
       <c r="I31" s="61" t="s">
         <v>250</v>
       </c>
-      <c r="J31" s="122"/>
+      <c r="J31" s="128"/>
     </row>
     <row r="32" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
@@ -4654,14 +4769,14 @@
       <c r="B32" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="C32" s="123" t="s">
+      <c r="C32" s="114" t="s">
         <v>218</v>
       </c>
-      <c r="D32" s="124"/>
-      <c r="E32" s="124"/>
-      <c r="F32" s="124"/>
-      <c r="G32" s="124"/>
-      <c r="H32" s="125"/>
+      <c r="D32" s="115"/>
+      <c r="E32" s="115"/>
+      <c r="F32" s="115"/>
+      <c r="G32" s="115"/>
+      <c r="H32" s="116"/>
       <c r="I32" s="83"/>
       <c r="J32" s="70" t="s">
         <v>251</v>
@@ -4674,14 +4789,14 @@
       <c r="B33" s="23" t="s">
         <v>253</v>
       </c>
-      <c r="C33" s="123" t="s">
+      <c r="C33" s="114" t="s">
         <v>255</v>
       </c>
-      <c r="D33" s="124"/>
-      <c r="E33" s="124"/>
-      <c r="F33" s="124"/>
-      <c r="G33" s="124"/>
-      <c r="H33" s="125"/>
+      <c r="D33" s="115"/>
+      <c r="E33" s="115"/>
+      <c r="F33" s="115"/>
+      <c r="G33" s="115"/>
+      <c r="H33" s="116"/>
       <c r="I33" s="84"/>
       <c r="J33" s="70" t="s">
         <v>254</v>
@@ -4694,14 +4809,14 @@
       <c r="B34" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="C34" s="124" t="s">
+      <c r="C34" s="115" t="s">
         <v>215</v>
       </c>
-      <c r="D34" s="124"/>
-      <c r="E34" s="124"/>
-      <c r="F34" s="124"/>
-      <c r="G34" s="124"/>
-      <c r="H34" s="124"/>
+      <c r="D34" s="115"/>
+      <c r="E34" s="115"/>
+      <c r="F34" s="115"/>
+      <c r="G34" s="115"/>
+      <c r="H34" s="115"/>
       <c r="I34" s="84"/>
       <c r="J34" s="61" t="s">
         <v>296</v>
@@ -4747,8 +4862,8 @@
       <c r="C36" s="50" t="s">
         <v>104</v>
       </c>
-      <c r="D36" s="129"/>
-      <c r="E36" s="130"/>
+      <c r="D36" s="155"/>
+      <c r="E36" s="142"/>
       <c r="F36" s="21" t="s">
         <v>103</v>
       </c>
@@ -4768,15 +4883,15 @@
       <c r="B37" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C37" s="163"/>
-      <c r="D37" s="127"/>
+      <c r="C37" s="117"/>
+      <c r="D37" s="118"/>
       <c r="E37" s="63" t="s">
         <v>273</v>
       </c>
-      <c r="F37" s="148"/>
-      <c r="G37" s="127"/>
-      <c r="H37" s="127"/>
-      <c r="I37" s="167"/>
+      <c r="F37" s="122"/>
+      <c r="G37" s="118"/>
+      <c r="H37" s="118"/>
+      <c r="I37" s="123"/>
       <c r="J37" s="61" t="s">
         <v>272</v>
       </c>
@@ -4791,10 +4906,10 @@
       <c r="C38" s="50" t="s">
         <v>205</v>
       </c>
-      <c r="D38" s="126"/>
-      <c r="E38" s="128"/>
-      <c r="F38" s="128"/>
-      <c r="G38" s="137"/>
+      <c r="D38" s="112"/>
+      <c r="E38" s="158"/>
+      <c r="F38" s="158"/>
+      <c r="G38" s="113"/>
       <c r="H38" s="21" t="s">
         <v>206</v>
       </c>
@@ -4806,60 +4921,60 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="133" t="s">
+      <c r="A39" s="137" t="s">
         <v>97</v>
       </c>
-      <c r="B39" s="135" t="s">
+      <c r="B39" s="148" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="123" t="s">
+      <c r="C39" s="114" t="s">
         <v>95</v>
       </c>
-      <c r="D39" s="124"/>
-      <c r="E39" s="124"/>
-      <c r="F39" s="124"/>
-      <c r="G39" s="124"/>
-      <c r="H39" s="124"/>
+      <c r="D39" s="115"/>
+      <c r="E39" s="115"/>
+      <c r="F39" s="115"/>
+      <c r="G39" s="115"/>
+      <c r="H39" s="115"/>
       <c r="I39" s="68" t="s">
         <v>265</v>
       </c>
       <c r="J39" s="59"/>
     </row>
     <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="134"/>
-      <c r="B40" s="136"/>
-      <c r="C40" s="113" t="s">
+      <c r="A40" s="138"/>
+      <c r="B40" s="140"/>
+      <c r="C40" s="124" t="s">
         <v>94</v>
       </c>
-      <c r="D40" s="114"/>
-      <c r="E40" s="114"/>
-      <c r="F40" s="114"/>
-      <c r="G40" s="114"/>
-      <c r="H40" s="114"/>
-      <c r="I40" s="114"/>
-      <c r="J40" s="115"/>
+      <c r="D40" s="125"/>
+      <c r="E40" s="125"/>
+      <c r="F40" s="125"/>
+      <c r="G40" s="125"/>
+      <c r="H40" s="125"/>
+      <c r="I40" s="125"/>
+      <c r="J40" s="126"/>
     </row>
     <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="133" t="s">
+      <c r="A41" s="137" t="s">
         <v>219</v>
       </c>
-      <c r="B41" s="135" t="s">
+      <c r="B41" s="148" t="s">
         <v>227</v>
       </c>
-      <c r="C41" s="113" t="s">
+      <c r="C41" s="124" t="s">
         <v>221</v>
       </c>
-      <c r="D41" s="114"/>
-      <c r="E41" s="114"/>
-      <c r="F41" s="114"/>
-      <c r="G41" s="114"/>
-      <c r="H41" s="114"/>
-      <c r="I41" s="114"/>
-      <c r="J41" s="115"/>
+      <c r="D41" s="125"/>
+      <c r="E41" s="125"/>
+      <c r="F41" s="125"/>
+      <c r="G41" s="125"/>
+      <c r="H41" s="125"/>
+      <c r="I41" s="125"/>
+      <c r="J41" s="126"/>
     </row>
     <row r="42" spans="1:10" ht="285" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="134"/>
-      <c r="B42" s="156"/>
+      <c r="A42" s="138"/>
+      <c r="B42" s="143"/>
       <c r="C42" s="53" t="s">
         <v>222</v>
       </c>
@@ -4908,8 +5023,8 @@
       <c r="H43" s="54" t="s">
         <v>230</v>
       </c>
-      <c r="I43" s="148"/>
-      <c r="J43" s="167"/>
+      <c r="I43" s="122"/>
+      <c r="J43" s="123"/>
     </row>
     <row r="44" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="24" t="s">
@@ -4944,26 +5059,26 @@
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="133" t="s">
+      <c r="A45" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="135" t="s">
+      <c r="B45" s="148" t="s">
         <v>86</v>
       </c>
-      <c r="C45" s="123" t="s">
+      <c r="C45" s="114" t="s">
         <v>282</v>
       </c>
-      <c r="D45" s="124"/>
-      <c r="E45" s="124"/>
-      <c r="F45" s="124"/>
-      <c r="G45" s="124"/>
-      <c r="H45" s="124"/>
-      <c r="I45" s="125"/>
-      <c r="J45" s="120"/>
+      <c r="D45" s="115"/>
+      <c r="E45" s="115"/>
+      <c r="F45" s="115"/>
+      <c r="G45" s="115"/>
+      <c r="H45" s="115"/>
+      <c r="I45" s="116"/>
+      <c r="J45" s="127"/>
     </row>
     <row r="46" spans="1:10" ht="195" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="134"/>
-      <c r="B46" s="136"/>
+      <c r="A46" s="138"/>
+      <c r="B46" s="140"/>
       <c r="C46" s="22" t="s">
         <v>285</v>
       </c>
@@ -4985,45 +5100,45 @@
       <c r="I46" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="J46" s="122"/>
+      <c r="J46" s="128"/>
     </row>
     <row r="47" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="133" t="s">
+      <c r="A47" s="137" t="s">
         <v>84</v>
       </c>
-      <c r="B47" s="135" t="s">
+      <c r="B47" s="148" t="s">
         <v>83</v>
       </c>
-      <c r="C47" s="160" t="s">
+      <c r="C47" s="149" t="s">
         <v>237</v>
       </c>
-      <c r="D47" s="161"/>
-      <c r="E47" s="161"/>
-      <c r="F47" s="161"/>
-      <c r="G47" s="161"/>
-      <c r="H47" s="162"/>
-      <c r="I47" s="164"/>
-      <c r="J47" s="168" t="s">
+      <c r="D47" s="150"/>
+      <c r="E47" s="150"/>
+      <c r="F47" s="150"/>
+      <c r="G47" s="150"/>
+      <c r="H47" s="151"/>
+      <c r="I47" s="119"/>
+      <c r="J47" s="129" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="300" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="134"/>
-      <c r="B48" s="136"/>
+      <c r="A48" s="138"/>
+      <c r="B48" s="140"/>
       <c r="C48" s="50" t="s">
         <v>82</v>
       </c>
       <c r="D48" s="4"/>
-      <c r="E48" s="166" t="s">
+      <c r="E48" s="121" t="s">
         <v>81</v>
       </c>
-      <c r="F48" s="125"/>
+      <c r="F48" s="116"/>
       <c r="G48" s="4"/>
       <c r="H48" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="I48" s="165"/>
-      <c r="J48" s="169"/>
+      <c r="I48" s="120"/>
+      <c r="J48" s="130"/>
     </row>
     <row r="49" spans="1:10" ht="195" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
@@ -5090,35 +5205,35 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="133" t="s">
+      <c r="A51" s="137" t="s">
         <v>63</v>
       </c>
-      <c r="B51" s="145" t="s">
+      <c r="B51" s="139" t="s">
         <v>62</v>
       </c>
-      <c r="C51" s="170" t="s">
+      <c r="C51" s="131" t="s">
         <v>269</v>
       </c>
-      <c r="D51" s="170"/>
-      <c r="E51" s="170"/>
-      <c r="F51" s="170"/>
-      <c r="G51" s="170"/>
-      <c r="H51" s="170"/>
-      <c r="I51" s="149"/>
-      <c r="J51" s="150"/>
+      <c r="D51" s="131"/>
+      <c r="E51" s="131"/>
+      <c r="F51" s="131"/>
+      <c r="G51" s="131"/>
+      <c r="H51" s="131"/>
+      <c r="I51" s="132"/>
+      <c r="J51" s="133"/>
     </row>
     <row r="52" spans="1:10" ht="345" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="134"/>
-      <c r="B52" s="136"/>
+      <c r="A52" s="138"/>
+      <c r="B52" s="140"/>
       <c r="C52" s="26" t="s">
         <v>268</v>
       </c>
       <c r="D52" s="25" t="s">
         <v>270</v>
       </c>
-      <c r="E52" s="149"/>
-      <c r="F52" s="132"/>
-      <c r="G52" s="130"/>
+      <c r="E52" s="132"/>
+      <c r="F52" s="141"/>
+      <c r="G52" s="142"/>
       <c r="H52" s="57" t="s">
         <v>271</v>
       </c>
@@ -5145,8 +5260,8 @@
       <c r="E53" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="F53" s="126"/>
-      <c r="G53" s="137"/>
+      <c r="F53" s="112"/>
+      <c r="G53" s="113"/>
       <c r="H53" s="28" t="s">
         <v>210</v>
       </c>
@@ -5187,19 +5302,44 @@
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="C45:I45"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="I47:I48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="C40:J40"/>
-    <mergeCell ref="C41:J41"/>
-    <mergeCell ref="J45:J46"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="J47:J48"/>
-    <mergeCell ref="C51:H51"/>
-    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="J11:J17"/>
+    <mergeCell ref="C20:J20"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="C34:H34"/>
+    <mergeCell ref="C21:J21"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="D12:H12"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="C18:I18"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="C23:J23"/>
+    <mergeCell ref="C24:J24"/>
+    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="C26:J26"/>
+    <mergeCell ref="C28:J28"/>
+    <mergeCell ref="J29:J31"/>
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="C8:J8"/>
     <mergeCell ref="C10:H10"/>
@@ -5216,44 +5356,19 @@
     <mergeCell ref="A45:A46"/>
     <mergeCell ref="A41:A42"/>
     <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C32:H32"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="C23:J23"/>
-    <mergeCell ref="C24:J24"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:H39"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="C25:J25"/>
-    <mergeCell ref="C26:J26"/>
-    <mergeCell ref="C28:J28"/>
-    <mergeCell ref="J29:J31"/>
-    <mergeCell ref="C34:H34"/>
-    <mergeCell ref="C21:J21"/>
-    <mergeCell ref="C22:J22"/>
-    <mergeCell ref="D12:H12"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="C18:I18"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="J11:J17"/>
-    <mergeCell ref="C20:J20"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="C45:I45"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="I47:I48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="C40:J40"/>
+    <mergeCell ref="C41:J41"/>
+    <mergeCell ref="J45:J46"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="C51:H51"/>
+    <mergeCell ref="I51:J51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5265,10 +5380,10 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5278,7 +5393,7 @@
     <col min="3" max="7" width="26.7109375" style="1" customWidth="1"/>
     <col min="8" max="9" width="27.140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="27.5703125" style="1" customWidth="1"/>
-    <col min="11" max="13" width="9.140625" style="101"/>
+    <col min="11" max="13" width="9.140625" style="100"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5312,337 +5427,367 @@
       <c r="J1" s="88" t="s">
         <v>292</v>
       </c>
-      <c r="K1" s="98"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
     </row>
     <row r="2" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="186" t="s">
+      <c r="A2" s="171" t="s">
         <v>198</v>
       </c>
-      <c r="B2" s="185" t="s">
+      <c r="B2" s="170" t="s">
         <v>309</v>
       </c>
-      <c r="C2" s="188" t="s">
+      <c r="C2" s="173" t="s">
         <v>340</v>
       </c>
-      <c r="D2" s="189"/>
-      <c r="E2" s="189"/>
-      <c r="F2" s="189"/>
-      <c r="G2" s="189"/>
-      <c r="H2" s="189"/>
-      <c r="I2" s="189"/>
-      <c r="J2" s="189"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-    </row>
-    <row r="3" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="187"/>
-      <c r="B3" s="136"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="106"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
+      <c r="I2" s="174"/>
+      <c r="J2" s="174"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+    </row>
+    <row r="3" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="172"/>
+      <c r="B3" s="140"/>
+      <c r="C3" s="191"/>
+      <c r="D3" s="133"/>
+      <c r="E3" s="46" t="s">
+        <v>354</v>
+      </c>
+      <c r="F3" s="132"/>
+      <c r="G3" s="190"/>
+      <c r="H3" s="190"/>
+      <c r="I3" s="133"/>
+      <c r="J3" s="192" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="4" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="183" t="s">
+      <c r="A4" s="175" t="s">
         <v>197</v>
       </c>
-      <c r="B4" s="177" t="s">
+      <c r="B4" s="176" t="s">
         <v>310</v>
       </c>
-      <c r="C4" s="180" t="s">
+      <c r="C4" s="177" t="s">
         <v>339</v>
       </c>
-      <c r="D4" s="181"/>
-      <c r="E4" s="181"/>
-      <c r="F4" s="181"/>
-      <c r="G4" s="181"/>
-      <c r="H4" s="181"/>
-      <c r="I4" s="181"/>
-      <c r="J4" s="181"/>
-      <c r="K4" s="98"/>
-      <c r="L4" s="98"/>
-      <c r="M4" s="98"/>
-    </row>
-    <row r="5" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="117"/>
-      <c r="B5" s="119"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="106"/>
+      <c r="D4" s="178"/>
+      <c r="E4" s="178"/>
+      <c r="F4" s="178"/>
+      <c r="G4" s="178"/>
+      <c r="H4" s="178"/>
+      <c r="I4" s="178"/>
+      <c r="J4" s="178"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="97"/>
+      <c r="M4" s="97"/>
+    </row>
+    <row r="5" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="165"/>
+      <c r="B5" s="167"/>
+      <c r="C5" s="191"/>
+      <c r="D5" s="190"/>
+      <c r="E5" s="190"/>
+      <c r="F5" s="190"/>
+      <c r="G5" s="133"/>
+      <c r="H5" s="46" t="s">
+        <v>365</v>
+      </c>
+      <c r="I5" s="58"/>
+      <c r="J5" s="192" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="6" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="183" t="s">
+      <c r="A6" s="175" t="s">
         <v>196</v>
       </c>
-      <c r="B6" s="177" t="s">
+      <c r="B6" s="176" t="s">
         <v>311</v>
       </c>
-      <c r="C6" s="180" t="s">
+      <c r="C6" s="177" t="s">
         <v>338</v>
       </c>
-      <c r="D6" s="181"/>
-      <c r="E6" s="181"/>
-      <c r="F6" s="181"/>
-      <c r="G6" s="181"/>
-      <c r="H6" s="181"/>
-      <c r="I6" s="181"/>
-      <c r="J6" s="181"/>
-      <c r="K6" s="98"/>
-      <c r="L6" s="98"/>
-      <c r="M6" s="98"/>
+      <c r="D6" s="178"/>
+      <c r="E6" s="178"/>
+      <c r="F6" s="178"/>
+      <c r="G6" s="178"/>
+      <c r="H6" s="178"/>
+      <c r="I6" s="178"/>
+      <c r="J6" s="178"/>
+      <c r="K6" s="97"/>
+      <c r="L6" s="97"/>
+      <c r="M6" s="97"/>
     </row>
     <row r="7" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="117"/>
-      <c r="B7" s="119"/>
-      <c r="C7" s="92"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="106"/>
+      <c r="A7" s="165"/>
+      <c r="B7" s="167"/>
+      <c r="C7" s="191"/>
+      <c r="D7" s="190"/>
+      <c r="E7" s="133"/>
+      <c r="F7" s="46" t="s">
+        <v>348</v>
+      </c>
+      <c r="G7" s="132"/>
+      <c r="H7" s="190"/>
+      <c r="I7" s="133"/>
+      <c r="J7" s="192" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="8" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="116" t="s">
+      <c r="A8" s="164" t="s">
         <v>195</v>
       </c>
-      <c r="B8" s="118" t="s">
+      <c r="B8" s="166" t="s">
         <v>312</v>
       </c>
-      <c r="C8" s="180" t="s">
+      <c r="C8" s="177" t="s">
         <v>337</v>
       </c>
-      <c r="D8" s="181"/>
-      <c r="E8" s="181"/>
-      <c r="F8" s="181"/>
-      <c r="G8" s="181"/>
-      <c r="H8" s="181"/>
-      <c r="I8" s="181"/>
-      <c r="J8" s="181"/>
-      <c r="K8" s="98"/>
-      <c r="L8" s="98"/>
-      <c r="M8" s="98"/>
-    </row>
-    <row r="9" spans="1:13" s="97" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="184"/>
-      <c r="B9" s="178"/>
-      <c r="C9" s="95"/>
-      <c r="D9" s="96"/>
-      <c r="E9" s="96"/>
-      <c r="F9" s="96"/>
-      <c r="G9" s="96"/>
-      <c r="H9" s="96"/>
-      <c r="I9" s="96"/>
-      <c r="J9" s="107"/>
-      <c r="K9" s="101"/>
-      <c r="L9" s="101"/>
-      <c r="M9" s="101"/>
+      <c r="D8" s="178"/>
+      <c r="E8" s="178"/>
+      <c r="F8" s="178"/>
+      <c r="G8" s="178"/>
+      <c r="H8" s="178"/>
+      <c r="I8" s="178"/>
+      <c r="J8" s="178"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="97"/>
+    </row>
+    <row r="9" spans="1:13" s="96" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="179"/>
+      <c r="B9" s="180"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="189" t="s">
+        <v>363</v>
+      </c>
+      <c r="E9" s="156"/>
+      <c r="F9" s="157"/>
+      <c r="G9" s="157"/>
+      <c r="H9" s="157"/>
+      <c r="I9" s="157"/>
+      <c r="J9" s="193" t="s">
+        <v>356</v>
+      </c>
+      <c r="K9" s="100"/>
+      <c r="L9" s="100"/>
+      <c r="M9" s="100"/>
     </row>
     <row r="10" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="175" t="s">
+      <c r="A10" s="181" t="s">
         <v>194</v>
       </c>
-      <c r="B10" s="177" t="s">
+      <c r="B10" s="176" t="s">
         <v>324</v>
       </c>
-      <c r="C10" s="180" t="s">
+      <c r="C10" s="177" t="s">
         <v>336</v>
       </c>
-      <c r="D10" s="181"/>
-      <c r="E10" s="181"/>
-      <c r="F10" s="181"/>
-      <c r="G10" s="181"/>
-      <c r="H10" s="181"/>
-      <c r="I10" s="181"/>
-      <c r="J10" s="181"/>
-      <c r="K10" s="98"/>
-      <c r="L10" s="98"/>
-      <c r="M10" s="98"/>
-    </row>
-    <row r="11" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="178"/>
+      <c r="E10" s="178"/>
+      <c r="F10" s="178"/>
+      <c r="G10" s="178"/>
+      <c r="H10" s="178"/>
+      <c r="I10" s="178"/>
+      <c r="J10" s="178"/>
+      <c r="K10" s="97"/>
+      <c r="L10" s="97"/>
+      <c r="M10" s="97"/>
+    </row>
+    <row r="11" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="182"/>
-      <c r="B11" s="119"/>
-      <c r="C11" s="92"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="106"/>
+      <c r="B11" s="167"/>
+      <c r="C11" s="108" t="s">
+        <v>353</v>
+      </c>
+      <c r="D11" s="132"/>
+      <c r="E11" s="190"/>
+      <c r="F11" s="190"/>
+      <c r="G11" s="190"/>
+      <c r="H11" s="190"/>
+      <c r="I11" s="190"/>
+      <c r="J11" s="192" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="12" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="175" t="s">
+      <c r="A12" s="181" t="s">
         <v>193</v>
       </c>
-      <c r="B12" s="177" t="s">
+      <c r="B12" s="176" t="s">
         <v>323</v>
       </c>
-      <c r="C12" s="173" t="s">
+      <c r="C12" s="183" t="s">
         <v>335</v>
       </c>
-      <c r="D12" s="174"/>
-      <c r="E12" s="174"/>
-      <c r="F12" s="174"/>
-      <c r="G12" s="174"/>
-      <c r="H12" s="174"/>
-      <c r="I12" s="174"/>
-      <c r="J12" s="174"/>
-      <c r="K12" s="98"/>
-      <c r="L12" s="98"/>
-      <c r="M12" s="98"/>
-    </row>
-    <row r="13" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="184"/>
+      <c r="E12" s="184"/>
+      <c r="F12" s="184"/>
+      <c r="G12" s="184"/>
+      <c r="H12" s="184"/>
+      <c r="I12" s="184"/>
+      <c r="J12" s="184"/>
+      <c r="K12" s="97"/>
+      <c r="L12" s="97"/>
+      <c r="M12" s="97"/>
+    </row>
+    <row r="13" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="182"/>
-      <c r="B13" s="119"/>
-      <c r="C13" s="92"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="106"/>
+      <c r="B13" s="167"/>
+      <c r="C13" s="191"/>
+      <c r="D13" s="190"/>
+      <c r="E13" s="190"/>
+      <c r="F13" s="133"/>
+      <c r="G13" s="46" t="s">
+        <v>364</v>
+      </c>
+      <c r="H13" s="132"/>
+      <c r="I13" s="133"/>
+      <c r="J13" s="194" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="14" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="175" t="s">
+      <c r="A14" s="181" t="s">
         <v>321</v>
       </c>
-      <c r="B14" s="177" t="s">
+      <c r="B14" s="176" t="s">
         <v>322</v>
       </c>
-      <c r="C14" s="180" t="s">
+      <c r="C14" s="177" t="s">
         <v>347</v>
       </c>
-      <c r="D14" s="181"/>
-      <c r="E14" s="181"/>
-      <c r="F14" s="181"/>
-      <c r="G14" s="181"/>
-      <c r="H14" s="181"/>
-      <c r="I14" s="181"/>
-      <c r="J14" s="181"/>
-      <c r="K14" s="98"/>
-      <c r="L14" s="98"/>
-      <c r="M14" s="98"/>
+      <c r="D14" s="178"/>
+      <c r="E14" s="178"/>
+      <c r="F14" s="178"/>
+      <c r="G14" s="178"/>
+      <c r="H14" s="178"/>
+      <c r="I14" s="178"/>
+      <c r="J14" s="178"/>
+      <c r="K14" s="97"/>
+      <c r="L14" s="97"/>
+      <c r="M14" s="97"/>
     </row>
     <row r="15" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="182"/>
-      <c r="B15" s="119"/>
-      <c r="C15" s="92"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="106"/>
+      <c r="B15" s="167"/>
+      <c r="C15" s="191"/>
+      <c r="D15" s="190"/>
+      <c r="E15" s="190"/>
+      <c r="F15" s="190"/>
+      <c r="G15" s="190"/>
+      <c r="H15" s="190"/>
+      <c r="I15" s="133"/>
+      <c r="J15" s="56" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="16" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="175" t="s">
+      <c r="A16" s="181" t="s">
         <v>192</v>
       </c>
-      <c r="B16" s="177" t="s">
+      <c r="B16" s="176" t="s">
         <v>325</v>
       </c>
-      <c r="C16" s="180" t="s">
+      <c r="C16" s="177" t="s">
         <v>334</v>
       </c>
-      <c r="D16" s="181"/>
-      <c r="E16" s="181"/>
-      <c r="F16" s="181"/>
-      <c r="G16" s="181"/>
-      <c r="H16" s="181"/>
-      <c r="I16" s="181"/>
-      <c r="J16" s="181"/>
-      <c r="K16" s="98"/>
-      <c r="L16" s="98"/>
-      <c r="M16" s="98"/>
+      <c r="D16" s="178"/>
+      <c r="E16" s="178"/>
+      <c r="F16" s="178"/>
+      <c r="G16" s="178"/>
+      <c r="H16" s="178"/>
+      <c r="I16" s="178"/>
+      <c r="J16" s="178"/>
+      <c r="K16" s="97"/>
+      <c r="L16" s="97"/>
+      <c r="M16" s="97"/>
     </row>
     <row r="17" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="182"/>
-      <c r="B17" s="119"/>
-      <c r="C17" s="92"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="106"/>
+      <c r="B17" s="167"/>
+      <c r="C17" s="191"/>
+      <c r="D17" s="190"/>
+      <c r="E17" s="190"/>
+      <c r="F17" s="190"/>
+      <c r="G17" s="190"/>
+      <c r="H17" s="133"/>
+      <c r="I17" s="46" t="s">
+        <v>349</v>
+      </c>
+      <c r="J17" s="56" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="18" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="179" t="s">
+      <c r="A18" s="185" t="s">
         <v>191</v>
       </c>
-      <c r="B18" s="118" t="s">
+      <c r="B18" s="166" t="s">
         <v>327</v>
       </c>
-      <c r="C18" s="180" t="s">
+      <c r="C18" s="195" t="s">
         <v>330</v>
       </c>
-      <c r="D18" s="181"/>
-      <c r="E18" s="181"/>
-      <c r="F18" s="181"/>
-      <c r="G18" s="181"/>
-      <c r="H18" s="181"/>
-      <c r="I18" s="181"/>
-      <c r="J18" s="181"/>
-      <c r="K18" s="98"/>
-      <c r="L18" s="98"/>
-      <c r="M18" s="98"/>
-    </row>
-    <row r="19" spans="1:13" s="101" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="172"/>
-      <c r="B19" s="136"/>
-      <c r="C19" s="104" t="s">
+      <c r="D18" s="196"/>
+      <c r="E18" s="196"/>
+      <c r="F18" s="196"/>
+      <c r="G18" s="196"/>
+      <c r="H18" s="196"/>
+      <c r="I18" s="196"/>
+      <c r="J18" s="196"/>
+      <c r="K18" s="97"/>
+      <c r="L18" s="97"/>
+      <c r="M18" s="97"/>
+    </row>
+    <row r="19" spans="1:13" s="100" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="186"/>
+      <c r="B19" s="140"/>
+      <c r="C19" s="103" t="s">
         <v>342</v>
       </c>
-      <c r="D19" s="100"/>
-      <c r="E19" s="100"/>
-      <c r="F19" s="100"/>
-      <c r="G19" s="100"/>
-      <c r="H19" s="100"/>
-      <c r="I19" s="100"/>
-      <c r="J19" s="108"/>
-    </row>
-    <row r="20" spans="1:13" s="102" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="171" t="s">
+      <c r="D19" s="99"/>
+      <c r="E19" s="99"/>
+      <c r="F19" s="99"/>
+      <c r="G19" s="99"/>
+      <c r="H19" s="99"/>
+      <c r="I19" s="99"/>
+      <c r="J19" s="106"/>
+    </row>
+    <row r="20" spans="1:13" s="101" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="187" t="s">
         <v>190</v>
       </c>
-      <c r="B20" s="135" t="s">
+      <c r="B20" s="148" t="s">
         <v>326</v>
       </c>
-      <c r="C20" s="173" t="s">
+      <c r="C20" s="183" t="s">
         <v>331</v>
       </c>
-      <c r="D20" s="174"/>
-      <c r="E20" s="174"/>
-      <c r="F20" s="174"/>
-      <c r="G20" s="174"/>
-      <c r="H20" s="174"/>
-      <c r="I20" s="174"/>
-      <c r="J20" s="174"/>
-      <c r="K20" s="98"/>
-      <c r="L20" s="98"/>
-      <c r="M20" s="98"/>
-    </row>
-    <row r="21" spans="1:13" s="99" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="172"/>
-      <c r="B21" s="136"/>
-      <c r="C21" s="104" t="s">
+      <c r="D20" s="184"/>
+      <c r="E20" s="184"/>
+      <c r="F20" s="184"/>
+      <c r="G20" s="184"/>
+      <c r="H20" s="184"/>
+      <c r="I20" s="184"/>
+      <c r="J20" s="184"/>
+      <c r="K20" s="97"/>
+      <c r="L20" s="97"/>
+      <c r="M20" s="97"/>
+    </row>
+    <row r="21" spans="1:13" s="98" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="186"/>
+      <c r="B21" s="140"/>
+      <c r="C21" s="103" t="s">
         <v>341</v>
       </c>
       <c r="D21" s="15"/>
@@ -5651,170 +5796,179 @@
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
-      <c r="J21" s="106"/>
-      <c r="K21" s="101"/>
-      <c r="L21" s="101"/>
-      <c r="M21" s="101"/>
+      <c r="J21" s="105"/>
+      <c r="K21" s="100"/>
+      <c r="L21" s="100"/>
+      <c r="M21" s="100"/>
     </row>
     <row r="22" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="171" t="s">
+      <c r="A22" s="187" t="s">
         <v>189</v>
       </c>
-      <c r="B22" s="135" t="s">
+      <c r="B22" s="148" t="s">
         <v>328</v>
       </c>
-      <c r="C22" s="173" t="s">
+      <c r="C22" s="183" t="s">
         <v>332</v>
       </c>
-      <c r="D22" s="174"/>
-      <c r="E22" s="174"/>
-      <c r="F22" s="174"/>
-      <c r="G22" s="174"/>
-      <c r="H22" s="174"/>
-      <c r="I22" s="174"/>
-      <c r="J22" s="174"/>
-      <c r="K22" s="98"/>
-      <c r="L22" s="98"/>
-      <c r="M22" s="98"/>
-    </row>
-    <row r="23" spans="1:13" s="101" customFormat="1" ht="210" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="172"/>
-      <c r="B23" s="136"/>
-      <c r="C23" s="104" t="s">
+      <c r="D22" s="184"/>
+      <c r="E22" s="184"/>
+      <c r="F22" s="184"/>
+      <c r="G22" s="184"/>
+      <c r="H22" s="184"/>
+      <c r="I22" s="184"/>
+      <c r="J22" s="184"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+    </row>
+    <row r="23" spans="1:13" s="100" customFormat="1" ht="210" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="186"/>
+      <c r="B23" s="140"/>
+      <c r="C23" s="103" t="s">
         <v>343</v>
       </c>
-      <c r="D23" s="100"/>
-      <c r="E23" s="100"/>
-      <c r="F23" s="100"/>
-      <c r="G23" s="100"/>
-      <c r="H23" s="100"/>
-      <c r="I23" s="100"/>
-      <c r="J23" s="108"/>
-    </row>
-    <row r="24" spans="1:13" s="103" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="175" t="s">
+      <c r="D23" s="99"/>
+      <c r="E23" s="99"/>
+      <c r="F23" s="99"/>
+      <c r="G23" s="99"/>
+      <c r="H23" s="99"/>
+      <c r="I23" s="99"/>
+      <c r="J23" s="106"/>
+    </row>
+    <row r="24" spans="1:13" s="102" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="181" t="s">
         <v>188</v>
       </c>
-      <c r="B24" s="177" t="s">
+      <c r="B24" s="176" t="s">
         <v>329</v>
       </c>
-      <c r="C24" s="173" t="s">
+      <c r="C24" s="183" t="s">
         <v>333</v>
       </c>
-      <c r="D24" s="174"/>
-      <c r="E24" s="174"/>
-      <c r="F24" s="174"/>
-      <c r="G24" s="174"/>
-      <c r="H24" s="174"/>
-      <c r="I24" s="174"/>
-      <c r="J24" s="174"/>
-      <c r="K24" s="98"/>
-      <c r="L24" s="98"/>
-      <c r="M24" s="98"/>
-    </row>
-    <row r="25" spans="1:13" s="97" customFormat="1" ht="285" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="176"/>
-      <c r="B25" s="178"/>
-      <c r="C25" s="105" t="s">
+      <c r="D24" s="184"/>
+      <c r="E24" s="184"/>
+      <c r="F24" s="184"/>
+      <c r="G24" s="184"/>
+      <c r="H24" s="184"/>
+      <c r="I24" s="184"/>
+      <c r="J24" s="184"/>
+      <c r="K24" s="97"/>
+      <c r="L24" s="97"/>
+      <c r="M24" s="97"/>
+    </row>
+    <row r="25" spans="1:13" s="96" customFormat="1" ht="300" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="188"/>
+      <c r="B25" s="180"/>
+      <c r="C25" s="104" t="s">
         <v>344</v>
       </c>
-      <c r="D25" s="96"/>
-      <c r="E25" s="96"/>
-      <c r="F25" s="96"/>
-      <c r="G25" s="96"/>
-      <c r="H25" s="105" t="s">
+      <c r="D25" s="189" t="s">
+        <v>352</v>
+      </c>
+      <c r="E25" s="95"/>
+      <c r="F25" s="95" t="s">
+        <v>351</v>
+      </c>
+      <c r="G25" s="95" t="s">
+        <v>350</v>
+      </c>
+      <c r="H25" s="104" t="s">
         <v>345</v>
       </c>
-      <c r="I25" s="96"/>
-      <c r="J25" s="109" t="s">
+      <c r="I25" s="95"/>
+      <c r="J25" s="107" t="s">
         <v>346</v>
       </c>
-      <c r="K25" s="101"/>
-      <c r="L25" s="101"/>
-      <c r="M25" s="101"/>
+      <c r="K25" s="100"/>
+      <c r="L25" s="100"/>
+      <c r="M25" s="100"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="94"/>
+      <c r="B26" s="93"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="94"/>
+      <c r="B27" s="93"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="94"/>
+      <c r="B28" s="93"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="94"/>
+      <c r="B29" s="93"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="94"/>
+      <c r="B30" s="93"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="94"/>
+      <c r="B31" s="93"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="94"/>
-    </row>
-    <row r="33" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B33" s="94" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B34" s="94" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B35" s="94" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B36" s="94" t="s">
-        <v>325</v>
-      </c>
+      <c r="B32" s="93"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="93"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="93"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="93"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="93"/>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="94"/>
+      <c r="B37" s="93"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="47">
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:J24"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:J18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:J20"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:J14"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:J16"/>
+    <mergeCell ref="C15:I15"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:J12"/>
+    <mergeCell ref="D11:I11"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:J8"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="E9:I9"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:J4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:J8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:J10"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:J12"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:J14"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:J16"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:J18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:J20"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:J22"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:J24"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
refined the weighting and categorisation of weapons and components.
</commit_message>
<xml_diff>
--- a/Tags and Affinities.xlsx
+++ b/Tags and Affinities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CK.DESKTOP-BR5NVLN\Documents\Git Repositories\Creative\materials_and_crafting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53031307-48AE-491C-B43C-0FAAEC6B96E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A1F173-9426-4E72-80D9-6A131FA54AFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{8FD76562-234B-40A6-8AC6-52675E21BBDC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="370">
   <si>
     <t>This component's weapon can be wound up in preparation for a powerful strike, however its strikes take a while to rewind.</t>
   </si>
@@ -1842,9 +1842,6 @@
     <t>Movement causes tremors</t>
   </si>
   <si>
-    <t>Flask stores soul</t>
-  </si>
-  <si>
     <t>Random movement size</t>
   </si>
   <si>
@@ -1886,9 +1883,6 @@
     <t>When ingested, this potion grants resistance to lightning damage.</t>
   </si>
   <si>
-    <t>When ingested, this potion grants resistance to poison and acid damage.</t>
-  </si>
-  <si>
     <t>When ingested, this potion grants resistance to cold damage.</t>
   </si>
   <si>
@@ -1911,7 +1905,72 @@
 When you are in dim light or darkness, as a bonus action you can teleport out to a radius equal to 20 times these boots' erebian affinity to an unoccupied space you can see that is also in dim light or darkness.</t>
   </si>
   <si>
-    <t>As an action while you wield this staff, you may conjure a large wave of water that pushes all creatures in a line.</t>
+    <t>Weighted</t>
+  </si>
+  <si>
+    <t>This item cannot be light.</t>
+  </si>
+  <si>
+    <t>This component weighs down items that incorporate it.</t>
+  </si>
+  <si>
+    <t>Double this component's weight (this is not factored into the material cost or MOD calculations).</t>
+  </si>
+  <si>
+    <t>When ingested, this potion grants resistance to poison or acid damage.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This flask can store a soul within its cavity.
+This flask can be used as the material component of the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>soul cage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>soul jar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> spells, and you may cast both of these spells once as a bonus action.
+These spells cannot be cast again from this flask until it has spent a long rest bathed in quintescent energy.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">As an action while you wield this staff, you may conjure a large wave of water that pushes all creatures in a line.
+</t>
   </si>
 </sst>
 </file>
@@ -2854,7 +2913,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="197">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3160,6 +3219,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="70" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="71" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="70" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3167,29 +3241,161 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3198,28 +3404,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3229,119 +3417,59 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3358,70 +3486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="70" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="71" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="70" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3739,11 +3804,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2676EF7-6059-47B8-9088-C8B7174E5212}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3848,33 +3913,29 @@
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
     </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="120" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="122" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="117" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="118"/>
+      <c r="I5" s="119"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="121"/>
+      <c r="B6" s="123"/>
+      <c r="C6" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -3886,13 +3947,13 @@
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -3902,15 +3963,15 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" s="3" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="3" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -3920,15 +3981,15 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" s="3" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="3" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -3938,15 +3999,15 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" s="3" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="3" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>16</v>
+        <v>20</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -3956,15 +4017,15 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="3" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>316</v>
+        <v>17</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -3974,15 +4035,15 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" s="3" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>11</v>
+        <v>316</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -3992,15 +4053,15 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="3" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -4012,13 +4073,13 @@
     </row>
     <row r="14" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -4030,13 +4091,13 @@
     </row>
     <row r="15" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -4046,65 +4107,105 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:10" s="73" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="74" t="s">
+    <row r="16" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" s="73" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="75" t="s">
+      <c r="B17" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="71" t="s">
+      <c r="C17" s="71" t="s">
         <v>317</v>
       </c>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
-    </row>
-    <row r="17" spans="1:10" s="73" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="92" t="s">
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
+    </row>
+    <row r="18" spans="1:10" s="73" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="92" t="s">
         <v>234</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B18" s="23" t="s">
         <v>293</v>
       </c>
-      <c r="C17" s="72" t="s">
+      <c r="C18" s="72" t="s">
         <v>235</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="21" t="s">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="76" t="s">
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" s="73" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="198" t="s">
+        <v>363</v>
+      </c>
+      <c r="B19" s="109" t="s">
+        <v>365</v>
+      </c>
+      <c r="C19" s="117" t="s">
+        <v>364</v>
+      </c>
+      <c r="D19" s="118"/>
+      <c r="E19" s="118"/>
+      <c r="F19" s="118"/>
+      <c r="G19" s="118"/>
+      <c r="H19" s="118"/>
+      <c r="I19" s="119"/>
+      <c r="J19" s="44"/>
+    </row>
+    <row r="20" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="76" t="s">
         <v>290</v>
       </c>
-      <c r="B18" s="77" t="s">
+      <c r="B20" s="77" t="s">
         <v>318</v>
       </c>
-      <c r="C18" s="109" t="s">
+      <c r="C20" s="114" t="s">
         <v>319</v>
       </c>
-      <c r="D18" s="110"/>
-      <c r="E18" s="110"/>
-      <c r="F18" s="110"/>
-      <c r="G18" s="110"/>
-      <c r="H18" s="110"/>
-      <c r="I18" s="111"/>
-      <c r="J18" s="35"/>
+      <c r="D20" s="115"/>
+      <c r="E20" s="115"/>
+      <c r="F20" s="115"/>
+      <c r="G20" s="115"/>
+      <c r="H20" s="115"/>
+      <c r="I20" s="116"/>
+      <c r="J20" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C18:I18"/>
+  <mergeCells count="5">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C20:I20"/>
+    <mergeCell ref="C19:I19"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4116,10 +4217,10 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4171,47 +4272,47 @@
       <c r="B2" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="C2" s="134" t="s">
+      <c r="C2" s="157" t="s">
         <v>185</v>
       </c>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="135"/>
-      <c r="H2" s="135"/>
-      <c r="I2" s="136"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="158"/>
+      <c r="H2" s="158"/>
+      <c r="I2" s="159"/>
       <c r="J2" s="78"/>
     </row>
     <row r="3" spans="1:10" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="164" t="s">
+      <c r="A3" s="120" t="s">
         <v>184</v>
       </c>
-      <c r="B3" s="166" t="s">
+      <c r="B3" s="122" t="s">
         <v>260</v>
       </c>
-      <c r="C3" s="124" t="s">
+      <c r="C3" s="117" t="s">
         <v>320</v>
       </c>
-      <c r="D3" s="125"/>
-      <c r="E3" s="125"/>
-      <c r="F3" s="125"/>
-      <c r="G3" s="125"/>
-      <c r="H3" s="125"/>
-      <c r="I3" s="125"/>
-      <c r="J3" s="126"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="119"/>
     </row>
     <row r="4" spans="1:10" s="18" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A4" s="165"/>
-      <c r="B4" s="167"/>
+      <c r="A4" s="121"/>
+      <c r="B4" s="123"/>
       <c r="C4" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="D4" s="147" t="s">
+      <c r="D4" s="130" t="s">
         <v>182</v>
       </c>
-      <c r="E4" s="147"/>
-      <c r="F4" s="147"/>
-      <c r="G4" s="147"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
+      <c r="G4" s="130"/>
       <c r="H4" s="54" t="s">
         <v>181</v>
       </c>
@@ -4227,15 +4328,15 @@
       <c r="B5" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C5" s="124" t="s">
+      <c r="C5" s="117" t="s">
         <v>178</v>
       </c>
-      <c r="D5" s="125"/>
-      <c r="E5" s="125"/>
-      <c r="F5" s="125"/>
-      <c r="G5" s="125"/>
-      <c r="H5" s="125"/>
-      <c r="I5" s="126"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="118"/>
+      <c r="I5" s="119"/>
       <c r="J5" s="80"/>
     </row>
     <row r="6" spans="1:10" s="18" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -4246,12 +4347,12 @@
         <v>259</v>
       </c>
       <c r="C6" s="31"/>
-      <c r="D6" s="147" t="s">
+      <c r="D6" s="130" t="s">
         <v>177</v>
       </c>
-      <c r="E6" s="147"/>
-      <c r="F6" s="147"/>
-      <c r="G6" s="147"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="130"/>
       <c r="H6" s="54" t="s">
         <v>176</v>
       </c>
@@ -4267,15 +4368,15 @@
       <c r="B7" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C7" s="124" t="s">
+      <c r="C7" s="117" t="s">
         <v>173</v>
       </c>
-      <c r="D7" s="125"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="125"/>
-      <c r="G7" s="125"/>
-      <c r="H7" s="125"/>
-      <c r="I7" s="126"/>
+      <c r="D7" s="118"/>
+      <c r="E7" s="118"/>
+      <c r="F7" s="118"/>
+      <c r="G7" s="118"/>
+      <c r="H7" s="118"/>
+      <c r="I7" s="119"/>
       <c r="J7" s="80"/>
     </row>
     <row r="8" spans="1:10" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -4285,16 +4386,16 @@
       <c r="B8" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="C8" s="124" t="s">
+      <c r="C8" s="117" t="s">
         <v>171</v>
       </c>
-      <c r="D8" s="125"/>
-      <c r="E8" s="125"/>
-      <c r="F8" s="125"/>
-      <c r="G8" s="125"/>
-      <c r="H8" s="125"/>
-      <c r="I8" s="125"/>
-      <c r="J8" s="126"/>
+      <c r="D8" s="118"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="118"/>
+      <c r="G8" s="118"/>
+      <c r="H8" s="118"/>
+      <c r="I8" s="118"/>
+      <c r="J8" s="119"/>
     </row>
     <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="42" t="s">
@@ -4303,15 +4404,15 @@
       <c r="B9" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="C9" s="124" t="s">
+      <c r="C9" s="117" t="s">
         <v>169</v>
       </c>
-      <c r="D9" s="125"/>
-      <c r="E9" s="125"/>
-      <c r="F9" s="125"/>
-      <c r="G9" s="125"/>
-      <c r="H9" s="125"/>
-      <c r="I9" s="126"/>
+      <c r="D9" s="118"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="118"/>
+      <c r="G9" s="118"/>
+      <c r="H9" s="118"/>
+      <c r="I9" s="119"/>
       <c r="J9" s="59"/>
     </row>
     <row r="10" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -4321,14 +4422,14 @@
       <c r="B10" s="69" t="s">
         <v>261</v>
       </c>
-      <c r="C10" s="124" t="s">
+      <c r="C10" s="117" t="s">
         <v>263</v>
       </c>
-      <c r="D10" s="125"/>
-      <c r="E10" s="125"/>
-      <c r="F10" s="125"/>
-      <c r="G10" s="125"/>
-      <c r="H10" s="126"/>
+      <c r="D10" s="118"/>
+      <c r="E10" s="118"/>
+      <c r="F10" s="118"/>
+      <c r="G10" s="118"/>
+      <c r="H10" s="119"/>
       <c r="I10" s="4"/>
       <c r="J10" s="70" t="s">
         <v>262</v>
@@ -4358,7 +4459,7 @@
       <c r="I11" s="61" t="s">
         <v>246</v>
       </c>
-      <c r="J11" s="127"/>
+      <c r="J11" s="124"/>
     </row>
     <row r="12" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
@@ -4370,15 +4471,15 @@
       <c r="C12" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="D12" s="112"/>
-      <c r="E12" s="118"/>
-      <c r="F12" s="158"/>
-      <c r="G12" s="158"/>
-      <c r="H12" s="158"/>
+      <c r="D12" s="134"/>
+      <c r="E12" s="135"/>
+      <c r="F12" s="136"/>
+      <c r="G12" s="136"/>
+      <c r="H12" s="136"/>
       <c r="I12" s="61" t="s">
         <v>294</v>
       </c>
-      <c r="J12" s="162"/>
+      <c r="J12" s="125"/>
     </row>
     <row r="13" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
@@ -4406,20 +4507,20 @@
       <c r="I13" s="60" t="s">
         <v>241</v>
       </c>
-      <c r="J13" s="162"/>
+      <c r="J13" s="125"/>
     </row>
     <row r="14" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="168" t="s">
+      <c r="A14" s="131" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="154" t="s">
+      <c r="B14" s="132" t="s">
         <v>157</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="D14" s="112"/>
-      <c r="E14" s="113"/>
+      <c r="D14" s="134"/>
+      <c r="E14" s="145"/>
       <c r="F14" s="32" t="s">
         <v>238</v>
       </c>
@@ -4430,34 +4531,34 @@
       <c r="I14" s="63" t="s">
         <v>243</v>
       </c>
-      <c r="J14" s="162"/>
+      <c r="J14" s="125"/>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="168"/>
-      <c r="B15" s="154"/>
-      <c r="C15" s="143" t="s">
+      <c r="A15" s="131"/>
+      <c r="B15" s="132"/>
+      <c r="C15" s="160" t="s">
         <v>155</v>
       </c>
-      <c r="D15" s="144"/>
-      <c r="E15" s="144"/>
-      <c r="F15" s="144"/>
-      <c r="G15" s="144"/>
-      <c r="H15" s="144"/>
-      <c r="I15" s="145"/>
-      <c r="J15" s="162"/>
+      <c r="D15" s="161"/>
+      <c r="E15" s="161"/>
+      <c r="F15" s="161"/>
+      <c r="G15" s="161"/>
+      <c r="H15" s="161"/>
+      <c r="I15" s="162"/>
+      <c r="J15" s="125"/>
     </row>
     <row r="16" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A16" s="168" t="s">
+      <c r="A16" s="131" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="154" t="s">
+      <c r="B16" s="132" t="s">
         <v>154</v>
       </c>
       <c r="C16" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="D16" s="155"/>
-      <c r="E16" s="142"/>
+      <c r="D16" s="137"/>
+      <c r="E16" s="138"/>
       <c r="F16" s="60" t="s">
         <v>152</v>
       </c>
@@ -4468,21 +4569,21 @@
       <c r="I16" s="64" t="s">
         <v>244</v>
       </c>
-      <c r="J16" s="162"/>
+      <c r="J16" s="125"/>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="168"/>
-      <c r="B17" s="169"/>
-      <c r="C17" s="146" t="s">
+      <c r="A17" s="131"/>
+      <c r="B17" s="133"/>
+      <c r="C17" s="163" t="s">
         <v>151</v>
       </c>
-      <c r="D17" s="147"/>
-      <c r="E17" s="147"/>
-      <c r="F17" s="147"/>
-      <c r="G17" s="147"/>
-      <c r="H17" s="147"/>
-      <c r="I17" s="147"/>
-      <c r="J17" s="128"/>
+      <c r="D17" s="130"/>
+      <c r="E17" s="130"/>
+      <c r="F17" s="130"/>
+      <c r="G17" s="130"/>
+      <c r="H17" s="130"/>
+      <c r="I17" s="130"/>
+      <c r="J17" s="126"/>
     </row>
     <row r="18" spans="1:10" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="90" t="s">
@@ -4491,13 +4592,13 @@
       <c r="B18" s="91" t="s">
         <v>315</v>
       </c>
-      <c r="C18" s="163"/>
-      <c r="D18" s="141"/>
-      <c r="E18" s="141"/>
-      <c r="F18" s="141"/>
-      <c r="G18" s="141"/>
-      <c r="H18" s="141"/>
-      <c r="I18" s="142"/>
+      <c r="C18" s="139"/>
+      <c r="D18" s="140"/>
+      <c r="E18" s="140"/>
+      <c r="F18" s="140"/>
+      <c r="G18" s="140"/>
+      <c r="H18" s="140"/>
+      <c r="I18" s="138"/>
       <c r="J18" s="46" t="s">
         <v>313</v>
       </c>
@@ -4509,14 +4610,14 @@
       <c r="B19" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="C19" s="124" t="s">
+      <c r="C19" s="117" t="s">
         <v>279</v>
       </c>
-      <c r="D19" s="125"/>
-      <c r="E19" s="125"/>
-      <c r="F19" s="125"/>
-      <c r="G19" s="125"/>
-      <c r="H19" s="126"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="118"/>
+      <c r="F19" s="118"/>
+      <c r="G19" s="118"/>
+      <c r="H19" s="119"/>
       <c r="I19" s="81"/>
       <c r="J19" s="62" t="s">
         <v>280</v>
@@ -4529,16 +4630,16 @@
       <c r="B20" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C20" s="114" t="s">
+      <c r="C20" s="127" t="s">
         <v>146</v>
       </c>
-      <c r="D20" s="115"/>
-      <c r="E20" s="115"/>
-      <c r="F20" s="115"/>
-      <c r="G20" s="115"/>
-      <c r="H20" s="115"/>
-      <c r="I20" s="115"/>
-      <c r="J20" s="116"/>
+      <c r="D20" s="128"/>
+      <c r="E20" s="128"/>
+      <c r="F20" s="128"/>
+      <c r="G20" s="128"/>
+      <c r="H20" s="128"/>
+      <c r="I20" s="128"/>
+      <c r="J20" s="129"/>
     </row>
     <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
@@ -4547,16 +4648,16 @@
       <c r="B21" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="C21" s="114" t="s">
+      <c r="C21" s="127" t="s">
         <v>143</v>
       </c>
-      <c r="D21" s="115"/>
-      <c r="E21" s="115"/>
-      <c r="F21" s="115"/>
-      <c r="G21" s="115"/>
-      <c r="H21" s="115"/>
-      <c r="I21" s="115"/>
-      <c r="J21" s="116"/>
+      <c r="D21" s="128"/>
+      <c r="E21" s="128"/>
+      <c r="F21" s="128"/>
+      <c r="G21" s="128"/>
+      <c r="H21" s="128"/>
+      <c r="I21" s="128"/>
+      <c r="J21" s="129"/>
     </row>
     <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
@@ -4565,16 +4666,16 @@
       <c r="B22" s="40" t="s">
         <v>200</v>
       </c>
-      <c r="C22" s="114" t="s">
+      <c r="C22" s="127" t="s">
         <v>201</v>
       </c>
-      <c r="D22" s="115"/>
-      <c r="E22" s="115"/>
-      <c r="F22" s="115"/>
-      <c r="G22" s="115"/>
-      <c r="H22" s="115"/>
-      <c r="I22" s="115"/>
-      <c r="J22" s="116"/>
+      <c r="D22" s="128"/>
+      <c r="E22" s="128"/>
+      <c r="F22" s="128"/>
+      <c r="G22" s="128"/>
+      <c r="H22" s="128"/>
+      <c r="I22" s="128"/>
+      <c r="J22" s="129"/>
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
@@ -4583,16 +4684,16 @@
       <c r="B23" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="C23" s="114" t="s">
+      <c r="C23" s="127" t="s">
         <v>140</v>
       </c>
-      <c r="D23" s="115"/>
-      <c r="E23" s="115"/>
-      <c r="F23" s="115"/>
-      <c r="G23" s="115"/>
-      <c r="H23" s="115"/>
-      <c r="I23" s="115"/>
-      <c r="J23" s="116"/>
+      <c r="D23" s="128"/>
+      <c r="E23" s="128"/>
+      <c r="F23" s="128"/>
+      <c r="G23" s="128"/>
+      <c r="H23" s="128"/>
+      <c r="I23" s="128"/>
+      <c r="J23" s="129"/>
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
@@ -4601,16 +4702,16 @@
       <c r="B24" s="40" t="s">
         <v>203</v>
       </c>
-      <c r="C24" s="114" t="s">
+      <c r="C24" s="127" t="s">
         <v>204</v>
       </c>
-      <c r="D24" s="115"/>
-      <c r="E24" s="115"/>
-      <c r="F24" s="115"/>
-      <c r="G24" s="115"/>
-      <c r="H24" s="115"/>
-      <c r="I24" s="115"/>
-      <c r="J24" s="116"/>
+      <c r="D24" s="128"/>
+      <c r="E24" s="128"/>
+      <c r="F24" s="128"/>
+      <c r="G24" s="128"/>
+      <c r="H24" s="128"/>
+      <c r="I24" s="128"/>
+      <c r="J24" s="129"/>
     </row>
     <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
@@ -4619,16 +4720,16 @@
       <c r="B25" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="C25" s="114" t="s">
+      <c r="C25" s="127" t="s">
         <v>137</v>
       </c>
-      <c r="D25" s="115"/>
-      <c r="E25" s="115"/>
-      <c r="F25" s="115"/>
-      <c r="G25" s="115"/>
-      <c r="H25" s="115"/>
-      <c r="I25" s="115"/>
-      <c r="J25" s="116"/>
+      <c r="D25" s="128"/>
+      <c r="E25" s="128"/>
+      <c r="F25" s="128"/>
+      <c r="G25" s="128"/>
+      <c r="H25" s="128"/>
+      <c r="I25" s="128"/>
+      <c r="J25" s="129"/>
     </row>
     <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
@@ -4637,16 +4738,16 @@
       <c r="B26" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="C26" s="114" t="s">
+      <c r="C26" s="127" t="s">
         <v>134</v>
       </c>
-      <c r="D26" s="115"/>
-      <c r="E26" s="115"/>
-      <c r="F26" s="115"/>
-      <c r="G26" s="115"/>
-      <c r="H26" s="115"/>
-      <c r="I26" s="115"/>
-      <c r="J26" s="116"/>
+      <c r="D26" s="128"/>
+      <c r="E26" s="128"/>
+      <c r="F26" s="128"/>
+      <c r="G26" s="128"/>
+      <c r="H26" s="128"/>
+      <c r="I26" s="128"/>
+      <c r="J26" s="129"/>
     </row>
     <row r="27" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="39" t="s">
@@ -4665,8 +4766,8 @@
       <c r="F27" s="45" t="s">
         <v>208</v>
       </c>
-      <c r="G27" s="156"/>
-      <c r="H27" s="157"/>
+      <c r="G27" s="152"/>
+      <c r="H27" s="153"/>
       <c r="I27" s="36" t="s">
         <v>295</v>
       </c>
@@ -4674,43 +4775,43 @@
         <v>242</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
         <v>130</v>
       </c>
       <c r="B28" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="C28" s="159" t="s">
+      <c r="C28" s="154" t="s">
         <v>128</v>
       </c>
-      <c r="D28" s="160"/>
-      <c r="E28" s="160"/>
-      <c r="F28" s="160"/>
-      <c r="G28" s="160"/>
-      <c r="H28" s="160"/>
-      <c r="I28" s="160"/>
-      <c r="J28" s="161"/>
-    </row>
-    <row r="29" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="155"/>
+      <c r="E28" s="155"/>
+      <c r="F28" s="155"/>
+      <c r="G28" s="155"/>
+      <c r="H28" s="155"/>
+      <c r="I28" s="155"/>
+      <c r="J28" s="156"/>
+    </row>
+    <row r="29" spans="1:10" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
         <v>127</v>
       </c>
       <c r="B29" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="C29" s="139" t="s">
+      <c r="C29" s="146" t="s">
         <v>125</v>
       </c>
-      <c r="D29" s="152"/>
-      <c r="E29" s="152"/>
-      <c r="F29" s="152"/>
-      <c r="G29" s="152"/>
-      <c r="H29" s="152"/>
-      <c r="I29" s="153"/>
-      <c r="J29" s="127"/>
-    </row>
-    <row r="30" spans="1:10" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="147"/>
+      <c r="E29" s="147"/>
+      <c r="F29" s="147"/>
+      <c r="G29" s="147"/>
+      <c r="H29" s="147"/>
+      <c r="I29" s="148"/>
+      <c r="J29" s="124"/>
+    </row>
+    <row r="30" spans="1:10" ht="105" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="34" t="s">
         <v>124</v>
       </c>
@@ -4720,21 +4821,21 @@
       <c r="C30" s="53" t="s">
         <v>122</v>
       </c>
-      <c r="D30" s="132"/>
-      <c r="E30" s="133"/>
+      <c r="D30" s="150"/>
+      <c r="E30" s="151"/>
       <c r="F30" s="41" t="s">
         <v>121</v>
       </c>
       <c r="G30" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="H30" s="155"/>
+      <c r="H30" s="137"/>
       <c r="I30" s="61" t="s">
         <v>248</v>
       </c>
-      <c r="J30" s="162"/>
-    </row>
-    <row r="31" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="J30" s="125"/>
+    </row>
+    <row r="31" spans="1:10" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
         <v>119</v>
       </c>
@@ -4756,73 +4857,73 @@
       <c r="G31" s="60" t="s">
         <v>113</v>
       </c>
-      <c r="H31" s="122"/>
+      <c r="H31" s="149"/>
       <c r="I31" s="61" t="s">
         <v>250</v>
       </c>
-      <c r="J31" s="128"/>
-    </row>
-    <row r="32" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J31" s="126"/>
+    </row>
+    <row r="32" spans="1:10" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
         <v>216</v>
       </c>
       <c r="B32" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="C32" s="114" t="s">
+      <c r="C32" s="127" t="s">
         <v>218</v>
       </c>
-      <c r="D32" s="115"/>
-      <c r="E32" s="115"/>
-      <c r="F32" s="115"/>
-      <c r="G32" s="115"/>
-      <c r="H32" s="116"/>
+      <c r="D32" s="128"/>
+      <c r="E32" s="128"/>
+      <c r="F32" s="128"/>
+      <c r="G32" s="128"/>
+      <c r="H32" s="129"/>
       <c r="I32" s="83"/>
       <c r="J32" s="70" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
         <v>252</v>
       </c>
       <c r="B33" s="23" t="s">
         <v>253</v>
       </c>
-      <c r="C33" s="114" t="s">
+      <c r="C33" s="127" t="s">
         <v>255</v>
       </c>
-      <c r="D33" s="115"/>
-      <c r="E33" s="115"/>
-      <c r="F33" s="115"/>
-      <c r="G33" s="115"/>
-      <c r="H33" s="116"/>
+      <c r="D33" s="128"/>
+      <c r="E33" s="128"/>
+      <c r="F33" s="128"/>
+      <c r="G33" s="128"/>
+      <c r="H33" s="129"/>
       <c r="I33" s="84"/>
       <c r="J33" s="70" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
         <v>214</v>
       </c>
       <c r="B34" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="C34" s="115" t="s">
+      <c r="C34" s="128" t="s">
         <v>215</v>
       </c>
-      <c r="D34" s="115"/>
-      <c r="E34" s="115"/>
-      <c r="F34" s="115"/>
-      <c r="G34" s="115"/>
-      <c r="H34" s="115"/>
+      <c r="D34" s="128"/>
+      <c r="E34" s="128"/>
+      <c r="F34" s="128"/>
+      <c r="G34" s="128"/>
+      <c r="H34" s="128"/>
       <c r="I34" s="84"/>
       <c r="J34" s="61" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="300" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="300" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
         <v>112</v>
       </c>
@@ -4852,7 +4953,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
         <v>106</v>
       </c>
@@ -4862,8 +4963,8 @@
       <c r="C36" s="50" t="s">
         <v>104</v>
       </c>
-      <c r="D36" s="155"/>
-      <c r="E36" s="142"/>
+      <c r="D36" s="137"/>
+      <c r="E36" s="138"/>
       <c r="F36" s="21" t="s">
         <v>103</v>
       </c>
@@ -4876,27 +4977,27 @@
         <v>297</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="240" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>101</v>
       </c>
       <c r="B37" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C37" s="117"/>
-      <c r="D37" s="118"/>
+      <c r="C37" s="167"/>
+      <c r="D37" s="135"/>
       <c r="E37" s="63" t="s">
         <v>273</v>
       </c>
-      <c r="F37" s="122"/>
-      <c r="G37" s="118"/>
-      <c r="H37" s="118"/>
-      <c r="I37" s="123"/>
+      <c r="F37" s="149"/>
+      <c r="G37" s="135"/>
+      <c r="H37" s="135"/>
+      <c r="I37" s="171"/>
       <c r="J37" s="61" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
         <v>99</v>
       </c>
@@ -4906,10 +5007,10 @@
       <c r="C38" s="50" t="s">
         <v>205</v>
       </c>
-      <c r="D38" s="112"/>
-      <c r="E38" s="158"/>
-      <c r="F38" s="158"/>
-      <c r="G38" s="113"/>
+      <c r="D38" s="134"/>
+      <c r="E38" s="136"/>
+      <c r="F38" s="136"/>
+      <c r="G38" s="145"/>
       <c r="H38" s="21" t="s">
         <v>206</v>
       </c>
@@ -4920,61 +5021,61 @@
         <v>298</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="137" t="s">
+    <row r="39" spans="1:10" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="141" t="s">
         <v>97</v>
       </c>
-      <c r="B39" s="148" t="s">
+      <c r="B39" s="143" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="114" t="s">
+      <c r="C39" s="127" t="s">
         <v>95</v>
       </c>
-      <c r="D39" s="115"/>
-      <c r="E39" s="115"/>
-      <c r="F39" s="115"/>
-      <c r="G39" s="115"/>
-      <c r="H39" s="115"/>
+      <c r="D39" s="128"/>
+      <c r="E39" s="128"/>
+      <c r="F39" s="128"/>
+      <c r="G39" s="128"/>
+      <c r="H39" s="128"/>
       <c r="I39" s="68" t="s">
         <v>265</v>
       </c>
       <c r="J39" s="59"/>
     </row>
-    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="138"/>
-      <c r="B40" s="140"/>
-      <c r="C40" s="124" t="s">
+    <row r="40" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="142"/>
+      <c r="B40" s="144"/>
+      <c r="C40" s="117" t="s">
         <v>94</v>
       </c>
-      <c r="D40" s="125"/>
-      <c r="E40" s="125"/>
-      <c r="F40" s="125"/>
-      <c r="G40" s="125"/>
-      <c r="H40" s="125"/>
-      <c r="I40" s="125"/>
-      <c r="J40" s="126"/>
-    </row>
-    <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="137" t="s">
+      <c r="D40" s="118"/>
+      <c r="E40" s="118"/>
+      <c r="F40" s="118"/>
+      <c r="G40" s="118"/>
+      <c r="H40" s="118"/>
+      <c r="I40" s="118"/>
+      <c r="J40" s="119"/>
+    </row>
+    <row r="41" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="141" t="s">
         <v>219</v>
       </c>
-      <c r="B41" s="148" t="s">
+      <c r="B41" s="143" t="s">
         <v>227</v>
       </c>
-      <c r="C41" s="124" t="s">
+      <c r="C41" s="117" t="s">
         <v>221</v>
       </c>
-      <c r="D41" s="125"/>
-      <c r="E41" s="125"/>
-      <c r="F41" s="125"/>
-      <c r="G41" s="125"/>
-      <c r="H41" s="125"/>
-      <c r="I41" s="125"/>
-      <c r="J41" s="126"/>
-    </row>
-    <row r="42" spans="1:10" ht="285" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="138"/>
-      <c r="B42" s="143"/>
+      <c r="D41" s="118"/>
+      <c r="E41" s="118"/>
+      <c r="F41" s="118"/>
+      <c r="G41" s="118"/>
+      <c r="H41" s="118"/>
+      <c r="I41" s="118"/>
+      <c r="J41" s="119"/>
+    </row>
+    <row r="42" spans="1:10" ht="285" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="142"/>
+      <c r="B42" s="160"/>
       <c r="C42" s="53" t="s">
         <v>222</v>
       </c>
@@ -4998,7 +5099,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="330" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="330" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
         <v>220</v>
       </c>
@@ -5023,10 +5124,10 @@
       <c r="H43" s="54" t="s">
         <v>230</v>
       </c>
-      <c r="I43" s="122"/>
-      <c r="J43" s="123"/>
-    </row>
-    <row r="44" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I43" s="149"/>
+      <c r="J43" s="171"/>
+    </row>
+    <row r="44" spans="1:10" ht="120" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="24" t="s">
         <v>93</v>
       </c>
@@ -5058,27 +5159,27 @@
         <v>301</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="137" t="s">
+    <row r="45" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="141" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="148" t="s">
+      <c r="B45" s="143" t="s">
         <v>86</v>
       </c>
-      <c r="C45" s="114" t="s">
+      <c r="C45" s="127" t="s">
         <v>282</v>
       </c>
-      <c r="D45" s="115"/>
-      <c r="E45" s="115"/>
-      <c r="F45" s="115"/>
-      <c r="G45" s="115"/>
-      <c r="H45" s="115"/>
-      <c r="I45" s="116"/>
-      <c r="J45" s="127"/>
-    </row>
-    <row r="46" spans="1:10" ht="195" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="138"/>
-      <c r="B46" s="140"/>
+      <c r="D45" s="128"/>
+      <c r="E45" s="128"/>
+      <c r="F45" s="128"/>
+      <c r="G45" s="128"/>
+      <c r="H45" s="128"/>
+      <c r="I45" s="129"/>
+      <c r="J45" s="124"/>
+    </row>
+    <row r="46" spans="1:10" ht="195" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="142"/>
+      <c r="B46" s="144"/>
       <c r="C46" s="22" t="s">
         <v>285</v>
       </c>
@@ -5100,47 +5201,47 @@
       <c r="I46" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="J46" s="128"/>
-    </row>
-    <row r="47" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="137" t="s">
+      <c r="J46" s="126"/>
+    </row>
+    <row r="47" spans="1:10" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="141" t="s">
         <v>84</v>
       </c>
-      <c r="B47" s="148" t="s">
+      <c r="B47" s="143" t="s">
         <v>83</v>
       </c>
-      <c r="C47" s="149" t="s">
+      <c r="C47" s="164" t="s">
         <v>237</v>
       </c>
-      <c r="D47" s="150"/>
-      <c r="E47" s="150"/>
-      <c r="F47" s="150"/>
-      <c r="G47" s="150"/>
-      <c r="H47" s="151"/>
-      <c r="I47" s="119"/>
-      <c r="J47" s="129" t="s">
+      <c r="D47" s="165"/>
+      <c r="E47" s="165"/>
+      <c r="F47" s="165"/>
+      <c r="G47" s="165"/>
+      <c r="H47" s="166"/>
+      <c r="I47" s="168"/>
+      <c r="J47" s="172" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="300" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="138"/>
-      <c r="B48" s="140"/>
+    <row r="48" spans="1:10" ht="300" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="142"/>
+      <c r="B48" s="144"/>
       <c r="C48" s="50" t="s">
         <v>82</v>
       </c>
       <c r="D48" s="4"/>
-      <c r="E48" s="121" t="s">
+      <c r="E48" s="170" t="s">
         <v>81</v>
       </c>
-      <c r="F48" s="116"/>
+      <c r="F48" s="129"/>
       <c r="G48" s="4"/>
       <c r="H48" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="I48" s="120"/>
-      <c r="J48" s="130"/>
-    </row>
-    <row r="49" spans="1:10" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I48" s="169"/>
+      <c r="J48" s="173"/>
+    </row>
+    <row r="49" spans="1:10" ht="195" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
         <v>79</v>
       </c>
@@ -5172,7 +5273,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="105" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
         <v>71</v>
       </c>
@@ -5204,36 +5305,36 @@
         <v>304</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="137" t="s">
+    <row r="51" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="141" t="s">
         <v>63</v>
       </c>
-      <c r="B51" s="139" t="s">
+      <c r="B51" s="146" t="s">
         <v>62</v>
       </c>
-      <c r="C51" s="131" t="s">
+      <c r="C51" s="174" t="s">
         <v>269</v>
       </c>
-      <c r="D51" s="131"/>
-      <c r="E51" s="131"/>
-      <c r="F51" s="131"/>
-      <c r="G51" s="131"/>
-      <c r="H51" s="131"/>
-      <c r="I51" s="132"/>
-      <c r="J51" s="133"/>
-    </row>
-    <row r="52" spans="1:10" ht="345" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="138"/>
-      <c r="B52" s="140"/>
+      <c r="D51" s="174"/>
+      <c r="E51" s="174"/>
+      <c r="F51" s="174"/>
+      <c r="G51" s="174"/>
+      <c r="H51" s="174"/>
+      <c r="I51" s="150"/>
+      <c r="J51" s="151"/>
+    </row>
+    <row r="52" spans="1:10" ht="345" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="142"/>
+      <c r="B52" s="144"/>
       <c r="C52" s="26" t="s">
         <v>268</v>
       </c>
       <c r="D52" s="25" t="s">
         <v>270</v>
       </c>
-      <c r="E52" s="132"/>
-      <c r="F52" s="141"/>
-      <c r="G52" s="142"/>
+      <c r="E52" s="150"/>
+      <c r="F52" s="140"/>
+      <c r="G52" s="138"/>
       <c r="H52" s="57" t="s">
         <v>271</v>
       </c>
@@ -5244,7 +5345,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="345" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="345" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="24" t="s">
         <v>61</v>
       </c>
@@ -5260,8 +5361,8 @@
       <c r="E53" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="F53" s="112"/>
-      <c r="G53" s="113"/>
+      <c r="F53" s="134"/>
+      <c r="G53" s="145"/>
       <c r="H53" s="28" t="s">
         <v>210</v>
       </c>
@@ -5270,7 +5371,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="405" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="405" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
         <v>58</v>
       </c>
@@ -5302,28 +5403,35 @@
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="J11:J17"/>
-    <mergeCell ref="C20:J20"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="C34:H34"/>
-    <mergeCell ref="C21:J21"/>
-    <mergeCell ref="C22:J22"/>
-    <mergeCell ref="D12:H12"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="C18:I18"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:H39"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="C45:I45"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="I47:I48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="C40:J40"/>
+    <mergeCell ref="C41:J41"/>
+    <mergeCell ref="J45:J46"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="C51:H51"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="C8:J8"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="C15:I15"/>
+    <mergeCell ref="C17:I17"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="C47:H47"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="C29:I29"/>
     <mergeCell ref="C33:H33"/>
@@ -5340,35 +5448,28 @@
     <mergeCell ref="C26:J26"/>
     <mergeCell ref="C28:J28"/>
     <mergeCell ref="J29:J31"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="C8:J8"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="C15:I15"/>
-    <mergeCell ref="C17:I17"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="C47:H47"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="C45:I45"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="I47:I48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="C40:J40"/>
-    <mergeCell ref="C41:J41"/>
-    <mergeCell ref="J45:J46"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="J47:J48"/>
-    <mergeCell ref="C51:H51"/>
-    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="C34:H34"/>
+    <mergeCell ref="C21:J21"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="D12:H12"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="C18:I18"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="J11:J17"/>
+    <mergeCell ref="C20:J20"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="A14:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5380,10 +5481,10 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4:J4"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5432,326 +5533,326 @@
       <c r="M1" s="97"/>
     </row>
     <row r="2" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="194" t="s">
         <v>198</v>
       </c>
-      <c r="B2" s="170" t="s">
+      <c r="B2" s="193" t="s">
         <v>309</v>
       </c>
-      <c r="C2" s="173" t="s">
+      <c r="C2" s="196" t="s">
         <v>340</v>
       </c>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="174"/>
-      <c r="I2" s="174"/>
-      <c r="J2" s="174"/>
+      <c r="D2" s="197"/>
+      <c r="E2" s="197"/>
+      <c r="F2" s="197"/>
+      <c r="G2" s="197"/>
+      <c r="H2" s="197"/>
+      <c r="I2" s="197"/>
+      <c r="J2" s="197"/>
       <c r="K2" s="97"/>
       <c r="L2" s="97"/>
       <c r="M2" s="97"/>
     </row>
     <row r="3" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="172"/>
-      <c r="B3" s="140"/>
-      <c r="C3" s="191"/>
-      <c r="D3" s="133"/>
+      <c r="A3" s="195"/>
+      <c r="B3" s="144"/>
+      <c r="C3" s="189"/>
+      <c r="D3" s="151"/>
       <c r="E3" s="46" t="s">
-        <v>354</v>
-      </c>
-      <c r="F3" s="132"/>
+        <v>353</v>
+      </c>
+      <c r="F3" s="150"/>
       <c r="G3" s="190"/>
       <c r="H3" s="190"/>
-      <c r="I3" s="133"/>
-      <c r="J3" s="192" t="s">
-        <v>359</v>
+      <c r="I3" s="151"/>
+      <c r="J3" s="111" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="175" t="s">
+      <c r="A4" s="191" t="s">
         <v>197</v>
       </c>
-      <c r="B4" s="176" t="s">
+      <c r="B4" s="181" t="s">
         <v>310</v>
       </c>
-      <c r="C4" s="177" t="s">
+      <c r="C4" s="187" t="s">
         <v>339</v>
       </c>
-      <c r="D4" s="178"/>
-      <c r="E4" s="178"/>
-      <c r="F4" s="178"/>
-      <c r="G4" s="178"/>
-      <c r="H4" s="178"/>
-      <c r="I4" s="178"/>
-      <c r="J4" s="178"/>
+      <c r="D4" s="188"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
+      <c r="I4" s="188"/>
+      <c r="J4" s="188"/>
       <c r="K4" s="97"/>
       <c r="L4" s="97"/>
       <c r="M4" s="97"/>
     </row>
     <row r="5" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="165"/>
-      <c r="B5" s="167"/>
-      <c r="C5" s="191"/>
+      <c r="A5" s="121"/>
+      <c r="B5" s="123"/>
+      <c r="C5" s="189"/>
       <c r="D5" s="190"/>
       <c r="E5" s="190"/>
       <c r="F5" s="190"/>
-      <c r="G5" s="133"/>
+      <c r="G5" s="151"/>
       <c r="H5" s="46" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="I5" s="58"/>
-      <c r="J5" s="192" t="s">
-        <v>358</v>
+      <c r="J5" s="111" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="175" t="s">
+      <c r="A6" s="191" t="s">
         <v>196</v>
       </c>
-      <c r="B6" s="176" t="s">
+      <c r="B6" s="181" t="s">
         <v>311</v>
       </c>
-      <c r="C6" s="177" t="s">
+      <c r="C6" s="187" t="s">
         <v>338</v>
       </c>
-      <c r="D6" s="178"/>
-      <c r="E6" s="178"/>
-      <c r="F6" s="178"/>
-      <c r="G6" s="178"/>
-      <c r="H6" s="178"/>
-      <c r="I6" s="178"/>
-      <c r="J6" s="178"/>
+      <c r="D6" s="188"/>
+      <c r="E6" s="188"/>
+      <c r="F6" s="188"/>
+      <c r="G6" s="188"/>
+      <c r="H6" s="188"/>
+      <c r="I6" s="188"/>
+      <c r="J6" s="188"/>
       <c r="K6" s="97"/>
       <c r="L6" s="97"/>
       <c r="M6" s="97"/>
     </row>
     <row r="7" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="165"/>
-      <c r="B7" s="167"/>
-      <c r="C7" s="191"/>
+      <c r="A7" s="121"/>
+      <c r="B7" s="123"/>
+      <c r="C7" s="189"/>
       <c r="D7" s="190"/>
-      <c r="E7" s="133"/>
+      <c r="E7" s="151"/>
       <c r="F7" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="G7" s="132"/>
+      <c r="G7" s="150"/>
       <c r="H7" s="190"/>
-      <c r="I7" s="133"/>
-      <c r="J7" s="192" t="s">
-        <v>357</v>
+      <c r="I7" s="151"/>
+      <c r="J7" s="111" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="164" t="s">
+      <c r="A8" s="120" t="s">
         <v>195</v>
       </c>
-      <c r="B8" s="166" t="s">
+      <c r="B8" s="122" t="s">
         <v>312</v>
       </c>
-      <c r="C8" s="177" t="s">
+      <c r="C8" s="187" t="s">
         <v>337</v>
       </c>
-      <c r="D8" s="178"/>
-      <c r="E8" s="178"/>
-      <c r="F8" s="178"/>
-      <c r="G8" s="178"/>
-      <c r="H8" s="178"/>
-      <c r="I8" s="178"/>
-      <c r="J8" s="178"/>
+      <c r="D8" s="188"/>
+      <c r="E8" s="188"/>
+      <c r="F8" s="188"/>
+      <c r="G8" s="188"/>
+      <c r="H8" s="188"/>
+      <c r="I8" s="188"/>
+      <c r="J8" s="188"/>
       <c r="K8" s="97"/>
       <c r="L8" s="97"/>
       <c r="M8" s="97"/>
     </row>
     <row r="9" spans="1:13" s="96" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="179"/>
-      <c r="B9" s="180"/>
+      <c r="A9" s="192"/>
+      <c r="B9" s="182"/>
       <c r="C9" s="94"/>
-      <c r="D9" s="189" t="s">
-        <v>363</v>
-      </c>
-      <c r="E9" s="156"/>
-      <c r="F9" s="157"/>
-      <c r="G9" s="157"/>
-      <c r="H9" s="157"/>
-      <c r="I9" s="157"/>
-      <c r="J9" s="193" t="s">
-        <v>356</v>
+      <c r="D9" s="110" t="s">
+        <v>361</v>
+      </c>
+      <c r="E9" s="152"/>
+      <c r="F9" s="153"/>
+      <c r="G9" s="153"/>
+      <c r="H9" s="153"/>
+      <c r="I9" s="153"/>
+      <c r="J9" s="112" t="s">
+        <v>355</v>
       </c>
       <c r="K9" s="100"/>
       <c r="L9" s="100"/>
       <c r="M9" s="100"/>
     </row>
     <row r="10" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="181" t="s">
+      <c r="A10" s="179" t="s">
         <v>194</v>
       </c>
-      <c r="B10" s="176" t="s">
+      <c r="B10" s="181" t="s">
         <v>324</v>
       </c>
-      <c r="C10" s="177" t="s">
+      <c r="C10" s="187" t="s">
         <v>336</v>
       </c>
-      <c r="D10" s="178"/>
-      <c r="E10" s="178"/>
-      <c r="F10" s="178"/>
-      <c r="G10" s="178"/>
-      <c r="H10" s="178"/>
-      <c r="I10" s="178"/>
-      <c r="J10" s="178"/>
+      <c r="D10" s="188"/>
+      <c r="E10" s="188"/>
+      <c r="F10" s="188"/>
+      <c r="G10" s="188"/>
+      <c r="H10" s="188"/>
+      <c r="I10" s="188"/>
+      <c r="J10" s="188"/>
       <c r="K10" s="97"/>
       <c r="L10" s="97"/>
       <c r="M10" s="97"/>
     </row>
     <row r="11" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="182"/>
-      <c r="B11" s="167"/>
+      <c r="A11" s="186"/>
+      <c r="B11" s="123"/>
       <c r="C11" s="108" t="s">
-        <v>353</v>
-      </c>
-      <c r="D11" s="132"/>
+        <v>352</v>
+      </c>
+      <c r="D11" s="150"/>
       <c r="E11" s="190"/>
       <c r="F11" s="190"/>
       <c r="G11" s="190"/>
       <c r="H11" s="190"/>
       <c r="I11" s="190"/>
-      <c r="J11" s="192" t="s">
-        <v>355</v>
+      <c r="J11" s="111" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="181" t="s">
+      <c r="A12" s="179" t="s">
         <v>193</v>
       </c>
-      <c r="B12" s="176" t="s">
+      <c r="B12" s="181" t="s">
         <v>323</v>
       </c>
-      <c r="C12" s="183" t="s">
+      <c r="C12" s="177" t="s">
         <v>335</v>
       </c>
-      <c r="D12" s="184"/>
-      <c r="E12" s="184"/>
-      <c r="F12" s="184"/>
-      <c r="G12" s="184"/>
-      <c r="H12" s="184"/>
-      <c r="I12" s="184"/>
-      <c r="J12" s="184"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="178"/>
+      <c r="F12" s="178"/>
+      <c r="G12" s="178"/>
+      <c r="H12" s="178"/>
+      <c r="I12" s="178"/>
+      <c r="J12" s="178"/>
       <c r="K12" s="97"/>
       <c r="L12" s="97"/>
       <c r="M12" s="97"/>
     </row>
     <row r="13" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="182"/>
-      <c r="B13" s="167"/>
-      <c r="C13" s="191"/>
+      <c r="A13" s="186"/>
+      <c r="B13" s="123"/>
+      <c r="C13" s="189"/>
       <c r="D13" s="190"/>
       <c r="E13" s="190"/>
-      <c r="F13" s="133"/>
+      <c r="F13" s="151"/>
       <c r="G13" s="46" t="s">
-        <v>364</v>
-      </c>
-      <c r="H13" s="132"/>
-      <c r="I13" s="133"/>
-      <c r="J13" s="194" t="s">
-        <v>360</v>
+        <v>362</v>
+      </c>
+      <c r="H13" s="150"/>
+      <c r="I13" s="151"/>
+      <c r="J13" s="113" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="181" t="s">
+      <c r="A14" s="179" t="s">
         <v>321</v>
       </c>
-      <c r="B14" s="176" t="s">
+      <c r="B14" s="181" t="s">
         <v>322</v>
       </c>
-      <c r="C14" s="177" t="s">
+      <c r="C14" s="187" t="s">
         <v>347</v>
       </c>
-      <c r="D14" s="178"/>
-      <c r="E14" s="178"/>
-      <c r="F14" s="178"/>
-      <c r="G14" s="178"/>
-      <c r="H14" s="178"/>
-      <c r="I14" s="178"/>
-      <c r="J14" s="178"/>
+      <c r="D14" s="188"/>
+      <c r="E14" s="188"/>
+      <c r="F14" s="188"/>
+      <c r="G14" s="188"/>
+      <c r="H14" s="188"/>
+      <c r="I14" s="188"/>
+      <c r="J14" s="188"/>
       <c r="K14" s="97"/>
       <c r="L14" s="97"/>
       <c r="M14" s="97"/>
     </row>
     <row r="15" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="182"/>
-      <c r="B15" s="167"/>
-      <c r="C15" s="191"/>
+      <c r="A15" s="186"/>
+      <c r="B15" s="123"/>
+      <c r="C15" s="189"/>
       <c r="D15" s="190"/>
       <c r="E15" s="190"/>
       <c r="F15" s="190"/>
       <c r="G15" s="190"/>
       <c r="H15" s="190"/>
-      <c r="I15" s="133"/>
+      <c r="I15" s="151"/>
       <c r="J15" s="56" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="181" t="s">
+      <c r="A16" s="179" t="s">
         <v>192</v>
       </c>
-      <c r="B16" s="176" t="s">
+      <c r="B16" s="181" t="s">
         <v>325</v>
       </c>
-      <c r="C16" s="177" t="s">
+      <c r="C16" s="187" t="s">
         <v>334</v>
       </c>
-      <c r="D16" s="178"/>
-      <c r="E16" s="178"/>
-      <c r="F16" s="178"/>
-      <c r="G16" s="178"/>
-      <c r="H16" s="178"/>
-      <c r="I16" s="178"/>
-      <c r="J16" s="178"/>
+      <c r="D16" s="188"/>
+      <c r="E16" s="188"/>
+      <c r="F16" s="188"/>
+      <c r="G16" s="188"/>
+      <c r="H16" s="188"/>
+      <c r="I16" s="188"/>
+      <c r="J16" s="188"/>
       <c r="K16" s="97"/>
       <c r="L16" s="97"/>
       <c r="M16" s="97"/>
     </row>
     <row r="17" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="182"/>
-      <c r="B17" s="167"/>
-      <c r="C17" s="191"/>
+      <c r="A17" s="186"/>
+      <c r="B17" s="123"/>
+      <c r="C17" s="189"/>
       <c r="D17" s="190"/>
       <c r="E17" s="190"/>
       <c r="F17" s="190"/>
       <c r="G17" s="190"/>
-      <c r="H17" s="133"/>
+      <c r="H17" s="151"/>
       <c r="I17" s="46" t="s">
-        <v>349</v>
+        <v>368</v>
       </c>
       <c r="J17" s="56" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="18" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="185" t="s">
+      <c r="A18" s="183" t="s">
         <v>191</v>
       </c>
-      <c r="B18" s="166" t="s">
+      <c r="B18" s="122" t="s">
         <v>327</v>
       </c>
-      <c r="C18" s="195" t="s">
+      <c r="C18" s="184" t="s">
         <v>330</v>
       </c>
-      <c r="D18" s="196"/>
-      <c r="E18" s="196"/>
-      <c r="F18" s="196"/>
-      <c r="G18" s="196"/>
-      <c r="H18" s="196"/>
-      <c r="I18" s="196"/>
-      <c r="J18" s="196"/>
+      <c r="D18" s="185"/>
+      <c r="E18" s="185"/>
+      <c r="F18" s="185"/>
+      <c r="G18" s="185"/>
+      <c r="H18" s="185"/>
+      <c r="I18" s="185"/>
+      <c r="J18" s="185"/>
       <c r="K18" s="97"/>
       <c r="L18" s="97"/>
       <c r="M18" s="97"/>
     </row>
     <row r="19" spans="1:13" s="100" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="186"/>
-      <c r="B19" s="140"/>
+      <c r="A19" s="176"/>
+      <c r="B19" s="144"/>
       <c r="C19" s="103" t="s">
         <v>342</v>
       </c>
@@ -5764,29 +5865,29 @@
       <c r="J19" s="106"/>
     </row>
     <row r="20" spans="1:13" s="101" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="187" t="s">
+      <c r="A20" s="175" t="s">
         <v>190</v>
       </c>
-      <c r="B20" s="148" t="s">
+      <c r="B20" s="143" t="s">
         <v>326</v>
       </c>
-      <c r="C20" s="183" t="s">
+      <c r="C20" s="177" t="s">
         <v>331</v>
       </c>
-      <c r="D20" s="184"/>
-      <c r="E20" s="184"/>
-      <c r="F20" s="184"/>
-      <c r="G20" s="184"/>
-      <c r="H20" s="184"/>
-      <c r="I20" s="184"/>
-      <c r="J20" s="184"/>
+      <c r="D20" s="178"/>
+      <c r="E20" s="178"/>
+      <c r="F20" s="178"/>
+      <c r="G20" s="178"/>
+      <c r="H20" s="178"/>
+      <c r="I20" s="178"/>
+      <c r="J20" s="178"/>
       <c r="K20" s="97"/>
       <c r="L20" s="97"/>
       <c r="M20" s="97"/>
     </row>
     <row r="21" spans="1:13" s="98" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="186"/>
-      <c r="B21" s="140"/>
+      <c r="A21" s="176"/>
+      <c r="B21" s="144"/>
       <c r="C21" s="103" t="s">
         <v>341</v>
       </c>
@@ -5802,29 +5903,29 @@
       <c r="M21" s="100"/>
     </row>
     <row r="22" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="187" t="s">
+      <c r="A22" s="175" t="s">
         <v>189</v>
       </c>
-      <c r="B22" s="148" t="s">
+      <c r="B22" s="143" t="s">
         <v>328</v>
       </c>
-      <c r="C22" s="183" t="s">
+      <c r="C22" s="177" t="s">
         <v>332</v>
       </c>
-      <c r="D22" s="184"/>
-      <c r="E22" s="184"/>
-      <c r="F22" s="184"/>
-      <c r="G22" s="184"/>
-      <c r="H22" s="184"/>
-      <c r="I22" s="184"/>
-      <c r="J22" s="184"/>
+      <c r="D22" s="178"/>
+      <c r="E22" s="178"/>
+      <c r="F22" s="178"/>
+      <c r="G22" s="178"/>
+      <c r="H22" s="178"/>
+      <c r="I22" s="178"/>
+      <c r="J22" s="178"/>
       <c r="K22" s="97"/>
       <c r="L22" s="97"/>
       <c r="M22" s="97"/>
     </row>
     <row r="23" spans="1:13" s="100" customFormat="1" ht="210" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="186"/>
-      <c r="B23" s="140"/>
+      <c r="A23" s="176"/>
+      <c r="B23" s="144"/>
       <c r="C23" s="103" t="s">
         <v>343</v>
       </c>
@@ -5837,41 +5938,41 @@
       <c r="J23" s="106"/>
     </row>
     <row r="24" spans="1:13" s="102" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="181" t="s">
+      <c r="A24" s="179" t="s">
         <v>188</v>
       </c>
-      <c r="B24" s="176" t="s">
+      <c r="B24" s="181" t="s">
         <v>329</v>
       </c>
-      <c r="C24" s="183" t="s">
+      <c r="C24" s="177" t="s">
         <v>333</v>
       </c>
-      <c r="D24" s="184"/>
-      <c r="E24" s="184"/>
-      <c r="F24" s="184"/>
-      <c r="G24" s="184"/>
-      <c r="H24" s="184"/>
-      <c r="I24" s="184"/>
-      <c r="J24" s="184"/>
+      <c r="D24" s="178"/>
+      <c r="E24" s="178"/>
+      <c r="F24" s="178"/>
+      <c r="G24" s="178"/>
+      <c r="H24" s="178"/>
+      <c r="I24" s="178"/>
+      <c r="J24" s="178"/>
       <c r="K24" s="97"/>
       <c r="L24" s="97"/>
       <c r="M24" s="97"/>
     </row>
     <row r="25" spans="1:13" s="96" customFormat="1" ht="300" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="188"/>
-      <c r="B25" s="180"/>
+      <c r="A25" s="180"/>
+      <c r="B25" s="182"/>
       <c r="C25" s="104" t="s">
         <v>344</v>
       </c>
-      <c r="D25" s="189" t="s">
-        <v>352</v>
+      <c r="D25" s="110" t="s">
+        <v>351</v>
       </c>
       <c r="E25" s="95"/>
       <c r="F25" s="95" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G25" s="95" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H25" s="104" t="s">
         <v>345</v>
@@ -5922,26 +6023,24 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:J22"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:J24"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:J18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:J20"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:J14"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:J16"/>
-    <mergeCell ref="C15:I15"/>
-    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:J8"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="E9:I9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:J10"/>
@@ -5951,24 +6050,26 @@
     <mergeCell ref="D11:I11"/>
     <mergeCell ref="H13:I13"/>
     <mergeCell ref="C13:F13"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:J8"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="E9:I9"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:J14"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:J16"/>
+    <mergeCell ref="C15:I15"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:J18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:J20"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:J24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
started working on a program to extract data from the 'Items and Components' excel file.
</commit_message>
<xml_diff>
--- a/Tags and Affinities.xlsx
+++ b/Tags and Affinities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Documents\Git Repositories\materials_and_crafting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC23F09-B9EA-4868-9A65-B2F6AB579A8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D75184-A8CD-4396-B714-69942CA85946}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{8FD76562-234B-40A6-8AC6-52675E21BBDC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{8FD76562-234B-40A6-8AC6-52675E21BBDC}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPONENT TAGS" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="529">
   <si>
     <t>This component's weapon can be wound up in preparation for a powerful strike, however its strikes take a while to rewind.</t>
   </si>
@@ -2478,12 +2478,6 @@
     <t>The bearer of this tattoo has all of their dice rolls averaged out, forcing them to always roll the middle value.</t>
   </si>
   <si>
-    <t>The bearer of this tattoo gains darkvision out to a range of 60 feet or has their darkvision increased by 30 feet. Magical darkness does not impede their darkvision.</t>
-  </si>
-  <si>
-    <t>&lt;Maddening Aura&gt;</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">The bearer of this tattoo permanently has the effect of the </t>
     </r>
@@ -3071,6 +3065,9 @@
       </rPr>
       <t xml:space="preserve"> spell on an air elemental, with a save DC equal to 10 + the headgear's auran affinity.</t>
     </r>
+  </si>
+  <si>
+    <t>The bearer of this tattoo gains darkvision out to a range of 30 feet or has their darkvision increased by 30 feet. Magical darkness does not impede their darkvision.</t>
   </si>
 </sst>
 </file>
@@ -4655,6 +4652,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -4664,58 +4727,196 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="81" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="75" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4724,305 +4925,101 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="75" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5342,7 +5339,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -5356,10 +5353,10 @@
   <sheetData>
     <row r="1" spans="1:11" s="16" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="18" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>381</v>
@@ -5399,14 +5396,14 @@
       <c r="C2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="155"/>
-      <c r="E2" s="156"/>
-      <c r="F2" s="156"/>
-      <c r="G2" s="156"/>
-      <c r="H2" s="156"/>
-      <c r="I2" s="156"/>
-      <c r="J2" s="156"/>
-      <c r="K2" s="157"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="178"/>
+      <c r="I2" s="178"/>
+      <c r="J2" s="178"/>
+      <c r="K2" s="179"/>
     </row>
     <row r="3" spans="1:11" ht="30">
       <c r="A3" s="10" t="s">
@@ -5418,48 +5415,48 @@
       <c r="C3" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="158"/>
-      <c r="E3" s="159"/>
-      <c r="F3" s="159"/>
-      <c r="G3" s="159"/>
-      <c r="H3" s="159"/>
-      <c r="I3" s="159"/>
-      <c r="J3" s="159"/>
-      <c r="K3" s="160"/>
+      <c r="D3" s="175"/>
+      <c r="E3" s="176"/>
+      <c r="F3" s="176"/>
+      <c r="G3" s="176"/>
+      <c r="H3" s="176"/>
+      <c r="I3" s="176"/>
+      <c r="J3" s="176"/>
+      <c r="K3" s="174"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="164" t="s">
+      <c r="A4" s="161" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="169" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="169" t="s">
+      <c r="C4" s="166" t="s">
         <v>311</v>
       </c>
-      <c r="D4" s="170"/>
-      <c r="E4" s="170"/>
-      <c r="F4" s="170"/>
-      <c r="G4" s="170"/>
-      <c r="H4" s="170"/>
-      <c r="I4" s="170"/>
-      <c r="J4" s="171"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
+      <c r="H4" s="167"/>
+      <c r="I4" s="167"/>
+      <c r="J4" s="168"/>
       <c r="K4" s="138"/>
     </row>
     <row r="5" spans="1:11" ht="30">
-      <c r="A5" s="165"/>
-      <c r="B5" s="173"/>
+      <c r="A5" s="162"/>
+      <c r="B5" s="170"/>
       <c r="C5" s="139" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="158"/>
-      <c r="E5" s="159"/>
-      <c r="F5" s="159"/>
-      <c r="G5" s="159"/>
-      <c r="H5" s="159"/>
-      <c r="I5" s="159"/>
-      <c r="J5" s="159"/>
-      <c r="K5" s="160"/>
+      <c r="D5" s="175"/>
+      <c r="E5" s="176"/>
+      <c r="F5" s="176"/>
+      <c r="G5" s="176"/>
+      <c r="H5" s="176"/>
+      <c r="I5" s="176"/>
+      <c r="J5" s="176"/>
+      <c r="K5" s="174"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="105" customHeight="1">
       <c r="A6" s="6" t="s">
@@ -5471,14 +5468,14 @@
       <c r="C6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="158"/>
-      <c r="E6" s="159"/>
-      <c r="F6" s="159"/>
-      <c r="G6" s="159"/>
-      <c r="H6" s="159"/>
-      <c r="I6" s="159"/>
-      <c r="J6" s="159"/>
-      <c r="K6" s="160"/>
+      <c r="D6" s="175"/>
+      <c r="E6" s="176"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="176"/>
+      <c r="H6" s="176"/>
+      <c r="I6" s="176"/>
+      <c r="J6" s="176"/>
+      <c r="K6" s="174"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="105" customHeight="1">
       <c r="A7" s="6" t="s">
@@ -5490,14 +5487,14 @@
       <c r="C7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="158"/>
-      <c r="E7" s="159"/>
-      <c r="F7" s="159"/>
-      <c r="G7" s="159"/>
-      <c r="H7" s="159"/>
-      <c r="I7" s="159"/>
-      <c r="J7" s="159"/>
-      <c r="K7" s="160"/>
+      <c r="D7" s="175"/>
+      <c r="E7" s="176"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="176"/>
+      <c r="H7" s="176"/>
+      <c r="I7" s="176"/>
+      <c r="J7" s="176"/>
+      <c r="K7" s="174"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="120" customHeight="1">
       <c r="A8" s="6" t="s">
@@ -5509,14 +5506,14 @@
       <c r="C8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="158"/>
-      <c r="E8" s="159"/>
-      <c r="F8" s="159"/>
-      <c r="G8" s="159"/>
-      <c r="H8" s="159"/>
-      <c r="I8" s="159"/>
-      <c r="J8" s="159"/>
-      <c r="K8" s="160"/>
+      <c r="D8" s="175"/>
+      <c r="E8" s="176"/>
+      <c r="F8" s="176"/>
+      <c r="G8" s="176"/>
+      <c r="H8" s="176"/>
+      <c r="I8" s="176"/>
+      <c r="J8" s="176"/>
+      <c r="K8" s="174"/>
     </row>
     <row r="9" spans="1:11" s="3" customFormat="1" ht="135" customHeight="1">
       <c r="A9" s="6" t="s">
@@ -5528,14 +5525,14 @@
       <c r="C9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="158"/>
-      <c r="E9" s="159"/>
-      <c r="F9" s="159"/>
-      <c r="G9" s="159"/>
-      <c r="H9" s="159"/>
-      <c r="I9" s="159"/>
-      <c r="J9" s="159"/>
-      <c r="K9" s="160"/>
+      <c r="D9" s="175"/>
+      <c r="E9" s="176"/>
+      <c r="F9" s="176"/>
+      <c r="G9" s="176"/>
+      <c r="H9" s="176"/>
+      <c r="I9" s="176"/>
+      <c r="J9" s="176"/>
+      <c r="K9" s="174"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="135" customHeight="1">
       <c r="A10" s="6" t="s">
@@ -5547,16 +5544,16 @@
       <c r="C10" s="83" t="s">
         <v>361</v>
       </c>
-      <c r="D10" s="158"/>
-      <c r="E10" s="159"/>
-      <c r="F10" s="159"/>
-      <c r="G10" s="159"/>
-      <c r="H10" s="160"/>
+      <c r="D10" s="175"/>
+      <c r="E10" s="176"/>
+      <c r="F10" s="176"/>
+      <c r="G10" s="176"/>
+      <c r="H10" s="174"/>
       <c r="I10" s="127" t="s">
         <v>360</v>
       </c>
-      <c r="J10" s="158"/>
-      <c r="K10" s="160"/>
+      <c r="J10" s="175"/>
+      <c r="K10" s="174"/>
     </row>
     <row r="11" spans="1:11" s="3" customFormat="1" ht="135" customHeight="1">
       <c r="A11" s="6" t="s">
@@ -5568,14 +5565,14 @@
       <c r="C11" s="89" t="s">
         <v>364</v>
       </c>
-      <c r="D11" s="158"/>
-      <c r="E11" s="159"/>
-      <c r="F11" s="159"/>
-      <c r="G11" s="159"/>
-      <c r="H11" s="159"/>
-      <c r="I11" s="159"/>
-      <c r="J11" s="159"/>
-      <c r="K11" s="160"/>
+      <c r="D11" s="175"/>
+      <c r="E11" s="176"/>
+      <c r="F11" s="176"/>
+      <c r="G11" s="176"/>
+      <c r="H11" s="176"/>
+      <c r="I11" s="176"/>
+      <c r="J11" s="176"/>
+      <c r="K11" s="174"/>
     </row>
     <row r="12" spans="1:11" s="3" customFormat="1" ht="135" customHeight="1">
       <c r="A12" s="6" t="s">
@@ -5584,36 +5581,36 @@
       <c r="B12" s="84" t="s">
         <v>348</v>
       </c>
-      <c r="C12" s="163"/>
-      <c r="D12" s="159"/>
-      <c r="E12" s="159"/>
-      <c r="F12" s="159"/>
-      <c r="G12" s="159"/>
-      <c r="H12" s="160"/>
+      <c r="C12" s="180"/>
+      <c r="D12" s="176"/>
+      <c r="E12" s="176"/>
+      <c r="F12" s="176"/>
+      <c r="G12" s="176"/>
+      <c r="H12" s="174"/>
       <c r="I12" s="127" t="s">
         <v>350</v>
       </c>
-      <c r="J12" s="158"/>
-      <c r="K12" s="160"/>
+      <c r="J12" s="175"/>
+      <c r="K12" s="174"/>
     </row>
     <row r="13" spans="1:11" s="3" customFormat="1" ht="180" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="141" t="s">
-        <v>515</v>
-      </c>
-      <c r="D13" s="158"/>
-      <c r="E13" s="159"/>
-      <c r="F13" s="159"/>
-      <c r="G13" s="159"/>
-      <c r="H13" s="159"/>
-      <c r="I13" s="159"/>
-      <c r="J13" s="159"/>
-      <c r="K13" s="160"/>
+        <v>513</v>
+      </c>
+      <c r="D13" s="175"/>
+      <c r="E13" s="176"/>
+      <c r="F13" s="176"/>
+      <c r="G13" s="176"/>
+      <c r="H13" s="176"/>
+      <c r="I13" s="176"/>
+      <c r="J13" s="176"/>
+      <c r="K13" s="174"/>
     </row>
     <row r="14" spans="1:11" s="3" customFormat="1" ht="90" customHeight="1">
       <c r="A14" s="6" t="s">
@@ -5625,52 +5622,52 @@
       <c r="C14" s="134" t="s">
         <v>274</v>
       </c>
-      <c r="D14" s="158"/>
-      <c r="E14" s="159"/>
-      <c r="F14" s="159"/>
-      <c r="G14" s="159"/>
-      <c r="H14" s="159"/>
-      <c r="I14" s="159"/>
-      <c r="J14" s="159"/>
-      <c r="K14" s="160"/>
+      <c r="D14" s="175"/>
+      <c r="E14" s="176"/>
+      <c r="F14" s="176"/>
+      <c r="G14" s="176"/>
+      <c r="H14" s="176"/>
+      <c r="I14" s="176"/>
+      <c r="J14" s="176"/>
+      <c r="K14" s="174"/>
     </row>
     <row r="15" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A15" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="B15" s="136" t="s">
+        <v>518</v>
+      </c>
+      <c r="C15" s="166" t="s">
         <v>519</v>
       </c>
-      <c r="B15" s="136" t="s">
-        <v>520</v>
-      </c>
-      <c r="C15" s="169" t="s">
-        <v>521</v>
-      </c>
-      <c r="D15" s="170"/>
-      <c r="E15" s="170"/>
-      <c r="F15" s="170"/>
-      <c r="G15" s="170"/>
-      <c r="H15" s="170"/>
-      <c r="I15" s="170"/>
-      <c r="J15" s="170"/>
-      <c r="K15" s="171"/>
+      <c r="D15" s="167"/>
+      <c r="E15" s="167"/>
+      <c r="F15" s="167"/>
+      <c r="G15" s="167"/>
+      <c r="H15" s="167"/>
+      <c r="I15" s="167"/>
+      <c r="J15" s="167"/>
+      <c r="K15" s="168"/>
     </row>
     <row r="16" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A16" s="6" t="s">
         <v>113</v>
       </c>
       <c r="B16" s="136" t="s">
-        <v>518</v>
-      </c>
-      <c r="C16" s="169" t="s">
         <v>516</v>
       </c>
-      <c r="D16" s="170"/>
-      <c r="E16" s="170"/>
-      <c r="F16" s="170"/>
-      <c r="G16" s="170"/>
-      <c r="H16" s="170"/>
-      <c r="I16" s="170"/>
-      <c r="J16" s="170"/>
-      <c r="K16" s="171"/>
+      <c r="C16" s="166" t="s">
+        <v>514</v>
+      </c>
+      <c r="D16" s="167"/>
+      <c r="E16" s="167"/>
+      <c r="F16" s="167"/>
+      <c r="G16" s="167"/>
+      <c r="H16" s="167"/>
+      <c r="I16" s="167"/>
+      <c r="J16" s="167"/>
+      <c r="K16" s="168"/>
     </row>
     <row r="17" spans="1:11" s="3" customFormat="1" ht="150" customHeight="1">
       <c r="A17" s="6" t="s">
@@ -5682,14 +5679,14 @@
       <c r="C17" s="135" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="158"/>
-      <c r="E17" s="159"/>
-      <c r="F17" s="159"/>
-      <c r="G17" s="159"/>
-      <c r="H17" s="159"/>
-      <c r="I17" s="159"/>
-      <c r="J17" s="159"/>
-      <c r="K17" s="160"/>
+      <c r="D17" s="175"/>
+      <c r="E17" s="176"/>
+      <c r="F17" s="176"/>
+      <c r="G17" s="176"/>
+      <c r="H17" s="176"/>
+      <c r="I17" s="176"/>
+      <c r="J17" s="176"/>
+      <c r="K17" s="174"/>
     </row>
     <row r="18" spans="1:11" s="3" customFormat="1" ht="60" customHeight="1">
       <c r="A18" s="6" t="s">
@@ -5701,14 +5698,14 @@
       <c r="C18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="158"/>
-      <c r="E18" s="159"/>
-      <c r="F18" s="159"/>
-      <c r="G18" s="159"/>
-      <c r="H18" s="159"/>
-      <c r="I18" s="159"/>
-      <c r="J18" s="159"/>
-      <c r="K18" s="160"/>
+      <c r="D18" s="175"/>
+      <c r="E18" s="176"/>
+      <c r="F18" s="176"/>
+      <c r="G18" s="176"/>
+      <c r="H18" s="176"/>
+      <c r="I18" s="176"/>
+      <c r="J18" s="176"/>
+      <c r="K18" s="174"/>
     </row>
     <row r="19" spans="1:11" s="3" customFormat="1" ht="60" customHeight="1">
       <c r="A19" s="6" t="s">
@@ -5720,14 +5717,14 @@
       <c r="C19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="158"/>
-      <c r="E19" s="159"/>
-      <c r="F19" s="159"/>
-      <c r="G19" s="159"/>
-      <c r="H19" s="159"/>
-      <c r="I19" s="159"/>
-      <c r="J19" s="159"/>
-      <c r="K19" s="160"/>
+      <c r="D19" s="175"/>
+      <c r="E19" s="176"/>
+      <c r="F19" s="176"/>
+      <c r="G19" s="176"/>
+      <c r="H19" s="176"/>
+      <c r="I19" s="176"/>
+      <c r="J19" s="176"/>
+      <c r="K19" s="174"/>
     </row>
     <row r="20" spans="1:11" s="3" customFormat="1" ht="60" customHeight="1">
       <c r="A20" s="6" t="s">
@@ -5739,14 +5736,14 @@
       <c r="C20" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="158"/>
-      <c r="E20" s="159"/>
-      <c r="F20" s="159"/>
-      <c r="G20" s="159"/>
-      <c r="H20" s="159"/>
-      <c r="I20" s="159"/>
-      <c r="J20" s="159"/>
-      <c r="K20" s="160"/>
+      <c r="D20" s="175"/>
+      <c r="E20" s="176"/>
+      <c r="F20" s="176"/>
+      <c r="G20" s="176"/>
+      <c r="H20" s="176"/>
+      <c r="I20" s="176"/>
+      <c r="J20" s="176"/>
+      <c r="K20" s="174"/>
     </row>
     <row r="21" spans="1:11" s="51" customFormat="1" ht="225" customHeight="1">
       <c r="A21" s="52" t="s">
@@ -5758,14 +5755,14 @@
       <c r="C21" s="49" t="s">
         <v>316</v>
       </c>
-      <c r="D21" s="158"/>
-      <c r="E21" s="159"/>
-      <c r="F21" s="159"/>
-      <c r="G21" s="159"/>
-      <c r="H21" s="159"/>
-      <c r="I21" s="159"/>
-      <c r="J21" s="159"/>
-      <c r="K21" s="160"/>
+      <c r="D21" s="175"/>
+      <c r="E21" s="176"/>
+      <c r="F21" s="176"/>
+      <c r="G21" s="176"/>
+      <c r="H21" s="176"/>
+      <c r="I21" s="176"/>
+      <c r="J21" s="176"/>
+      <c r="K21" s="174"/>
     </row>
     <row r="22" spans="1:11" s="51" customFormat="1" ht="225" customHeight="1">
       <c r="A22" s="64" t="s">
@@ -5777,18 +5774,18 @@
       <c r="C22" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="D22" s="174"/>
-      <c r="E22" s="162"/>
-      <c r="F22" s="162"/>
-      <c r="G22" s="175"/>
+      <c r="D22" s="171"/>
+      <c r="E22" s="172"/>
+      <c r="F22" s="172"/>
+      <c r="G22" s="173"/>
       <c r="H22" s="19" t="s">
         <v>211</v>
       </c>
       <c r="I22" s="126" t="s">
-        <v>475</v>
-      </c>
-      <c r="J22" s="174"/>
-      <c r="K22" s="160"/>
+        <v>473</v>
+      </c>
+      <c r="J22" s="171"/>
+      <c r="K22" s="174"/>
     </row>
     <row r="23" spans="1:11" s="51" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="77" t="s">
@@ -5797,16 +5794,16 @@
       <c r="B23" s="73" t="s">
         <v>310</v>
       </c>
-      <c r="C23" s="169" t="s">
+      <c r="C23" s="166" t="s">
         <v>309</v>
       </c>
-      <c r="D23" s="170"/>
-      <c r="E23" s="170"/>
-      <c r="F23" s="170"/>
-      <c r="G23" s="170"/>
-      <c r="H23" s="170"/>
-      <c r="I23" s="170"/>
-      <c r="J23" s="171"/>
+      <c r="D23" s="167"/>
+      <c r="E23" s="167"/>
+      <c r="F23" s="167"/>
+      <c r="G23" s="167"/>
+      <c r="H23" s="167"/>
+      <c r="I23" s="167"/>
+      <c r="J23" s="168"/>
       <c r="K23" s="69"/>
     </row>
     <row r="24" spans="1:11" ht="60">
@@ -5816,20 +5813,27 @@
       <c r="B24" s="55" t="s">
         <v>275</v>
       </c>
-      <c r="C24" s="166" t="s">
+      <c r="C24" s="163" t="s">
         <v>276</v>
       </c>
-      <c r="D24" s="167"/>
-      <c r="E24" s="167"/>
-      <c r="F24" s="167"/>
-      <c r="G24" s="167"/>
-      <c r="H24" s="167"/>
-      <c r="I24" s="167"/>
-      <c r="J24" s="168"/>
+      <c r="D24" s="164"/>
+      <c r="E24" s="164"/>
+      <c r="F24" s="164"/>
+      <c r="G24" s="164"/>
+      <c r="H24" s="164"/>
+      <c r="I24" s="164"/>
+      <c r="J24" s="165"/>
       <c r="K24" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="D2:K3"/>
+    <mergeCell ref="D5:K9"/>
+    <mergeCell ref="D11:K11"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="J10:K10"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="C24:J24"/>
     <mergeCell ref="C23:J23"/>
@@ -5841,13 +5845,6 @@
     <mergeCell ref="D17:K21"/>
     <mergeCell ref="C16:K16"/>
     <mergeCell ref="C15:K15"/>
-    <mergeCell ref="D2:K3"/>
-    <mergeCell ref="D5:K9"/>
-    <mergeCell ref="D11:K11"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="J10:K10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5859,10 +5856,10 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="L37" sqref="L37"/>
+      <selection pane="bottomLeft" activeCell="L59" sqref="L59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5878,10 +5875,10 @@
   <sheetData>
     <row r="1" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="18" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>381</v>
@@ -5908,7 +5905,7 @@
         <v>251</v>
       </c>
       <c r="K1" s="61" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="L1" s="61" t="s">
         <v>411</v>
@@ -5921,58 +5918,58 @@
       <c r="B2" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="C2" s="184" t="s">
+      <c r="C2" s="229" t="s">
         <v>162</v>
       </c>
-      <c r="D2" s="185"/>
-      <c r="E2" s="185"/>
-      <c r="F2" s="185"/>
-      <c r="G2" s="185"/>
-      <c r="H2" s="185"/>
-      <c r="I2" s="185"/>
-      <c r="J2" s="186"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="177"/>
+      <c r="D2" s="230"/>
+      <c r="E2" s="230"/>
+      <c r="F2" s="230"/>
+      <c r="G2" s="230"/>
+      <c r="H2" s="230"/>
+      <c r="I2" s="230"/>
+      <c r="J2" s="231"/>
+      <c r="K2" s="244"/>
+      <c r="L2" s="245"/>
     </row>
     <row r="3" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="164" t="s">
+      <c r="A3" s="161" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="172" t="s">
+      <c r="B3" s="169" t="s">
         <v>228</v>
       </c>
-      <c r="C3" s="169" t="s">
+      <c r="C3" s="166" t="s">
         <v>277</v>
       </c>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="170"/>
-      <c r="H3" s="170"/>
-      <c r="I3" s="170"/>
-      <c r="J3" s="170"/>
-      <c r="K3" s="170"/>
-      <c r="L3" s="171"/>
+      <c r="D3" s="167"/>
+      <c r="E3" s="167"/>
+      <c r="F3" s="167"/>
+      <c r="G3" s="167"/>
+      <c r="H3" s="167"/>
+      <c r="I3" s="167"/>
+      <c r="J3" s="167"/>
+      <c r="K3" s="167"/>
+      <c r="L3" s="168"/>
     </row>
     <row r="4" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A4" s="227"/>
-      <c r="B4" s="202"/>
-      <c r="C4" s="169" t="s">
-        <v>496</v>
-      </c>
-      <c r="D4" s="170"/>
-      <c r="E4" s="170"/>
-      <c r="F4" s="170"/>
-      <c r="G4" s="170"/>
-      <c r="H4" s="170"/>
-      <c r="I4" s="170"/>
-      <c r="J4" s="170"/>
-      <c r="K4" s="170"/>
-      <c r="L4" s="171"/>
+      <c r="A4" s="181"/>
+      <c r="B4" s="182"/>
+      <c r="C4" s="166" t="s">
+        <v>494</v>
+      </c>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
+      <c r="H4" s="167"/>
+      <c r="I4" s="167"/>
+      <c r="J4" s="167"/>
+      <c r="K4" s="167"/>
+      <c r="L4" s="168"/>
     </row>
     <row r="5" spans="1:12" s="16" customFormat="1" ht="180">
-      <c r="A5" s="165"/>
-      <c r="B5" s="173"/>
+      <c r="A5" s="162"/>
+      <c r="B5" s="170"/>
       <c r="C5" s="12" t="s">
         <v>160</v>
       </c>
@@ -6003,16 +6000,16 @@
       <c r="B6" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C6" s="169" t="s">
+      <c r="C6" s="166" t="s">
         <v>156</v>
       </c>
-      <c r="D6" s="170"/>
-      <c r="E6" s="170"/>
-      <c r="F6" s="170"/>
-      <c r="G6" s="170"/>
-      <c r="H6" s="170"/>
-      <c r="I6" s="170"/>
-      <c r="J6" s="171"/>
+      <c r="D6" s="167"/>
+      <c r="E6" s="167"/>
+      <c r="F6" s="167"/>
+      <c r="G6" s="167"/>
+      <c r="H6" s="167"/>
+      <c r="I6" s="167"/>
+      <c r="J6" s="168"/>
       <c r="K6" s="115"/>
       <c r="L6" s="87" t="s">
         <v>413</v>
@@ -6035,10 +6032,10 @@
       <c r="H7" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="I7" s="224"/>
-      <c r="J7" s="225"/>
+      <c r="I7" s="242"/>
+      <c r="J7" s="243"/>
       <c r="K7" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="L7" s="46" t="s">
         <v>414</v>
@@ -6051,16 +6048,16 @@
       <c r="B8" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C8" s="229" t="s">
+      <c r="C8" s="185" t="s">
         <v>151</v>
       </c>
-      <c r="D8" s="230"/>
-      <c r="E8" s="230"/>
-      <c r="F8" s="230"/>
-      <c r="G8" s="230"/>
-      <c r="H8" s="230"/>
-      <c r="I8" s="230"/>
-      <c r="J8" s="231"/>
+      <c r="D8" s="186"/>
+      <c r="E8" s="186"/>
+      <c r="F8" s="186"/>
+      <c r="G8" s="186"/>
+      <c r="H8" s="186"/>
+      <c r="I8" s="186"/>
+      <c r="J8" s="187"/>
       <c r="K8" s="115"/>
       <c r="L8" s="87" t="s">
         <v>151</v>
@@ -6073,7 +6070,7 @@
       <c r="B9" s="48" t="s">
         <v>226</v>
       </c>
-      <c r="C9" s="171" t="s">
+      <c r="C9" s="168" t="s">
         <v>149</v>
       </c>
       <c r="D9" s="183"/>
@@ -6093,16 +6090,16 @@
       <c r="B10" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="C10" s="229" t="s">
+      <c r="C10" s="185" t="s">
         <v>147</v>
       </c>
-      <c r="D10" s="230"/>
-      <c r="E10" s="230"/>
-      <c r="F10" s="230"/>
-      <c r="G10" s="230"/>
-      <c r="H10" s="230"/>
-      <c r="I10" s="230"/>
-      <c r="J10" s="231"/>
+      <c r="D10" s="186"/>
+      <c r="E10" s="186"/>
+      <c r="F10" s="186"/>
+      <c r="G10" s="186"/>
+      <c r="H10" s="186"/>
+      <c r="I10" s="186"/>
+      <c r="J10" s="187"/>
       <c r="K10" s="86"/>
       <c r="L10" s="87" t="s">
         <v>412</v>
@@ -6115,16 +6112,16 @@
       <c r="B11" s="48" t="s">
         <v>229</v>
       </c>
-      <c r="C11" s="169" t="s">
+      <c r="C11" s="166" t="s">
         <v>321</v>
       </c>
-      <c r="D11" s="170"/>
-      <c r="E11" s="170"/>
-      <c r="F11" s="170"/>
-      <c r="G11" s="170"/>
-      <c r="H11" s="171"/>
-      <c r="I11" s="161"/>
-      <c r="J11" s="219"/>
+      <c r="D11" s="167"/>
+      <c r="E11" s="167"/>
+      <c r="F11" s="167"/>
+      <c r="G11" s="167"/>
+      <c r="H11" s="168"/>
+      <c r="I11" s="190"/>
+      <c r="J11" s="191"/>
       <c r="K11" s="79" t="s">
         <v>317</v>
       </c>
@@ -6137,14 +6134,14 @@
         <v>322</v>
       </c>
       <c r="B12" s="76"/>
-      <c r="C12" s="232"/>
-      <c r="D12" s="233"/>
-      <c r="E12" s="233"/>
-      <c r="F12" s="233"/>
-      <c r="G12" s="233"/>
-      <c r="H12" s="233"/>
-      <c r="I12" s="162"/>
-      <c r="J12" s="175"/>
+      <c r="C12" s="194"/>
+      <c r="D12" s="195"/>
+      <c r="E12" s="195"/>
+      <c r="F12" s="195"/>
+      <c r="G12" s="195"/>
+      <c r="H12" s="195"/>
+      <c r="I12" s="172"/>
+      <c r="J12" s="173"/>
       <c r="K12" s="41" t="s">
         <v>323</v>
       </c>
@@ -6179,8 +6176,8 @@
       <c r="J13" s="42" t="s">
         <v>357</v>
       </c>
-      <c r="K13" s="187"/>
-      <c r="L13" s="188"/>
+      <c r="K13" s="232"/>
+      <c r="L13" s="233"/>
     </row>
     <row r="14" spans="1:12" ht="135">
       <c r="A14" s="13" t="s">
@@ -6192,19 +6189,19 @@
       <c r="C14" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="D14" s="174"/>
-      <c r="E14" s="159"/>
-      <c r="F14" s="162"/>
-      <c r="G14" s="162"/>
-      <c r="H14" s="162"/>
+      <c r="D14" s="171"/>
+      <c r="E14" s="176"/>
+      <c r="F14" s="172"/>
+      <c r="G14" s="172"/>
+      <c r="H14" s="172"/>
       <c r="I14" s="42" t="s">
         <v>351</v>
       </c>
       <c r="J14" s="42" t="s">
         <v>254</v>
       </c>
-      <c r="K14" s="189"/>
-      <c r="L14" s="190"/>
+      <c r="K14" s="234"/>
+      <c r="L14" s="235"/>
     </row>
     <row r="15" spans="1:12" ht="135">
       <c r="A15" s="13" t="s">
@@ -6237,21 +6234,21 @@
       <c r="J15" s="41" t="s">
         <v>214</v>
       </c>
-      <c r="K15" s="189"/>
-      <c r="L15" s="190"/>
+      <c r="K15" s="234"/>
+      <c r="L15" s="235"/>
     </row>
     <row r="16" spans="1:12" ht="150" customHeight="1">
-      <c r="A16" s="228" t="s">
+      <c r="A16" s="184" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="207" t="s">
+      <c r="B16" s="205" t="s">
         <v>137</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="D16" s="217"/>
-      <c r="E16" s="210"/>
+      <c r="D16" s="188"/>
+      <c r="E16" s="189"/>
       <c r="F16" s="28" t="s">
         <v>314</v>
       </c>
@@ -6265,37 +6262,37 @@
       <c r="J16" s="44" t="s">
         <v>216</v>
       </c>
-      <c r="K16" s="189"/>
-      <c r="L16" s="190"/>
+      <c r="K16" s="234"/>
+      <c r="L16" s="235"/>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1">
-      <c r="A17" s="228"/>
-      <c r="B17" s="207"/>
-      <c r="C17" s="169" t="s">
+      <c r="A17" s="184"/>
+      <c r="B17" s="205"/>
+      <c r="C17" s="166" t="s">
         <v>136</v>
       </c>
-      <c r="D17" s="170"/>
-      <c r="E17" s="170"/>
-      <c r="F17" s="170"/>
-      <c r="G17" s="170"/>
-      <c r="H17" s="212"/>
-      <c r="I17" s="212"/>
-      <c r="J17" s="195"/>
-      <c r="K17" s="189"/>
-      <c r="L17" s="190"/>
+      <c r="D17" s="167"/>
+      <c r="E17" s="167"/>
+      <c r="F17" s="167"/>
+      <c r="G17" s="167"/>
+      <c r="H17" s="192"/>
+      <c r="I17" s="192"/>
+      <c r="J17" s="193"/>
+      <c r="K17" s="234"/>
+      <c r="L17" s="235"/>
     </row>
     <row r="18" spans="1:12" ht="135" customHeight="1">
-      <c r="A18" s="228" t="s">
+      <c r="A18" s="184" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="207" t="s">
+      <c r="B18" s="205" t="s">
         <v>135</v>
       </c>
       <c r="C18" s="93" t="s">
         <v>312</v>
       </c>
-      <c r="D18" s="217"/>
-      <c r="E18" s="210"/>
+      <c r="D18" s="188"/>
+      <c r="E18" s="189"/>
       <c r="F18" s="94" t="s">
         <v>313</v>
       </c>
@@ -6309,24 +6306,24 @@
       <c r="J18" s="44" t="s">
         <v>217</v>
       </c>
-      <c r="K18" s="191"/>
-      <c r="L18" s="192"/>
+      <c r="K18" s="236"/>
+      <c r="L18" s="237"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1">
-      <c r="A19" s="228"/>
-      <c r="B19" s="216"/>
-      <c r="C19" s="193" t="s">
+      <c r="A19" s="184"/>
+      <c r="B19" s="212"/>
+      <c r="C19" s="238" t="s">
         <v>134</v>
       </c>
-      <c r="D19" s="170"/>
-      <c r="E19" s="170"/>
-      <c r="F19" s="170"/>
-      <c r="G19" s="170"/>
-      <c r="H19" s="170"/>
-      <c r="I19" s="170"/>
-      <c r="J19" s="170"/>
-      <c r="K19" s="170"/>
-      <c r="L19" s="171"/>
+      <c r="D19" s="167"/>
+      <c r="E19" s="167"/>
+      <c r="F19" s="167"/>
+      <c r="G19" s="167"/>
+      <c r="H19" s="167"/>
+      <c r="I19" s="167"/>
+      <c r="J19" s="167"/>
+      <c r="K19" s="167"/>
+      <c r="L19" s="168"/>
     </row>
     <row r="20" spans="1:12" ht="105" customHeight="1">
       <c r="A20" s="62" t="s">
@@ -6335,14 +6332,14 @@
       <c r="B20" s="63" t="s">
         <v>273</v>
       </c>
-      <c r="C20" s="208"/>
-      <c r="D20" s="209"/>
-      <c r="E20" s="209"/>
-      <c r="F20" s="209"/>
-      <c r="G20" s="209"/>
-      <c r="H20" s="209"/>
-      <c r="I20" s="209"/>
-      <c r="J20" s="210"/>
+      <c r="C20" s="206"/>
+      <c r="D20" s="207"/>
+      <c r="E20" s="207"/>
+      <c r="F20" s="207"/>
+      <c r="G20" s="207"/>
+      <c r="H20" s="207"/>
+      <c r="I20" s="207"/>
+      <c r="J20" s="189"/>
       <c r="K20" s="81" t="s">
         <v>271</v>
       </c>
@@ -6357,16 +6354,16 @@
       <c r="B21" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C21" s="169" t="s">
+      <c r="C21" s="166" t="s">
         <v>241</v>
       </c>
-      <c r="D21" s="170"/>
-      <c r="E21" s="170"/>
-      <c r="F21" s="170"/>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170"/>
-      <c r="J21" s="171"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="167"/>
+      <c r="F21" s="167"/>
+      <c r="G21" s="167"/>
+      <c r="H21" s="167"/>
+      <c r="I21" s="167"/>
+      <c r="J21" s="168"/>
       <c r="K21" s="43" t="s">
         <v>319</v>
       </c>
@@ -6375,60 +6372,60 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="90" customHeight="1">
-      <c r="A22" s="199" t="s">
+      <c r="A22" s="217" t="s">
         <v>396</v>
       </c>
-      <c r="B22" s="172" t="s">
+      <c r="B22" s="169" t="s">
         <v>401</v>
       </c>
-      <c r="C22" s="169" t="s">
+      <c r="C22" s="166" t="s">
         <v>398</v>
       </c>
-      <c r="D22" s="170"/>
-      <c r="E22" s="170"/>
-      <c r="F22" s="170"/>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170"/>
-      <c r="J22" s="171"/>
-      <c r="K22" s="195" t="s">
+      <c r="D22" s="167"/>
+      <c r="E22" s="167"/>
+      <c r="F22" s="167"/>
+      <c r="G22" s="167"/>
+      <c r="H22" s="167"/>
+      <c r="I22" s="167"/>
+      <c r="J22" s="168"/>
+      <c r="K22" s="193" t="s">
         <v>400</v>
       </c>
-      <c r="L22" s="195" t="s">
+      <c r="L22" s="193" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1">
-      <c r="A23" s="200"/>
-      <c r="B23" s="202"/>
-      <c r="C23" s="169" t="s">
+      <c r="A23" s="218"/>
+      <c r="B23" s="182"/>
+      <c r="C23" s="166" t="s">
         <v>397</v>
       </c>
-      <c r="D23" s="170"/>
-      <c r="E23" s="170"/>
-      <c r="F23" s="170"/>
-      <c r="G23" s="170"/>
-      <c r="H23" s="170"/>
-      <c r="I23" s="170"/>
-      <c r="J23" s="171"/>
-      <c r="K23" s="196"/>
-      <c r="L23" s="196"/>
+      <c r="D23" s="167"/>
+      <c r="E23" s="167"/>
+      <c r="F23" s="167"/>
+      <c r="G23" s="167"/>
+      <c r="H23" s="167"/>
+      <c r="I23" s="167"/>
+      <c r="J23" s="168"/>
+      <c r="K23" s="220"/>
+      <c r="L23" s="220"/>
     </row>
     <row r="24" spans="1:12" ht="45" customHeight="1">
-      <c r="A24" s="201"/>
-      <c r="B24" s="173"/>
-      <c r="C24" s="169" t="s">
+      <c r="A24" s="219"/>
+      <c r="B24" s="170"/>
+      <c r="C24" s="166" t="s">
         <v>399</v>
       </c>
-      <c r="D24" s="170"/>
-      <c r="E24" s="170"/>
-      <c r="F24" s="170"/>
-      <c r="G24" s="170"/>
-      <c r="H24" s="170"/>
-      <c r="I24" s="170"/>
-      <c r="J24" s="171"/>
-      <c r="K24" s="180"/>
-      <c r="L24" s="180"/>
+      <c r="D24" s="167"/>
+      <c r="E24" s="167"/>
+      <c r="F24" s="167"/>
+      <c r="G24" s="167"/>
+      <c r="H24" s="167"/>
+      <c r="I24" s="167"/>
+      <c r="J24" s="168"/>
+      <c r="K24" s="209"/>
+      <c r="L24" s="209"/>
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="13" t="s">
@@ -6437,18 +6434,18 @@
       <c r="B25" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="C25" s="194" t="s">
+      <c r="C25" s="223" t="s">
         <v>129</v>
       </c>
-      <c r="D25" s="182"/>
-      <c r="E25" s="182"/>
-      <c r="F25" s="182"/>
-      <c r="G25" s="182"/>
-      <c r="H25" s="182"/>
-      <c r="I25" s="182"/>
-      <c r="J25" s="182"/>
-      <c r="K25" s="182"/>
-      <c r="L25" s="182"/>
+      <c r="D25" s="228"/>
+      <c r="E25" s="228"/>
+      <c r="F25" s="228"/>
+      <c r="G25" s="228"/>
+      <c r="H25" s="228"/>
+      <c r="I25" s="228"/>
+      <c r="J25" s="228"/>
+      <c r="K25" s="228"/>
+      <c r="L25" s="228"/>
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1">
       <c r="A26" s="10" t="s">
@@ -6457,18 +6454,18 @@
       <c r="B26" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="C26" s="194" t="s">
+      <c r="C26" s="223" t="s">
         <v>126</v>
       </c>
-      <c r="D26" s="182"/>
-      <c r="E26" s="182"/>
-      <c r="F26" s="182"/>
-      <c r="G26" s="182"/>
-      <c r="H26" s="182"/>
-      <c r="I26" s="182"/>
-      <c r="J26" s="182"/>
-      <c r="K26" s="182"/>
-      <c r="L26" s="182"/>
+      <c r="D26" s="228"/>
+      <c r="E26" s="228"/>
+      <c r="F26" s="228"/>
+      <c r="G26" s="228"/>
+      <c r="H26" s="228"/>
+      <c r="I26" s="228"/>
+      <c r="J26" s="228"/>
+      <c r="K26" s="228"/>
+      <c r="L26" s="228"/>
     </row>
     <row r="27" spans="1:12" ht="30" customHeight="1">
       <c r="A27" s="10" t="s">
@@ -6477,18 +6474,18 @@
       <c r="B27" s="103" t="s">
         <v>177</v>
       </c>
-      <c r="C27" s="194" t="s">
+      <c r="C27" s="223" t="s">
         <v>178</v>
       </c>
-      <c r="D27" s="182"/>
-      <c r="E27" s="182"/>
-      <c r="F27" s="182"/>
-      <c r="G27" s="182"/>
-      <c r="H27" s="182"/>
-      <c r="I27" s="182"/>
-      <c r="J27" s="182"/>
-      <c r="K27" s="182"/>
-      <c r="L27" s="182"/>
+      <c r="D27" s="228"/>
+      <c r="E27" s="228"/>
+      <c r="F27" s="228"/>
+      <c r="G27" s="228"/>
+      <c r="H27" s="228"/>
+      <c r="I27" s="228"/>
+      <c r="J27" s="228"/>
+      <c r="K27" s="228"/>
+      <c r="L27" s="228"/>
     </row>
     <row r="28" spans="1:12" ht="30" customHeight="1">
       <c r="A28" s="10" t="s">
@@ -6497,18 +6494,18 @@
       <c r="B28" s="103" t="s">
         <v>124</v>
       </c>
-      <c r="C28" s="194" t="s">
+      <c r="C28" s="223" t="s">
         <v>123</v>
       </c>
-      <c r="D28" s="182"/>
-      <c r="E28" s="182"/>
-      <c r="F28" s="182"/>
-      <c r="G28" s="182"/>
-      <c r="H28" s="182"/>
-      <c r="I28" s="182"/>
-      <c r="J28" s="182"/>
-      <c r="K28" s="182"/>
-      <c r="L28" s="182"/>
+      <c r="D28" s="228"/>
+      <c r="E28" s="228"/>
+      <c r="F28" s="228"/>
+      <c r="G28" s="228"/>
+      <c r="H28" s="228"/>
+      <c r="I28" s="228"/>
+      <c r="J28" s="228"/>
+      <c r="K28" s="228"/>
+      <c r="L28" s="228"/>
     </row>
     <row r="29" spans="1:12" ht="30" customHeight="1">
       <c r="A29" s="10" t="s">
@@ -6517,18 +6514,18 @@
       <c r="B29" s="103" t="s">
         <v>180</v>
       </c>
-      <c r="C29" s="194" t="s">
+      <c r="C29" s="223" t="s">
         <v>181</v>
       </c>
-      <c r="D29" s="182"/>
-      <c r="E29" s="182"/>
-      <c r="F29" s="182"/>
-      <c r="G29" s="182"/>
-      <c r="H29" s="182"/>
-      <c r="I29" s="182"/>
-      <c r="J29" s="182"/>
-      <c r="K29" s="182"/>
-      <c r="L29" s="182"/>
+      <c r="D29" s="228"/>
+      <c r="E29" s="228"/>
+      <c r="F29" s="228"/>
+      <c r="G29" s="228"/>
+      <c r="H29" s="228"/>
+      <c r="I29" s="228"/>
+      <c r="J29" s="228"/>
+      <c r="K29" s="228"/>
+      <c r="L29" s="228"/>
     </row>
     <row r="30" spans="1:12" ht="30" customHeight="1">
       <c r="A30" s="10" t="s">
@@ -6537,18 +6534,18 @@
       <c r="B30" s="103" t="s">
         <v>121</v>
       </c>
-      <c r="C30" s="194" t="s">
+      <c r="C30" s="223" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="182"/>
-      <c r="E30" s="182"/>
-      <c r="F30" s="182"/>
-      <c r="G30" s="182"/>
-      <c r="H30" s="182"/>
-      <c r="I30" s="182"/>
-      <c r="J30" s="182"/>
-      <c r="K30" s="182"/>
-      <c r="L30" s="182"/>
+      <c r="D30" s="228"/>
+      <c r="E30" s="228"/>
+      <c r="F30" s="228"/>
+      <c r="G30" s="228"/>
+      <c r="H30" s="228"/>
+      <c r="I30" s="228"/>
+      <c r="J30" s="228"/>
+      <c r="K30" s="228"/>
+      <c r="L30" s="228"/>
     </row>
     <row r="31" spans="1:12" ht="30" customHeight="1">
       <c r="A31" s="10" t="s">
@@ -6557,83 +6554,83 @@
       <c r="B31" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="C31" s="194" t="s">
+      <c r="C31" s="223" t="s">
         <v>117</v>
       </c>
-      <c r="D31" s="182"/>
-      <c r="E31" s="182"/>
-      <c r="F31" s="182"/>
-      <c r="G31" s="182"/>
-      <c r="H31" s="182"/>
-      <c r="I31" s="182"/>
-      <c r="J31" s="182"/>
-      <c r="K31" s="182"/>
-      <c r="L31" s="182"/>
+      <c r="D31" s="228"/>
+      <c r="E31" s="228"/>
+      <c r="F31" s="228"/>
+      <c r="G31" s="228"/>
+      <c r="H31" s="228"/>
+      <c r="I31" s="228"/>
+      <c r="J31" s="228"/>
+      <c r="K31" s="228"/>
+      <c r="L31" s="228"/>
     </row>
     <row r="32" spans="1:12" ht="75" customHeight="1">
-      <c r="A32" s="272" t="s">
+      <c r="A32" s="155" t="s">
         <v>116</v>
       </c>
-      <c r="B32" s="273" t="s">
+      <c r="B32" s="156" t="s">
         <v>115</v>
       </c>
       <c r="C32" s="133" t="s">
         <v>183</v>
       </c>
-      <c r="D32" s="274"/>
-      <c r="E32" s="275" t="s">
+      <c r="D32" s="157"/>
+      <c r="E32" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="F32" s="276" t="s">
+      <c r="F32" s="159" t="s">
         <v>184</v>
       </c>
-      <c r="G32" s="239"/>
-      <c r="H32" s="240"/>
-      <c r="I32" s="275" t="s">
+      <c r="G32" s="215"/>
+      <c r="H32" s="216"/>
+      <c r="I32" s="158" t="s">
         <v>332</v>
       </c>
-      <c r="J32" s="275" t="s">
+      <c r="J32" s="158" t="s">
         <v>255</v>
       </c>
-      <c r="K32" s="277" t="s">
+      <c r="K32" s="160" t="s">
         <v>215</v>
       </c>
-      <c r="L32" s="277" t="s">
+      <c r="L32" s="160" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="33" spans="1:13" s="70" customFormat="1" ht="15" customHeight="1">
-      <c r="A33" s="226" t="s">
+      <c r="A33" s="196" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="268" t="s">
+      <c r="B33" s="197" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="269" t="s">
+      <c r="C33" s="239" t="s">
         <v>410</v>
       </c>
-      <c r="D33" s="270"/>
-      <c r="E33" s="270"/>
-      <c r="F33" s="270"/>
-      <c r="G33" s="270"/>
-      <c r="H33" s="270"/>
-      <c r="I33" s="270"/>
-      <c r="J33" s="270"/>
-      <c r="K33" s="270"/>
-      <c r="L33" s="271"/>
+      <c r="D33" s="240"/>
+      <c r="E33" s="240"/>
+      <c r="F33" s="240"/>
+      <c r="G33" s="240"/>
+      <c r="H33" s="240"/>
+      <c r="I33" s="240"/>
+      <c r="J33" s="240"/>
+      <c r="K33" s="240"/>
+      <c r="L33" s="241"/>
     </row>
     <row r="34" spans="1:13" ht="345" customHeight="1">
-      <c r="A34" s="226"/>
-      <c r="B34" s="202"/>
+      <c r="A34" s="196"/>
+      <c r="B34" s="182"/>
       <c r="C34" s="116" t="s">
         <v>233</v>
       </c>
       <c r="D34" s="101" t="s">
         <v>409</v>
       </c>
-      <c r="E34" s="158"/>
-      <c r="F34" s="159"/>
-      <c r="G34" s="160"/>
+      <c r="E34" s="175"/>
+      <c r="F34" s="176"/>
+      <c r="G34" s="174"/>
       <c r="H34" s="117" t="s">
         <v>234</v>
       </c>
@@ -6655,20 +6652,20 @@
         <v>113</v>
       </c>
       <c r="B35" s="132" t="s">
-        <v>517</v>
-      </c>
-      <c r="C35" s="178" t="s">
+        <v>515</v>
+      </c>
+      <c r="C35" s="204" t="s">
         <v>112</v>
       </c>
-      <c r="D35" s="179"/>
-      <c r="E35" s="179"/>
-      <c r="F35" s="179"/>
-      <c r="G35" s="179"/>
-      <c r="H35" s="179"/>
-      <c r="I35" s="179"/>
-      <c r="J35" s="179"/>
-      <c r="K35" s="179"/>
-      <c r="L35" s="180"/>
+      <c r="D35" s="208"/>
+      <c r="E35" s="208"/>
+      <c r="F35" s="208"/>
+      <c r="G35" s="208"/>
+      <c r="H35" s="208"/>
+      <c r="I35" s="208"/>
+      <c r="J35" s="208"/>
+      <c r="K35" s="208"/>
+      <c r="L35" s="209"/>
     </row>
     <row r="36" spans="1:13" ht="45" customHeight="1">
       <c r="A36" s="131" t="s">
@@ -6677,41 +6674,41 @@
       <c r="B36" s="132" t="s">
         <v>110</v>
       </c>
-      <c r="C36" s="211" t="s">
-        <v>469</v>
-      </c>
-      <c r="D36" s="212"/>
-      <c r="E36" s="212"/>
-      <c r="F36" s="212"/>
-      <c r="G36" s="212"/>
-      <c r="H36" s="212"/>
-      <c r="I36" s="212"/>
-      <c r="J36" s="212"/>
-      <c r="K36" s="212"/>
-      <c r="L36" s="195"/>
+      <c r="C36" s="203" t="s">
+        <v>467</v>
+      </c>
+      <c r="D36" s="192"/>
+      <c r="E36" s="192"/>
+      <c r="F36" s="192"/>
+      <c r="G36" s="192"/>
+      <c r="H36" s="192"/>
+      <c r="I36" s="192"/>
+      <c r="J36" s="192"/>
+      <c r="K36" s="192"/>
+      <c r="L36" s="193"/>
     </row>
     <row r="37" spans="1:13" ht="60" customHeight="1">
       <c r="A37" s="129" t="s">
+        <v>520</v>
+      </c>
+      <c r="B37" s="130" t="s">
+        <v>521</v>
+      </c>
+      <c r="C37" s="166" t="s">
+        <v>466</v>
+      </c>
+      <c r="D37" s="167"/>
+      <c r="E37" s="167"/>
+      <c r="F37" s="167"/>
+      <c r="G37" s="167"/>
+      <c r="H37" s="167"/>
+      <c r="I37" s="167"/>
+      <c r="J37" s="168"/>
+      <c r="K37" s="124" t="s">
+        <v>468</v>
+      </c>
+      <c r="L37" s="124" t="s">
         <v>522</v>
-      </c>
-      <c r="B37" s="130" t="s">
-        <v>523</v>
-      </c>
-      <c r="C37" s="169" t="s">
-        <v>468</v>
-      </c>
-      <c r="D37" s="170"/>
-      <c r="E37" s="170"/>
-      <c r="F37" s="170"/>
-      <c r="G37" s="170"/>
-      <c r="H37" s="170"/>
-      <c r="I37" s="170"/>
-      <c r="J37" s="171"/>
-      <c r="K37" s="124" t="s">
-        <v>470</v>
-      </c>
-      <c r="L37" s="124" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="105" customHeight="1">
@@ -6724,20 +6721,20 @@
       <c r="C38" s="37" t="s">
         <v>353</v>
       </c>
-      <c r="D38" s="217"/>
-      <c r="E38" s="210"/>
+      <c r="D38" s="188"/>
+      <c r="E38" s="189"/>
       <c r="F38" s="29" t="s">
         <v>107</v>
       </c>
       <c r="G38" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="H38" s="206"/>
+      <c r="H38" s="213"/>
       <c r="I38" s="82" t="s">
         <v>352</v>
       </c>
-      <c r="J38" s="213"/>
-      <c r="K38" s="214"/>
+      <c r="J38" s="210"/>
+      <c r="K38" s="211"/>
       <c r="L38" s="105" t="s">
         <v>419</v>
       </c>
@@ -6764,15 +6761,15 @@
       <c r="G39" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="H39" s="205"/>
+      <c r="H39" s="214"/>
       <c r="I39" s="85" t="s">
         <v>335</v>
       </c>
       <c r="J39" s="43" t="s">
         <v>219</v>
       </c>
-      <c r="K39" s="215"/>
-      <c r="L39" s="215"/>
+      <c r="K39" s="225"/>
+      <c r="L39" s="225"/>
     </row>
     <row r="40" spans="1:13" ht="60" customHeight="1">
       <c r="A40" s="22" t="s">
@@ -6781,16 +6778,16 @@
       <c r="B40" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="C40" s="197" t="s">
+      <c r="C40" s="222" t="s">
         <v>193</v>
       </c>
-      <c r="D40" s="198"/>
-      <c r="E40" s="198"/>
-      <c r="F40" s="198"/>
-      <c r="G40" s="198"/>
-      <c r="H40" s="194"/>
-      <c r="I40" s="218"/>
-      <c r="J40" s="219"/>
+      <c r="D40" s="202"/>
+      <c r="E40" s="202"/>
+      <c r="F40" s="202"/>
+      <c r="G40" s="202"/>
+      <c r="H40" s="223"/>
+      <c r="I40" s="226"/>
+      <c r="J40" s="191"/>
       <c r="K40" s="79" t="s">
         <v>220</v>
       </c>
@@ -6805,16 +6802,16 @@
       <c r="B41" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="C41" s="197" t="s">
+      <c r="C41" s="222" t="s">
         <v>224</v>
       </c>
-      <c r="D41" s="198"/>
-      <c r="E41" s="198"/>
-      <c r="F41" s="198"/>
-      <c r="G41" s="198"/>
-      <c r="H41" s="194"/>
-      <c r="I41" s="158"/>
-      <c r="J41" s="160"/>
+      <c r="D41" s="202"/>
+      <c r="E41" s="202"/>
+      <c r="F41" s="202"/>
+      <c r="G41" s="202"/>
+      <c r="H41" s="223"/>
+      <c r="I41" s="175"/>
+      <c r="J41" s="174"/>
       <c r="K41" s="79" t="s">
         <v>223</v>
       </c>
@@ -6829,14 +6826,14 @@
       <c r="B42" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="C42" s="198" t="s">
+      <c r="C42" s="202" t="s">
         <v>190</v>
       </c>
-      <c r="D42" s="198"/>
-      <c r="E42" s="198"/>
-      <c r="F42" s="198"/>
-      <c r="G42" s="198"/>
-      <c r="H42" s="198"/>
+      <c r="D42" s="202"/>
+      <c r="E42" s="202"/>
+      <c r="F42" s="202"/>
+      <c r="G42" s="202"/>
+      <c r="H42" s="202"/>
       <c r="I42" s="44" t="s">
         <v>331</v>
       </c>
@@ -6862,7 +6859,7 @@
         <v>367</v>
       </c>
       <c r="E43" s="32" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F43" s="32" t="s">
         <v>431</v>
@@ -6873,13 +6870,13 @@
       <c r="H43" s="81" t="s">
         <v>430</v>
       </c>
-      <c r="I43" s="158"/>
-      <c r="J43" s="160"/>
+      <c r="I43" s="175"/>
+      <c r="J43" s="174"/>
       <c r="K43" s="42" t="s">
         <v>240</v>
       </c>
       <c r="L43" s="42" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="285">
@@ -6902,14 +6899,14 @@
       <c r="G44" s="19" t="s">
         <v>429</v>
       </c>
-      <c r="H44" s="158"/>
-      <c r="I44" s="159"/>
-      <c r="J44" s="160"/>
+      <c r="H44" s="175"/>
+      <c r="I44" s="176"/>
+      <c r="J44" s="174"/>
       <c r="K44" s="42" t="s">
         <v>426</v>
       </c>
       <c r="L44" s="42" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="240">
@@ -6919,15 +6916,15 @@
       <c r="B45" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C45" s="203"/>
-      <c r="D45" s="159"/>
+      <c r="C45" s="221"/>
+      <c r="D45" s="176"/>
       <c r="E45" s="44" t="s">
         <v>236</v>
       </c>
-      <c r="F45" s="158"/>
-      <c r="G45" s="159"/>
-      <c r="H45" s="159"/>
-      <c r="I45" s="160"/>
+      <c r="F45" s="175"/>
+      <c r="G45" s="176"/>
+      <c r="H45" s="176"/>
+      <c r="I45" s="174"/>
       <c r="J45" s="42" t="s">
         <v>235</v>
       </c>
@@ -6946,10 +6943,10 @@
       <c r="C46" s="35" t="s">
         <v>328</v>
       </c>
-      <c r="D46" s="174"/>
-      <c r="E46" s="162"/>
-      <c r="F46" s="162"/>
-      <c r="G46" s="175"/>
+      <c r="D46" s="171"/>
+      <c r="E46" s="172"/>
+      <c r="F46" s="172"/>
+      <c r="G46" s="173"/>
       <c r="H46" s="19" t="s">
         <v>182</v>
       </c>
@@ -6963,29 +6960,29 @@
         <v>257</v>
       </c>
       <c r="L46" s="104" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="M46" s="7"/>
     </row>
     <row r="47" spans="1:13" ht="210" customHeight="1">
-      <c r="A47" s="221" t="s">
+      <c r="A47" s="198" t="s">
         <v>87</v>
       </c>
-      <c r="B47" s="223" t="s">
+      <c r="B47" s="200" t="s">
         <v>86</v>
       </c>
-      <c r="C47" s="197" t="s">
+      <c r="C47" s="222" t="s">
         <v>327</v>
       </c>
-      <c r="D47" s="198"/>
+      <c r="D47" s="202"/>
       <c r="E47" s="44" t="s">
         <v>329</v>
       </c>
-      <c r="F47" s="198" t="s">
+      <c r="F47" s="202" t="s">
         <v>326</v>
       </c>
-      <c r="G47" s="198"/>
-      <c r="H47" s="194"/>
+      <c r="G47" s="202"/>
+      <c r="H47" s="223"/>
       <c r="I47" s="42" t="s">
         <v>333</v>
       </c>
@@ -6998,44 +6995,44 @@
       <c r="L47" s="11"/>
     </row>
     <row r="48" spans="1:13" ht="15" customHeight="1">
-      <c r="A48" s="222"/>
-      <c r="B48" s="220"/>
-      <c r="C48" s="169" t="s">
+      <c r="A48" s="199"/>
+      <c r="B48" s="201"/>
+      <c r="C48" s="166" t="s">
         <v>85</v>
       </c>
-      <c r="D48" s="170"/>
-      <c r="E48" s="170"/>
-      <c r="F48" s="170"/>
-      <c r="G48" s="170"/>
-      <c r="H48" s="170"/>
-      <c r="I48" s="170"/>
-      <c r="J48" s="170"/>
-      <c r="K48" s="170"/>
-      <c r="L48" s="171"/>
+      <c r="D48" s="167"/>
+      <c r="E48" s="167"/>
+      <c r="F48" s="167"/>
+      <c r="G48" s="167"/>
+      <c r="H48" s="167"/>
+      <c r="I48" s="167"/>
+      <c r="J48" s="167"/>
+      <c r="K48" s="167"/>
+      <c r="L48" s="168"/>
     </row>
     <row r="49" spans="1:12" ht="15" customHeight="1">
-      <c r="A49" s="221" t="s">
+      <c r="A49" s="198" t="s">
         <v>194</v>
       </c>
-      <c r="B49" s="223" t="s">
+      <c r="B49" s="200" t="s">
         <v>202</v>
       </c>
-      <c r="C49" s="178" t="s">
+      <c r="C49" s="204" t="s">
         <v>196</v>
       </c>
-      <c r="D49" s="179"/>
-      <c r="E49" s="179"/>
-      <c r="F49" s="179"/>
-      <c r="G49" s="179"/>
-      <c r="H49" s="179"/>
-      <c r="I49" s="179"/>
-      <c r="J49" s="179"/>
-      <c r="K49" s="179"/>
-      <c r="L49" s="180"/>
+      <c r="D49" s="208"/>
+      <c r="E49" s="208"/>
+      <c r="F49" s="208"/>
+      <c r="G49" s="208"/>
+      <c r="H49" s="208"/>
+      <c r="I49" s="208"/>
+      <c r="J49" s="208"/>
+      <c r="K49" s="208"/>
+      <c r="L49" s="209"/>
     </row>
     <row r="50" spans="1:12" ht="285" customHeight="1">
-      <c r="A50" s="222"/>
-      <c r="B50" s="178"/>
+      <c r="A50" s="199"/>
+      <c r="B50" s="204"/>
       <c r="C50" s="37" t="s">
         <v>197</v>
       </c>
@@ -7057,12 +7054,12 @@
       <c r="I50" s="44" t="s">
         <v>337</v>
       </c>
-      <c r="J50" s="206"/>
+      <c r="J50" s="213"/>
       <c r="K50" s="42" t="s">
         <v>232</v>
       </c>
       <c r="L50" s="42" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="352.5" customHeight="1">
@@ -7093,12 +7090,12 @@
       <c r="I51" s="44" t="s">
         <v>339</v>
       </c>
-      <c r="J51" s="205"/>
+      <c r="J51" s="214"/>
       <c r="K51" s="42" t="s">
         <v>338</v>
       </c>
       <c r="L51" s="42" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="135" customHeight="1">
@@ -7115,7 +7112,7 @@
         <v>81</v>
       </c>
       <c r="E52" s="32" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F52" s="32" t="s">
         <v>80</v>
@@ -7138,28 +7135,28 @@
       </c>
     </row>
     <row r="53" spans="1:12" ht="30" customHeight="1">
-      <c r="A53" s="221" t="s">
+      <c r="A53" s="198" t="s">
         <v>78</v>
       </c>
-      <c r="B53" s="211" t="s">
+      <c r="B53" s="203" t="s">
         <v>77</v>
       </c>
-      <c r="C53" s="181" t="s">
-        <v>441</v>
-      </c>
-      <c r="D53" s="182"/>
-      <c r="E53" s="182"/>
-      <c r="F53" s="182"/>
-      <c r="G53" s="182"/>
-      <c r="H53" s="182"/>
-      <c r="I53" s="182"/>
-      <c r="J53" s="182"/>
-      <c r="K53" s="182"/>
-      <c r="L53" s="182"/>
+      <c r="C53" s="227" t="s">
+        <v>439</v>
+      </c>
+      <c r="D53" s="228"/>
+      <c r="E53" s="228"/>
+      <c r="F53" s="228"/>
+      <c r="G53" s="228"/>
+      <c r="H53" s="228"/>
+      <c r="I53" s="228"/>
+      <c r="J53" s="228"/>
+      <c r="K53" s="228"/>
+      <c r="L53" s="228"/>
     </row>
     <row r="54" spans="1:12" ht="195" customHeight="1">
-      <c r="A54" s="222"/>
-      <c r="B54" s="220"/>
+      <c r="A54" s="199"/>
+      <c r="B54" s="201"/>
       <c r="C54" s="116" t="s">
         <v>245</v>
       </c>
@@ -7188,34 +7185,34 @@
       </c>
     </row>
     <row r="55" spans="1:12" ht="30" customHeight="1">
-      <c r="A55" s="221" t="s">
+      <c r="A55" s="198" t="s">
         <v>76</v>
       </c>
-      <c r="B55" s="211" t="s">
+      <c r="B55" s="203" t="s">
         <v>75</v>
       </c>
-      <c r="C55" s="181" t="s">
-        <v>442</v>
-      </c>
-      <c r="D55" s="182"/>
-      <c r="E55" s="182"/>
-      <c r="F55" s="182"/>
-      <c r="G55" s="182"/>
-      <c r="H55" s="182"/>
-      <c r="I55" s="182"/>
-      <c r="J55" s="182"/>
-      <c r="K55" s="182"/>
-      <c r="L55" s="182"/>
+      <c r="C55" s="227" t="s">
+        <v>440</v>
+      </c>
+      <c r="D55" s="228"/>
+      <c r="E55" s="228"/>
+      <c r="F55" s="228"/>
+      <c r="G55" s="228"/>
+      <c r="H55" s="228"/>
+      <c r="I55" s="228"/>
+      <c r="J55" s="228"/>
+      <c r="K55" s="228"/>
+      <c r="L55" s="228"/>
     </row>
     <row r="56" spans="1:12" ht="326.25" customHeight="1">
-      <c r="A56" s="222"/>
-      <c r="B56" s="220"/>
+      <c r="A56" s="199"/>
+      <c r="B56" s="201"/>
       <c r="C56" s="122" t="s">
         <v>74</v>
       </c>
       <c r="D56" s="14"/>
       <c r="E56" s="142" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="F56" s="142" t="s">
         <v>73</v>
@@ -7230,7 +7227,7 @@
         <v>242</v>
       </c>
       <c r="L56" s="99" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="195" customHeight="1">
@@ -7258,7 +7255,7 @@
       <c r="H57" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="I57" s="204"/>
+      <c r="I57" s="224"/>
       <c r="J57" s="42" t="s">
         <v>262</v>
       </c>
@@ -7266,7 +7263,7 @@
         <v>261</v>
       </c>
       <c r="L57" s="42" t="s">
-        <v>435</v>
+        <v>528</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="105" customHeight="1">
@@ -7294,7 +7291,7 @@
       <c r="H58" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="I58" s="205"/>
+      <c r="I58" s="214"/>
       <c r="J58" s="42" t="s">
         <v>264</v>
       </c>
@@ -7321,21 +7318,19 @@
       <c r="E59" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="F59" s="174"/>
-      <c r="G59" s="175"/>
+      <c r="F59" s="171"/>
+      <c r="G59" s="173"/>
       <c r="H59" s="25" t="s">
         <v>185</v>
       </c>
       <c r="I59" s="80" t="s">
         <v>341</v>
       </c>
-      <c r="J59" s="206"/>
+      <c r="J59" s="213"/>
       <c r="K59" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="L59" s="106" t="s">
-        <v>436</v>
-      </c>
+      <c r="L59" s="106"/>
     </row>
     <row r="60" spans="1:12" ht="405" customHeight="1">
       <c r="A60" s="22" t="s">
@@ -7365,16 +7360,81 @@
       <c r="I60" s="44" t="s">
         <v>349</v>
       </c>
-      <c r="J60" s="205"/>
+      <c r="J60" s="214"/>
       <c r="K60" s="42" t="s">
         <v>266</v>
       </c>
       <c r="L60" s="42" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="81">
+    <mergeCell ref="C3:L3"/>
+    <mergeCell ref="C9:L9"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="K13:L18"/>
+    <mergeCell ref="C19:L19"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="C4:L4"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="J59:J60"/>
+    <mergeCell ref="J50:J51"/>
+    <mergeCell ref="C41:H41"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="I40:J41"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C55:L55"/>
+    <mergeCell ref="C48:L48"/>
+    <mergeCell ref="C49:L49"/>
+    <mergeCell ref="C53:L53"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="I57:I58"/>
+    <mergeCell ref="C20:J20"/>
+    <mergeCell ref="C35:L35"/>
+    <mergeCell ref="C36:L36"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="C37:J37"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C24:J24"/>
+    <mergeCell ref="K22:K24"/>
+    <mergeCell ref="C25:L25"/>
+    <mergeCell ref="C26:L26"/>
+    <mergeCell ref="C27:L27"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="C42:H42"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="C21:J21"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="C23:J23"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="C28:L28"/>
+    <mergeCell ref="C29:L29"/>
+    <mergeCell ref="C30:L30"/>
+    <mergeCell ref="L22:L24"/>
+    <mergeCell ref="C31:L31"/>
+    <mergeCell ref="C33:L33"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="D5:G5"/>
@@ -7390,72 +7450,7 @@
     <mergeCell ref="I11:J12"/>
     <mergeCell ref="C17:J17"/>
     <mergeCell ref="C12:H12"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="C21:J21"/>
-    <mergeCell ref="C22:J22"/>
-    <mergeCell ref="C23:J23"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="C42:H42"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B53:B54"/>
     <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C20:J20"/>
-    <mergeCell ref="C35:L35"/>
-    <mergeCell ref="C36:L36"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="C37:J37"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="C24:J24"/>
-    <mergeCell ref="K22:K24"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="I57:I58"/>
-    <mergeCell ref="J59:J60"/>
-    <mergeCell ref="J50:J51"/>
-    <mergeCell ref="C41:H41"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="I40:J41"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C55:L55"/>
-    <mergeCell ref="C3:L3"/>
-    <mergeCell ref="C9:L9"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="K13:L18"/>
-    <mergeCell ref="C19:L19"/>
-    <mergeCell ref="C25:L25"/>
-    <mergeCell ref="C26:L26"/>
-    <mergeCell ref="C27:L27"/>
-    <mergeCell ref="C28:L28"/>
-    <mergeCell ref="C29:L29"/>
-    <mergeCell ref="C30:L30"/>
-    <mergeCell ref="L22:L24"/>
-    <mergeCell ref="C31:L31"/>
-    <mergeCell ref="C33:L33"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="C4:L4"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="C48:L48"/>
-    <mergeCell ref="C49:L49"/>
-    <mergeCell ref="C53:L53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7467,7 +7462,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:XFB56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
@@ -7486,13 +7481,13 @@
   <sheetData>
     <row r="1" spans="1:14" s="16" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="59" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B1" s="60" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C1" s="144" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D1" s="60" t="s">
         <v>381</v>
@@ -7526,51 +7521,51 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="247" t="s">
+      <c r="A2" s="272" t="s">
         <v>402</v>
       </c>
-      <c r="B2" s="245" t="s">
+      <c r="B2" s="270" t="s">
         <v>403</v>
       </c>
       <c r="C2" s="145">
         <v>1</v>
       </c>
-      <c r="D2" s="251" t="s">
+      <c r="D2" s="266" t="s">
         <v>404</v>
       </c>
-      <c r="E2" s="251"/>
-      <c r="F2" s="251"/>
-      <c r="G2" s="251"/>
-      <c r="H2" s="251"/>
-      <c r="I2" s="251"/>
-      <c r="J2" s="251"/>
-      <c r="K2" s="251"/>
-      <c r="L2" s="251"/>
-      <c r="M2" s="252"/>
+      <c r="E2" s="266"/>
+      <c r="F2" s="266"/>
+      <c r="G2" s="266"/>
+      <c r="H2" s="266"/>
+      <c r="I2" s="266"/>
+      <c r="J2" s="266"/>
+      <c r="K2" s="266"/>
+      <c r="L2" s="266"/>
+      <c r="M2" s="267"/>
     </row>
     <row r="3" spans="1:14" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="227"/>
-      <c r="B3" s="243"/>
+      <c r="A3" s="181"/>
+      <c r="B3" s="261"/>
       <c r="C3" s="146">
         <v>2</v>
       </c>
-      <c r="D3" s="253" t="s">
-        <v>506</v>
-      </c>
-      <c r="E3" s="253"/>
-      <c r="F3" s="253"/>
-      <c r="G3" s="253"/>
-      <c r="H3" s="253"/>
-      <c r="I3" s="253"/>
-      <c r="J3" s="253"/>
-      <c r="K3" s="253"/>
-      <c r="L3" s="253"/>
-      <c r="M3" s="253"/>
+      <c r="D3" s="268" t="s">
+        <v>504</v>
+      </c>
+      <c r="E3" s="268"/>
+      <c r="F3" s="268"/>
+      <c r="G3" s="268"/>
+      <c r="H3" s="268"/>
+      <c r="I3" s="268"/>
+      <c r="J3" s="268"/>
+      <c r="K3" s="268"/>
+      <c r="L3" s="268"/>
+      <c r="M3" s="268"/>
       <c r="N3" s="88"/>
     </row>
     <row r="4" spans="1:14" s="16" customFormat="1" ht="120" customHeight="1">
-      <c r="A4" s="227"/>
-      <c r="B4" s="243"/>
+      <c r="A4" s="181"/>
+      <c r="B4" s="261"/>
       <c r="C4" s="146">
         <v>3</v>
       </c>
@@ -7578,16 +7573,16 @@
         <v>405</v>
       </c>
       <c r="E4" s="96" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="F4" s="96" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="G4" s="44" t="s">
         <v>407</v>
       </c>
       <c r="H4" s="114" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="I4" s="46"/>
       <c r="J4" s="109" t="s">
@@ -7598,73 +7593,73 @@
         <v>408</v>
       </c>
       <c r="M4" s="96" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="90" customHeight="1">
-      <c r="A5" s="248"/>
-      <c r="B5" s="246"/>
+      <c r="A5" s="273"/>
+      <c r="B5" s="271"/>
       <c r="C5" s="152">
         <v>4</v>
       </c>
-      <c r="D5" s="209"/>
-      <c r="E5" s="209"/>
-      <c r="F5" s="209"/>
-      <c r="G5" s="209"/>
-      <c r="H5" s="209"/>
-      <c r="I5" s="209"/>
-      <c r="J5" s="209"/>
-      <c r="K5" s="209"/>
-      <c r="L5" s="210"/>
+      <c r="D5" s="207"/>
+      <c r="E5" s="207"/>
+      <c r="F5" s="207"/>
+      <c r="G5" s="207"/>
+      <c r="H5" s="207"/>
+      <c r="I5" s="207"/>
+      <c r="J5" s="207"/>
+      <c r="K5" s="207"/>
+      <c r="L5" s="189"/>
       <c r="M5" s="44" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A6" s="227" t="s">
+      <c r="A6" s="181" t="s">
         <v>175</v>
       </c>
-      <c r="B6" s="243" t="s">
+      <c r="B6" s="261" t="s">
         <v>267</v>
       </c>
       <c r="C6" s="153">
         <v>1</v>
       </c>
-      <c r="D6" s="236" t="s">
+      <c r="D6" s="254" t="s">
         <v>292</v>
       </c>
-      <c r="E6" s="236"/>
-      <c r="F6" s="236"/>
-      <c r="G6" s="236"/>
-      <c r="H6" s="236"/>
-      <c r="I6" s="236"/>
-      <c r="J6" s="236"/>
-      <c r="K6" s="236"/>
-      <c r="L6" s="236"/>
-      <c r="M6" s="234"/>
+      <c r="E6" s="254"/>
+      <c r="F6" s="254"/>
+      <c r="G6" s="254"/>
+      <c r="H6" s="254"/>
+      <c r="I6" s="254"/>
+      <c r="J6" s="254"/>
+      <c r="K6" s="254"/>
+      <c r="L6" s="254"/>
+      <c r="M6" s="255"/>
     </row>
     <row r="7" spans="1:14" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A7" s="227"/>
-      <c r="B7" s="243"/>
+      <c r="A7" s="181"/>
+      <c r="B7" s="261"/>
       <c r="C7" s="146">
         <v>2</v>
       </c>
-      <c r="D7" s="237" t="s">
-        <v>505</v>
-      </c>
-      <c r="E7" s="237"/>
-      <c r="F7" s="237"/>
-      <c r="G7" s="237"/>
-      <c r="H7" s="237"/>
-      <c r="I7" s="237"/>
-      <c r="J7" s="237"/>
-      <c r="K7" s="237"/>
-      <c r="L7" s="237"/>
-      <c r="M7" s="238"/>
+      <c r="D7" s="256" t="s">
+        <v>503</v>
+      </c>
+      <c r="E7" s="256"/>
+      <c r="F7" s="256"/>
+      <c r="G7" s="256"/>
+      <c r="H7" s="256"/>
+      <c r="I7" s="256"/>
+      <c r="J7" s="256"/>
+      <c r="K7" s="256"/>
+      <c r="L7" s="256"/>
+      <c r="M7" s="257"/>
     </row>
     <row r="8" spans="1:14" s="16" customFormat="1" ht="105" customHeight="1">
-      <c r="A8" s="227"/>
-      <c r="B8" s="243"/>
+      <c r="A8" s="181"/>
+      <c r="B8" s="261"/>
       <c r="C8" s="146">
         <v>3</v>
       </c>
@@ -7672,16 +7667,16 @@
         <v>387</v>
       </c>
       <c r="E8" s="137" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F8" s="128" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="G8" s="114" t="s">
         <v>369</v>
       </c>
       <c r="H8" s="114" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="I8" s="114"/>
       <c r="J8" s="113" t="s">
@@ -7692,73 +7687,73 @@
         <v>304</v>
       </c>
       <c r="M8" s="125" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="75" customHeight="1">
-      <c r="A9" s="248"/>
-      <c r="B9" s="246"/>
+      <c r="A9" s="273"/>
+      <c r="B9" s="271"/>
       <c r="C9" s="147">
         <v>4</v>
       </c>
-      <c r="D9" s="209"/>
-      <c r="E9" s="210"/>
+      <c r="D9" s="207"/>
+      <c r="E9" s="189"/>
       <c r="F9" s="108" t="s">
         <v>374</v>
       </c>
-      <c r="G9" s="217"/>
-      <c r="H9" s="209"/>
-      <c r="I9" s="209"/>
-      <c r="J9" s="209"/>
-      <c r="K9" s="209"/>
-      <c r="L9" s="209"/>
-      <c r="M9" s="210"/>
+      <c r="G9" s="188"/>
+      <c r="H9" s="207"/>
+      <c r="I9" s="207"/>
+      <c r="J9" s="207"/>
+      <c r="K9" s="207"/>
+      <c r="L9" s="207"/>
+      <c r="M9" s="189"/>
     </row>
     <row r="10" spans="1:14" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A10" s="249" t="s">
+      <c r="A10" s="274" t="s">
         <v>174</v>
       </c>
-      <c r="B10" s="250" t="s">
+      <c r="B10" s="275" t="s">
         <v>268</v>
       </c>
       <c r="C10" s="153">
         <v>1</v>
       </c>
-      <c r="D10" s="236" t="s">
+      <c r="D10" s="254" t="s">
         <v>291</v>
       </c>
-      <c r="E10" s="236"/>
-      <c r="F10" s="236"/>
-      <c r="G10" s="236"/>
-      <c r="H10" s="236"/>
-      <c r="I10" s="236"/>
-      <c r="J10" s="236"/>
-      <c r="K10" s="236"/>
-      <c r="L10" s="236"/>
-      <c r="M10" s="234"/>
+      <c r="E10" s="254"/>
+      <c r="F10" s="254"/>
+      <c r="G10" s="254"/>
+      <c r="H10" s="254"/>
+      <c r="I10" s="254"/>
+      <c r="J10" s="254"/>
+      <c r="K10" s="254"/>
+      <c r="L10" s="254"/>
+      <c r="M10" s="255"/>
     </row>
     <row r="11" spans="1:14" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="227"/>
-      <c r="B11" s="243"/>
+      <c r="A11" s="181"/>
+      <c r="B11" s="261"/>
       <c r="C11" s="146">
         <v>2</v>
       </c>
-      <c r="D11" s="237" t="s">
-        <v>507</v>
-      </c>
-      <c r="E11" s="237"/>
-      <c r="F11" s="237"/>
-      <c r="G11" s="237"/>
-      <c r="H11" s="237"/>
-      <c r="I11" s="237"/>
-      <c r="J11" s="237"/>
-      <c r="K11" s="237"/>
-      <c r="L11" s="237"/>
-      <c r="M11" s="238"/>
+      <c r="D11" s="256" t="s">
+        <v>505</v>
+      </c>
+      <c r="E11" s="256"/>
+      <c r="F11" s="256"/>
+      <c r="G11" s="256"/>
+      <c r="H11" s="256"/>
+      <c r="I11" s="256"/>
+      <c r="J11" s="256"/>
+      <c r="K11" s="256"/>
+      <c r="L11" s="256"/>
+      <c r="M11" s="257"/>
     </row>
     <row r="12" spans="1:14" s="16" customFormat="1" ht="105" customHeight="1">
-      <c r="A12" s="227"/>
-      <c r="B12" s="243"/>
+      <c r="A12" s="181"/>
+      <c r="B12" s="261"/>
       <c r="C12" s="146">
         <v>3</v>
       </c>
@@ -7766,16 +7761,16 @@
         <v>386</v>
       </c>
       <c r="E12" s="137" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="F12" s="46" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="G12" s="44" t="s">
         <v>368</v>
       </c>
       <c r="H12" s="114" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I12" s="96"/>
       <c r="J12" s="113" t="s">
@@ -7786,200 +7781,200 @@
         <v>303</v>
       </c>
       <c r="M12" s="125" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="90" customHeight="1">
-      <c r="A13" s="165"/>
-      <c r="B13" s="244"/>
+      <c r="A13" s="162"/>
+      <c r="B13" s="269"/>
       <c r="C13" s="147">
         <v>4</v>
       </c>
-      <c r="D13" s="209"/>
-      <c r="E13" s="209"/>
-      <c r="F13" s="209"/>
-      <c r="G13" s="209"/>
-      <c r="H13" s="210"/>
+      <c r="D13" s="207"/>
+      <c r="E13" s="207"/>
+      <c r="F13" s="207"/>
+      <c r="G13" s="207"/>
+      <c r="H13" s="189"/>
       <c r="I13" s="99" t="s">
         <v>375</v>
       </c>
-      <c r="J13" s="217"/>
-      <c r="K13" s="209"/>
-      <c r="L13" s="209"/>
-      <c r="M13" s="210"/>
+      <c r="J13" s="188"/>
+      <c r="K13" s="207"/>
+      <c r="L13" s="207"/>
+      <c r="M13" s="189"/>
     </row>
     <row r="14" spans="1:14" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A14" s="164" t="s">
+      <c r="A14" s="161" t="s">
         <v>173</v>
       </c>
-      <c r="B14" s="242" t="s">
+      <c r="B14" s="260" t="s">
         <v>269</v>
       </c>
       <c r="C14" s="153">
         <v>1</v>
       </c>
-      <c r="D14" s="236" t="s">
+      <c r="D14" s="254" t="s">
         <v>290</v>
       </c>
-      <c r="E14" s="236"/>
-      <c r="F14" s="236"/>
-      <c r="G14" s="236"/>
-      <c r="H14" s="236"/>
-      <c r="I14" s="236"/>
-      <c r="J14" s="236"/>
-      <c r="K14" s="236"/>
-      <c r="L14" s="236"/>
-      <c r="M14" s="234"/>
+      <c r="E14" s="254"/>
+      <c r="F14" s="254"/>
+      <c r="G14" s="254"/>
+      <c r="H14" s="254"/>
+      <c r="I14" s="254"/>
+      <c r="J14" s="254"/>
+      <c r="K14" s="254"/>
+      <c r="L14" s="254"/>
+      <c r="M14" s="255"/>
     </row>
     <row r="15" spans="1:14" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A15" s="227"/>
-      <c r="B15" s="243"/>
+      <c r="A15" s="181"/>
+      <c r="B15" s="261"/>
       <c r="C15" s="146">
         <v>2</v>
       </c>
-      <c r="D15" s="237" t="s">
-        <v>508</v>
-      </c>
-      <c r="E15" s="237"/>
-      <c r="F15" s="237"/>
-      <c r="G15" s="237"/>
-      <c r="H15" s="237"/>
-      <c r="I15" s="237"/>
-      <c r="J15" s="237"/>
-      <c r="K15" s="237"/>
-      <c r="L15" s="237"/>
-      <c r="M15" s="238"/>
+      <c r="D15" s="256" t="s">
+        <v>506</v>
+      </c>
+      <c r="E15" s="256"/>
+      <c r="F15" s="256"/>
+      <c r="G15" s="256"/>
+      <c r="H15" s="256"/>
+      <c r="I15" s="256"/>
+      <c r="J15" s="256"/>
+      <c r="K15" s="256"/>
+      <c r="L15" s="256"/>
+      <c r="M15" s="257"/>
     </row>
     <row r="16" spans="1:14" s="16" customFormat="1" ht="105" customHeight="1">
-      <c r="A16" s="227"/>
-      <c r="B16" s="243"/>
+      <c r="A16" s="181"/>
+      <c r="B16" s="261"/>
       <c r="C16" s="146">
         <v>3</v>
       </c>
       <c r="D16" s="92" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E16" s="137" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="F16" s="46" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="G16" s="44" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="H16" s="114" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="I16" s="112"/>
       <c r="J16" s="113" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="K16" s="112"/>
       <c r="L16" s="112" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="M16" s="125" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="17" spans="1:16382" ht="75" customHeight="1">
-      <c r="A17" s="165"/>
-      <c r="B17" s="244"/>
+      <c r="A17" s="162"/>
+      <c r="B17" s="269"/>
       <c r="C17" s="147">
         <v>4</v>
       </c>
-      <c r="D17" s="209"/>
-      <c r="E17" s="209"/>
-      <c r="F17" s="210"/>
+      <c r="D17" s="207"/>
+      <c r="E17" s="207"/>
+      <c r="F17" s="189"/>
       <c r="G17" s="99" t="s">
         <v>324</v>
       </c>
-      <c r="H17" s="217"/>
-      <c r="I17" s="209"/>
-      <c r="J17" s="209"/>
-      <c r="K17" s="209"/>
-      <c r="L17" s="209"/>
-      <c r="M17" s="210"/>
+      <c r="H17" s="188"/>
+      <c r="I17" s="207"/>
+      <c r="J17" s="207"/>
+      <c r="K17" s="207"/>
+      <c r="L17" s="207"/>
+      <c r="M17" s="189"/>
     </row>
     <row r="18" spans="1:16382" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A18" s="164" t="s">
+      <c r="A18" s="161" t="s">
         <v>172</v>
       </c>
-      <c r="B18" s="242" t="s">
+      <c r="B18" s="260" t="s">
         <v>270</v>
       </c>
       <c r="C18" s="153">
         <v>1</v>
       </c>
-      <c r="D18" s="236" t="s">
-        <v>451</v>
-      </c>
-      <c r="E18" s="236"/>
-      <c r="F18" s="236"/>
-      <c r="G18" s="236"/>
-      <c r="H18" s="236"/>
-      <c r="I18" s="236"/>
-      <c r="J18" s="236"/>
-      <c r="K18" s="236"/>
-      <c r="L18" s="236"/>
-      <c r="M18" s="234"/>
+      <c r="D18" s="254" t="s">
+        <v>449</v>
+      </c>
+      <c r="E18" s="254"/>
+      <c r="F18" s="254"/>
+      <c r="G18" s="254"/>
+      <c r="H18" s="254"/>
+      <c r="I18" s="254"/>
+      <c r="J18" s="254"/>
+      <c r="K18" s="254"/>
+      <c r="L18" s="254"/>
+      <c r="M18" s="255"/>
     </row>
     <row r="19" spans="1:16382" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A19" s="227"/>
-      <c r="B19" s="243"/>
+      <c r="A19" s="181"/>
+      <c r="B19" s="261"/>
       <c r="C19" s="146">
         <v>2</v>
       </c>
-      <c r="D19" s="237" t="s">
-        <v>509</v>
-      </c>
-      <c r="E19" s="237"/>
-      <c r="F19" s="237"/>
-      <c r="G19" s="237"/>
-      <c r="H19" s="237"/>
-      <c r="I19" s="237"/>
-      <c r="J19" s="237"/>
-      <c r="K19" s="237"/>
-      <c r="L19" s="237"/>
-      <c r="M19" s="238"/>
+      <c r="D19" s="256" t="s">
+        <v>507</v>
+      </c>
+      <c r="E19" s="256"/>
+      <c r="F19" s="256"/>
+      <c r="G19" s="256"/>
+      <c r="H19" s="256"/>
+      <c r="I19" s="256"/>
+      <c r="J19" s="256"/>
+      <c r="K19" s="256"/>
+      <c r="L19" s="256"/>
+      <c r="M19" s="257"/>
     </row>
     <row r="20" spans="1:16382" s="16" customFormat="1" ht="105" customHeight="1">
-      <c r="A20" s="227"/>
-      <c r="B20" s="243"/>
+      <c r="A20" s="181"/>
+      <c r="B20" s="261"/>
       <c r="C20" s="146">
         <v>3</v>
       </c>
       <c r="D20" s="92" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E20" s="137" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="F20" s="112" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="G20" s="112" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="H20" s="114" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="I20" s="112"/>
       <c r="J20" s="113" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="K20" s="112"/>
       <c r="L20" s="112" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="M20" s="125" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="21" spans="1:16382" s="67" customFormat="1" ht="60" customHeight="1">
-      <c r="A21" s="260"/>
-      <c r="B21" s="254"/>
+      <c r="A21" s="265"/>
+      <c r="B21" s="262"/>
       <c r="C21" s="147">
         <v>4</v>
       </c>
@@ -7987,14 +7982,14 @@
       <c r="E21" s="123" t="s">
         <v>373</v>
       </c>
-      <c r="F21" s="239"/>
-      <c r="G21" s="240"/>
-      <c r="H21" s="240"/>
-      <c r="I21" s="240"/>
-      <c r="J21" s="240"/>
-      <c r="K21" s="240"/>
-      <c r="L21" s="240"/>
-      <c r="M21" s="241"/>
+      <c r="F21" s="215"/>
+      <c r="G21" s="216"/>
+      <c r="H21" s="216"/>
+      <c r="I21" s="216"/>
+      <c r="J21" s="216"/>
+      <c r="K21" s="216"/>
+      <c r="L21" s="216"/>
+      <c r="M21" s="277"/>
       <c r="N21" s="70"/>
       <c r="O21" s="70"/>
       <c r="P21" s="70"/>
@@ -24366,50 +24361,50 @@
       <c r="XFB21" s="70"/>
     </row>
     <row r="22" spans="1:16382" s="68" customFormat="1" ht="15" customHeight="1">
-      <c r="A22" s="259" t="s">
+      <c r="A22" s="264" t="s">
         <v>171</v>
       </c>
-      <c r="B22" s="258" t="s">
-        <v>459</v>
+      <c r="B22" s="263" t="s">
+        <v>457</v>
       </c>
       <c r="C22" s="153">
         <v>1</v>
       </c>
-      <c r="D22" s="237" t="s">
+      <c r="D22" s="256" t="s">
         <v>289</v>
       </c>
-      <c r="E22" s="237"/>
-      <c r="F22" s="237"/>
-      <c r="G22" s="237"/>
-      <c r="H22" s="237"/>
-      <c r="I22" s="237"/>
-      <c r="J22" s="237"/>
-      <c r="K22" s="237"/>
-      <c r="L22" s="237"/>
-      <c r="M22" s="238"/>
+      <c r="E22" s="256"/>
+      <c r="F22" s="256"/>
+      <c r="G22" s="256"/>
+      <c r="H22" s="256"/>
+      <c r="I22" s="256"/>
+      <c r="J22" s="256"/>
+      <c r="K22" s="256"/>
+      <c r="L22" s="256"/>
+      <c r="M22" s="257"/>
     </row>
     <row r="23" spans="1:16382" s="68" customFormat="1" ht="15" customHeight="1">
-      <c r="A23" s="256"/>
-      <c r="B23" s="202"/>
+      <c r="A23" s="250"/>
+      <c r="B23" s="182"/>
       <c r="C23" s="146">
         <v>2</v>
       </c>
-      <c r="D23" s="237" t="s">
-        <v>510</v>
-      </c>
-      <c r="E23" s="237"/>
-      <c r="F23" s="237"/>
-      <c r="G23" s="237"/>
-      <c r="H23" s="237"/>
-      <c r="I23" s="237"/>
-      <c r="J23" s="237"/>
-      <c r="K23" s="237"/>
-      <c r="L23" s="237"/>
-      <c r="M23" s="238"/>
+      <c r="D23" s="256" t="s">
+        <v>508</v>
+      </c>
+      <c r="E23" s="256"/>
+      <c r="F23" s="256"/>
+      <c r="G23" s="256"/>
+      <c r="H23" s="256"/>
+      <c r="I23" s="256"/>
+      <c r="J23" s="256"/>
+      <c r="K23" s="256"/>
+      <c r="L23" s="256"/>
+      <c r="M23" s="257"/>
     </row>
     <row r="24" spans="1:16382" s="68" customFormat="1" ht="105" customHeight="1">
-      <c r="A24" s="256"/>
-      <c r="B24" s="202"/>
+      <c r="A24" s="250"/>
+      <c r="B24" s="182"/>
       <c r="C24" s="146">
         <v>3</v>
       </c>
@@ -24418,13 +24413,13 @@
       </c>
       <c r="E24" s="137"/>
       <c r="F24" s="112" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G24" s="112" t="s">
         <v>372</v>
       </c>
       <c r="H24" s="112" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="I24" s="112"/>
       <c r="J24" s="113" t="s">
@@ -24435,73 +24430,73 @@
         <v>302</v>
       </c>
       <c r="M24" s="125" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="25" spans="1:16382" s="70" customFormat="1" ht="90" customHeight="1">
-      <c r="A25" s="257"/>
-      <c r="B25" s="173"/>
+      <c r="A25" s="253"/>
+      <c r="B25" s="170"/>
       <c r="C25" s="147">
         <v>4</v>
       </c>
       <c r="D25" s="98" t="s">
         <v>376</v>
       </c>
-      <c r="E25" s="217"/>
-      <c r="F25" s="209"/>
-      <c r="G25" s="209"/>
-      <c r="H25" s="209"/>
-      <c r="I25" s="209"/>
-      <c r="J25" s="209"/>
-      <c r="K25" s="209"/>
-      <c r="L25" s="209"/>
-      <c r="M25" s="210"/>
+      <c r="E25" s="188"/>
+      <c r="F25" s="207"/>
+      <c r="G25" s="207"/>
+      <c r="H25" s="207"/>
+      <c r="I25" s="207"/>
+      <c r="J25" s="207"/>
+      <c r="K25" s="207"/>
+      <c r="L25" s="207"/>
+      <c r="M25" s="189"/>
     </row>
     <row r="26" spans="1:16382" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A26" s="261" t="s">
+      <c r="A26" s="252" t="s">
         <v>170</v>
       </c>
-      <c r="B26" s="172" t="s">
-        <v>460</v>
+      <c r="B26" s="169" t="s">
+        <v>458</v>
       </c>
       <c r="C26" s="153">
         <v>1</v>
       </c>
-      <c r="D26" s="236" t="s">
+      <c r="D26" s="254" t="s">
         <v>288</v>
       </c>
-      <c r="E26" s="236"/>
-      <c r="F26" s="236"/>
-      <c r="G26" s="236"/>
-      <c r="H26" s="236"/>
-      <c r="I26" s="236"/>
-      <c r="J26" s="236"/>
-      <c r="K26" s="236"/>
-      <c r="L26" s="236"/>
-      <c r="M26" s="234"/>
+      <c r="E26" s="254"/>
+      <c r="F26" s="254"/>
+      <c r="G26" s="254"/>
+      <c r="H26" s="254"/>
+      <c r="I26" s="254"/>
+      <c r="J26" s="254"/>
+      <c r="K26" s="254"/>
+      <c r="L26" s="254"/>
+      <c r="M26" s="255"/>
     </row>
     <row r="27" spans="1:16382" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A27" s="256"/>
-      <c r="B27" s="202"/>
+      <c r="A27" s="250"/>
+      <c r="B27" s="182"/>
       <c r="C27" s="146">
         <v>2</v>
       </c>
-      <c r="D27" s="237" t="s">
-        <v>511</v>
-      </c>
-      <c r="E27" s="237"/>
-      <c r="F27" s="237"/>
-      <c r="G27" s="237"/>
-      <c r="H27" s="237"/>
-      <c r="I27" s="237"/>
-      <c r="J27" s="237"/>
-      <c r="K27" s="237"/>
-      <c r="L27" s="237"/>
-      <c r="M27" s="238"/>
+      <c r="D27" s="256" t="s">
+        <v>509</v>
+      </c>
+      <c r="E27" s="256"/>
+      <c r="F27" s="256"/>
+      <c r="G27" s="256"/>
+      <c r="H27" s="256"/>
+      <c r="I27" s="256"/>
+      <c r="J27" s="256"/>
+      <c r="K27" s="256"/>
+      <c r="L27" s="256"/>
+      <c r="M27" s="257"/>
     </row>
     <row r="28" spans="1:16382" s="16" customFormat="1" ht="105" customHeight="1">
-      <c r="A28" s="256"/>
-      <c r="B28" s="202"/>
+      <c r="A28" s="250"/>
+      <c r="B28" s="182"/>
       <c r="C28" s="146">
         <v>3</v>
       </c>
@@ -24510,13 +24505,13 @@
       </c>
       <c r="E28" s="96"/>
       <c r="F28" s="112" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="G28" s="96" t="s">
         <v>371</v>
       </c>
       <c r="H28" s="128" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="I28" s="112"/>
       <c r="J28" s="112" t="s">
@@ -24525,73 +24520,73 @@
       <c r="K28" s="112"/>
       <c r="L28" s="112"/>
       <c r="M28" s="125" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="29" spans="1:16382" ht="60" customHeight="1">
-      <c r="A29" s="257"/>
-      <c r="B29" s="173"/>
+      <c r="A29" s="253"/>
+      <c r="B29" s="170"/>
       <c r="C29" s="147">
         <v>4</v>
       </c>
-      <c r="D29" s="209"/>
-      <c r="E29" s="209"/>
-      <c r="F29" s="209"/>
-      <c r="G29" s="210"/>
+      <c r="D29" s="207"/>
+      <c r="E29" s="207"/>
+      <c r="F29" s="207"/>
+      <c r="G29" s="189"/>
       <c r="H29" s="90" t="s">
         <v>307</v>
       </c>
-      <c r="I29" s="217"/>
-      <c r="J29" s="209"/>
-      <c r="K29" s="209"/>
-      <c r="L29" s="209"/>
-      <c r="M29" s="210"/>
+      <c r="I29" s="188"/>
+      <c r="J29" s="207"/>
+      <c r="K29" s="207"/>
+      <c r="L29" s="207"/>
+      <c r="M29" s="189"/>
     </row>
     <row r="30" spans="1:16382" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A30" s="261" t="s">
+      <c r="A30" s="252" t="s">
         <v>278</v>
       </c>
-      <c r="B30" s="172" t="s">
-        <v>461</v>
+      <c r="B30" s="169" t="s">
+        <v>459</v>
       </c>
       <c r="C30" s="153">
         <v>1</v>
       </c>
-      <c r="D30" s="236" t="s">
+      <c r="D30" s="254" t="s">
         <v>299</v>
       </c>
-      <c r="E30" s="236"/>
-      <c r="F30" s="236"/>
-      <c r="G30" s="236"/>
-      <c r="H30" s="236"/>
-      <c r="I30" s="236"/>
-      <c r="J30" s="236"/>
-      <c r="K30" s="236"/>
-      <c r="L30" s="236"/>
-      <c r="M30" s="234"/>
+      <c r="E30" s="254"/>
+      <c r="F30" s="254"/>
+      <c r="G30" s="254"/>
+      <c r="H30" s="254"/>
+      <c r="I30" s="254"/>
+      <c r="J30" s="254"/>
+      <c r="K30" s="254"/>
+      <c r="L30" s="254"/>
+      <c r="M30" s="255"/>
     </row>
     <row r="31" spans="1:16382" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A31" s="256"/>
-      <c r="B31" s="202"/>
+      <c r="A31" s="250"/>
+      <c r="B31" s="182"/>
       <c r="C31" s="146">
         <v>2</v>
       </c>
-      <c r="D31" s="237" t="s">
-        <v>512</v>
-      </c>
-      <c r="E31" s="237"/>
-      <c r="F31" s="237"/>
-      <c r="G31" s="237"/>
-      <c r="H31" s="237"/>
-      <c r="I31" s="237"/>
-      <c r="J31" s="237"/>
-      <c r="K31" s="237"/>
-      <c r="L31" s="237"/>
-      <c r="M31" s="238"/>
+      <c r="D31" s="256" t="s">
+        <v>510</v>
+      </c>
+      <c r="E31" s="256"/>
+      <c r="F31" s="256"/>
+      <c r="G31" s="256"/>
+      <c r="H31" s="256"/>
+      <c r="I31" s="256"/>
+      <c r="J31" s="256"/>
+      <c r="K31" s="256"/>
+      <c r="L31" s="256"/>
+      <c r="M31" s="257"/>
     </row>
     <row r="32" spans="1:16382" ht="105" customHeight="1">
-      <c r="A32" s="256"/>
-      <c r="B32" s="202"/>
+      <c r="A32" s="250"/>
+      <c r="B32" s="182"/>
       <c r="C32" s="146">
         <v>3</v>
       </c>
@@ -24600,13 +24595,13 @@
       </c>
       <c r="E32" s="44"/>
       <c r="F32" s="112" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G32" s="44" t="s">
         <v>370</v>
       </c>
       <c r="H32" s="128" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I32" s="44"/>
       <c r="J32" s="96" t="s">
@@ -24617,73 +24612,73 @@
         <v>305</v>
       </c>
       <c r="M32" s="125" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="33" spans="1:13" s="16" customFormat="1" ht="45" customHeight="1">
-      <c r="A33" s="256"/>
-      <c r="B33" s="202"/>
+      <c r="A33" s="250"/>
+      <c r="B33" s="182"/>
       <c r="C33" s="147">
         <v>4</v>
       </c>
-      <c r="D33" s="209"/>
-      <c r="E33" s="209"/>
-      <c r="F33" s="209"/>
-      <c r="G33" s="209"/>
-      <c r="H33" s="209"/>
-      <c r="I33" s="209"/>
-      <c r="J33" s="209"/>
-      <c r="K33" s="210"/>
+      <c r="D33" s="207"/>
+      <c r="E33" s="207"/>
+      <c r="F33" s="207"/>
+      <c r="G33" s="207"/>
+      <c r="H33" s="207"/>
+      <c r="I33" s="207"/>
+      <c r="J33" s="207"/>
+      <c r="K33" s="189"/>
       <c r="L33" s="46" t="s">
         <v>366</v>
       </c>
       <c r="M33" s="57"/>
     </row>
     <row r="34" spans="1:13" ht="15" customHeight="1">
-      <c r="A34" s="255" t="s">
+      <c r="A34" s="249" t="s">
         <v>169</v>
       </c>
-      <c r="B34" s="223" t="s">
-        <v>462</v>
+      <c r="B34" s="200" t="s">
+        <v>460</v>
       </c>
       <c r="C34" s="153">
         <v>1</v>
       </c>
-      <c r="D34" s="236" t="s">
+      <c r="D34" s="254" t="s">
         <v>287</v>
       </c>
-      <c r="E34" s="236"/>
-      <c r="F34" s="236"/>
-      <c r="G34" s="236"/>
-      <c r="H34" s="236"/>
-      <c r="I34" s="236"/>
-      <c r="J34" s="236"/>
-      <c r="K34" s="236"/>
-      <c r="L34" s="236"/>
-      <c r="M34" s="234"/>
+      <c r="E34" s="254"/>
+      <c r="F34" s="254"/>
+      <c r="G34" s="254"/>
+      <c r="H34" s="254"/>
+      <c r="I34" s="254"/>
+      <c r="J34" s="254"/>
+      <c r="K34" s="254"/>
+      <c r="L34" s="254"/>
+      <c r="M34" s="255"/>
     </row>
     <row r="35" spans="1:13" ht="15" customHeight="1">
-      <c r="A35" s="256"/>
-      <c r="B35" s="202"/>
+      <c r="A35" s="250"/>
+      <c r="B35" s="182"/>
       <c r="C35" s="146">
         <v>2</v>
       </c>
-      <c r="D35" s="237" t="s">
-        <v>513</v>
-      </c>
-      <c r="E35" s="237"/>
-      <c r="F35" s="237"/>
-      <c r="G35" s="237"/>
-      <c r="H35" s="237"/>
-      <c r="I35" s="237"/>
-      <c r="J35" s="237"/>
-      <c r="K35" s="237"/>
-      <c r="L35" s="237"/>
-      <c r="M35" s="238"/>
+      <c r="D35" s="256" t="s">
+        <v>511</v>
+      </c>
+      <c r="E35" s="256"/>
+      <c r="F35" s="256"/>
+      <c r="G35" s="256"/>
+      <c r="H35" s="256"/>
+      <c r="I35" s="256"/>
+      <c r="J35" s="256"/>
+      <c r="K35" s="256"/>
+      <c r="L35" s="256"/>
+      <c r="M35" s="257"/>
     </row>
     <row r="36" spans="1:13" ht="105" customHeight="1">
-      <c r="A36" s="256"/>
-      <c r="B36" s="202"/>
+      <c r="A36" s="250"/>
+      <c r="B36" s="182"/>
       <c r="C36" s="146">
         <v>3</v>
       </c>
@@ -24692,13 +24687,13 @@
       </c>
       <c r="E36" s="96"/>
       <c r="F36" s="112" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G36" s="96" t="s">
         <v>380</v>
       </c>
       <c r="H36" s="96" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="I36" s="96"/>
       <c r="J36" s="96" t="s">
@@ -24709,22 +24704,22 @@
         <v>306</v>
       </c>
       <c r="M36" s="125" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="37" spans="1:13" s="16" customFormat="1" ht="45" customHeight="1">
-      <c r="A37" s="257"/>
-      <c r="B37" s="173"/>
+      <c r="A37" s="253"/>
+      <c r="B37" s="170"/>
       <c r="C37" s="147">
         <v>4</v>
       </c>
-      <c r="D37" s="209"/>
-      <c r="E37" s="209"/>
-      <c r="F37" s="209"/>
-      <c r="G37" s="209"/>
-      <c r="H37" s="209"/>
-      <c r="I37" s="209"/>
-      <c r="J37" s="210"/>
+      <c r="D37" s="207"/>
+      <c r="E37" s="207"/>
+      <c r="F37" s="207"/>
+      <c r="G37" s="207"/>
+      <c r="H37" s="207"/>
+      <c r="I37" s="207"/>
+      <c r="J37" s="189"/>
       <c r="K37" s="90" t="s">
         <v>365</v>
       </c>
@@ -24732,31 +24727,31 @@
       <c r="M37" s="110"/>
     </row>
     <row r="38" spans="1:13" s="70" customFormat="1" ht="15" customHeight="1">
-      <c r="A38" s="261" t="s">
+      <c r="A38" s="252" t="s">
         <v>168</v>
       </c>
-      <c r="B38" s="172" t="s">
+      <c r="B38" s="169" t="s">
         <v>280</v>
       </c>
       <c r="C38" s="146">
         <v>1</v>
       </c>
-      <c r="D38" s="263" t="s">
+      <c r="D38" s="258" t="s">
         <v>283</v>
       </c>
-      <c r="E38" s="264"/>
-      <c r="F38" s="264"/>
-      <c r="G38" s="264"/>
-      <c r="H38" s="264"/>
-      <c r="I38" s="264"/>
-      <c r="J38" s="264"/>
-      <c r="K38" s="264"/>
-      <c r="L38" s="264"/>
-      <c r="M38" s="264"/>
+      <c r="E38" s="259"/>
+      <c r="F38" s="259"/>
+      <c r="G38" s="259"/>
+      <c r="H38" s="259"/>
+      <c r="I38" s="259"/>
+      <c r="J38" s="259"/>
+      <c r="K38" s="259"/>
+      <c r="L38" s="259"/>
+      <c r="M38" s="259"/>
     </row>
     <row r="39" spans="1:13" s="68" customFormat="1" ht="120" customHeight="1">
-      <c r="A39" s="262"/>
-      <c r="B39" s="220"/>
+      <c r="A39" s="251"/>
+      <c r="B39" s="201"/>
       <c r="C39" s="146">
         <v>4</v>
       </c>
@@ -24768,7 +24763,7 @@
       </c>
       <c r="F39" s="101"/>
       <c r="G39" s="101" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="H39" s="69"/>
       <c r="I39" s="69"/>
@@ -24778,31 +24773,31 @@
       <c r="M39" s="69"/>
     </row>
     <row r="40" spans="1:13" s="70" customFormat="1" ht="15" customHeight="1">
-      <c r="A40" s="255" t="s">
+      <c r="A40" s="249" t="s">
         <v>167</v>
       </c>
-      <c r="B40" s="223" t="s">
+      <c r="B40" s="200" t="s">
         <v>279</v>
       </c>
       <c r="C40" s="148">
         <v>1</v>
       </c>
-      <c r="D40" s="234" t="s">
+      <c r="D40" s="255" t="s">
         <v>284</v>
       </c>
-      <c r="E40" s="235"/>
-      <c r="F40" s="235"/>
-      <c r="G40" s="235"/>
-      <c r="H40" s="235"/>
-      <c r="I40" s="235"/>
-      <c r="J40" s="235"/>
-      <c r="K40" s="235"/>
-      <c r="L40" s="235"/>
-      <c r="M40" s="235"/>
+      <c r="E40" s="276"/>
+      <c r="F40" s="276"/>
+      <c r="G40" s="276"/>
+      <c r="H40" s="276"/>
+      <c r="I40" s="276"/>
+      <c r="J40" s="276"/>
+      <c r="K40" s="276"/>
+      <c r="L40" s="276"/>
+      <c r="M40" s="276"/>
     </row>
     <row r="41" spans="1:13" s="16" customFormat="1" ht="150" customHeight="1">
-      <c r="A41" s="262"/>
-      <c r="B41" s="220"/>
+      <c r="A41" s="251"/>
+      <c r="B41" s="201"/>
       <c r="C41" s="146">
         <v>4</v>
       </c>
@@ -24814,7 +24809,7 @@
       </c>
       <c r="F41" s="101"/>
       <c r="G41" s="101" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="H41" s="69"/>
       <c r="I41" s="69"/>
@@ -24824,31 +24819,31 @@
       <c r="M41" s="69"/>
     </row>
     <row r="42" spans="1:13" s="70" customFormat="1" ht="15" customHeight="1">
-      <c r="A42" s="255" t="s">
+      <c r="A42" s="249" t="s">
         <v>166</v>
       </c>
-      <c r="B42" s="223" t="s">
+      <c r="B42" s="200" t="s">
         <v>281</v>
       </c>
       <c r="C42" s="148">
         <v>1</v>
       </c>
-      <c r="D42" s="234" t="s">
+      <c r="D42" s="255" t="s">
         <v>285</v>
       </c>
-      <c r="E42" s="235"/>
-      <c r="F42" s="235"/>
-      <c r="G42" s="235"/>
-      <c r="H42" s="235"/>
-      <c r="I42" s="235"/>
-      <c r="J42" s="235"/>
-      <c r="K42" s="235"/>
-      <c r="L42" s="235"/>
-      <c r="M42" s="235"/>
+      <c r="E42" s="276"/>
+      <c r="F42" s="276"/>
+      <c r="G42" s="276"/>
+      <c r="H42" s="276"/>
+      <c r="I42" s="276"/>
+      <c r="J42" s="276"/>
+      <c r="K42" s="276"/>
+      <c r="L42" s="276"/>
+      <c r="M42" s="276"/>
     </row>
     <row r="43" spans="1:13" s="100" customFormat="1" ht="225" customHeight="1">
-      <c r="A43" s="256"/>
-      <c r="B43" s="220"/>
+      <c r="A43" s="250"/>
+      <c r="B43" s="201"/>
       <c r="C43" s="154">
         <v>4</v>
       </c>
@@ -24860,7 +24855,7 @@
       </c>
       <c r="F43" s="101"/>
       <c r="G43" s="101" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="H43" s="69"/>
       <c r="I43" s="69"/>
@@ -24870,31 +24865,31 @@
       <c r="M43" s="69"/>
     </row>
     <row r="44" spans="1:13" s="70" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A44" s="265" t="s">
+      <c r="A44" s="246" t="s">
         <v>165</v>
       </c>
-      <c r="B44" s="202" t="s">
+      <c r="B44" s="182" t="s">
         <v>282</v>
       </c>
       <c r="C44" s="146">
         <v>1</v>
       </c>
-      <c r="D44" s="234" t="s">
+      <c r="D44" s="255" t="s">
         <v>286</v>
       </c>
-      <c r="E44" s="235"/>
-      <c r="F44" s="235"/>
-      <c r="G44" s="235"/>
-      <c r="H44" s="235"/>
-      <c r="I44" s="235"/>
-      <c r="J44" s="235"/>
-      <c r="K44" s="235"/>
-      <c r="L44" s="235"/>
-      <c r="M44" s="235"/>
+      <c r="E44" s="276"/>
+      <c r="F44" s="276"/>
+      <c r="G44" s="276"/>
+      <c r="H44" s="276"/>
+      <c r="I44" s="276"/>
+      <c r="J44" s="276"/>
+      <c r="K44" s="276"/>
+      <c r="L44" s="276"/>
+      <c r="M44" s="276"/>
     </row>
     <row r="45" spans="1:13" ht="300" customHeight="1">
-      <c r="A45" s="266"/>
-      <c r="B45" s="267"/>
+      <c r="A45" s="247"/>
+      <c r="B45" s="248"/>
       <c r="C45" s="149">
         <v>4</v>
       </c>
@@ -24905,10 +24900,10 @@
         <v>301</v>
       </c>
       <c r="F45" s="74" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="G45" s="74" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="H45" s="66" t="s">
         <v>300</v>
@@ -24973,31 +24968,27 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="D30:M30"/>
-    <mergeCell ref="D33:K33"/>
-    <mergeCell ref="D37:J37"/>
-    <mergeCell ref="D35:M35"/>
-    <mergeCell ref="D34:M34"/>
-    <mergeCell ref="D38:M38"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="D40:M40"/>
+    <mergeCell ref="D42:M42"/>
+    <mergeCell ref="D44:M44"/>
+    <mergeCell ref="D18:M18"/>
+    <mergeCell ref="D19:M19"/>
+    <mergeCell ref="D31:M31"/>
+    <mergeCell ref="D26:M26"/>
+    <mergeCell ref="D27:M27"/>
+    <mergeCell ref="F21:M21"/>
+    <mergeCell ref="E25:M25"/>
+    <mergeCell ref="D22:M22"/>
+    <mergeCell ref="D23:M23"/>
+    <mergeCell ref="I29:M29"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
     <mergeCell ref="D2:M2"/>
     <mergeCell ref="D3:M3"/>
     <mergeCell ref="D6:M6"/>
@@ -25013,27 +25004,31 @@
     <mergeCell ref="D11:M11"/>
     <mergeCell ref="D14:M14"/>
     <mergeCell ref="D15:M15"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="D40:M40"/>
-    <mergeCell ref="D42:M42"/>
-    <mergeCell ref="D44:M44"/>
-    <mergeCell ref="D18:M18"/>
-    <mergeCell ref="D19:M19"/>
-    <mergeCell ref="D31:M31"/>
-    <mergeCell ref="D26:M26"/>
-    <mergeCell ref="D27:M27"/>
-    <mergeCell ref="F21:M21"/>
-    <mergeCell ref="E25:M25"/>
-    <mergeCell ref="D22:M22"/>
-    <mergeCell ref="D23:M23"/>
-    <mergeCell ref="I29:M29"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="D30:M30"/>
+    <mergeCell ref="D33:K33"/>
+    <mergeCell ref="D37:J37"/>
+    <mergeCell ref="D35:M35"/>
+    <mergeCell ref="D34:M34"/>
+    <mergeCell ref="D38:M38"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A40:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fleshed out the enchanting system's point buy mechanic.
</commit_message>
<xml_diff>
--- a/Tags and Affinities.xlsx
+++ b/Tags and Affinities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Documents\Git Repositories\materials_and_crafting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719AE8E4-CACB-4244-94E3-791FD4073682}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9FFE48-0C5E-467D-8966-01A1F016CC70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{8FD76562-234B-40A6-8AC6-52675E21BBDC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{8FD76562-234B-40A6-8AC6-52675E21BBDC}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPONENT TAGS" sheetId="2" r:id="rId1"/>
@@ -2180,9 +2180,6 @@
     <t>WEAPON</t>
   </si>
   <si>
-    <t>When you intercept an attack with this cloak, roll a d20. On a 10 or lower, the cloak is irrepearably damaged and becomes unusable.</t>
-  </si>
-  <si>
     <t>This item confers to the wielder damage resistance to the specified damage type equal to its damage affinity.</t>
   </si>
   <si>
@@ -2741,32 +2738,6 @@
 You become immune to the damage type you rolled until the end of your next turn.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Increase the MCI of any </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>force binding</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> spells that conduct through this material by its force affinity.</t>
-    </r>
-  </si>
-  <si>
     <t>TIER</t>
   </si>
   <si>
@@ -2806,9 +2777,6 @@
   </si>
   <si>
     <t>This item counts as holding a number of tier of fire affinity equal to its ignan affinity.</t>
-  </si>
-  <si>
-    <t>This item counts as holding a number of tier of acid or poison affinity equal to its primal affinity</t>
   </si>
   <si>
     <t>This item counts as holding a number of tier of cold affinity equal to its aquan affinity.</t>
@@ -3151,6 +3119,38 @@
   </si>
   <si>
     <t>The bearer of this tattoo gains 1d4 temporary hit points per nourishing tier at the start of each of their turns. The first time they are reduced to 0 hit points each day, they regain hit points equal to the tattoo's nourishing tier at the start of their next turn.</t>
+  </si>
+  <si>
+    <t>The cloak takes double damage when used to intercept damage.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Increase the MCI of any </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>magic weapon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> spells that conduct through this material by its force affinity.</t>
+    </r>
+  </si>
+  <si>
+    <t>This item counts as holding a number of tier of acid or poison affinity equal to its primal affinity.</t>
   </si>
 </sst>
 </file>
@@ -4798,6 +4798,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="91" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -4858,119 +4877,299 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="90" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="88" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="86" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="87" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="75" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -4978,208 +5177,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="90" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="88" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="86" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="87" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="91" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5512,10 +5512,10 @@
   <sheetData>
     <row r="1" spans="1:11" s="16" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="18" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>373</v>
@@ -5555,14 +5555,14 @@
       <c r="C2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="171"/>
-      <c r="E2" s="172"/>
-      <c r="F2" s="172"/>
-      <c r="G2" s="172"/>
-      <c r="H2" s="172"/>
-      <c r="I2" s="172"/>
-      <c r="J2" s="172"/>
-      <c r="K2" s="173"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="179"/>
+      <c r="F2" s="179"/>
+      <c r="G2" s="179"/>
+      <c r="H2" s="179"/>
+      <c r="I2" s="179"/>
+      <c r="J2" s="179"/>
+      <c r="K2" s="180"/>
     </row>
     <row r="3" spans="1:11" ht="30">
       <c r="A3" s="10" t="s">
@@ -5574,48 +5574,48 @@
       <c r="C3" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="169"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="170"/>
-      <c r="H3" s="170"/>
-      <c r="I3" s="170"/>
-      <c r="J3" s="170"/>
-      <c r="K3" s="168"/>
+      <c r="D3" s="176"/>
+      <c r="E3" s="177"/>
+      <c r="F3" s="177"/>
+      <c r="G3" s="177"/>
+      <c r="H3" s="177"/>
+      <c r="I3" s="177"/>
+      <c r="J3" s="177"/>
+      <c r="K3" s="175"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="155" t="s">
+      <c r="A4" s="162" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="170" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="160" t="s">
+      <c r="C4" s="167" t="s">
         <v>304</v>
       </c>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
-      <c r="H4" s="161"/>
-      <c r="I4" s="161"/>
-      <c r="J4" s="162"/>
+      <c r="D4" s="168"/>
+      <c r="E4" s="168"/>
+      <c r="F4" s="168"/>
+      <c r="G4" s="168"/>
+      <c r="H4" s="168"/>
+      <c r="I4" s="168"/>
+      <c r="J4" s="169"/>
       <c r="K4" s="135"/>
     </row>
     <row r="5" spans="1:11" ht="30">
-      <c r="A5" s="156"/>
-      <c r="B5" s="164"/>
+      <c r="A5" s="163"/>
+      <c r="B5" s="171"/>
       <c r="C5" s="136" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="169"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="170"/>
-      <c r="H5" s="170"/>
-      <c r="I5" s="170"/>
-      <c r="J5" s="170"/>
-      <c r="K5" s="168"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="177"/>
+      <c r="F5" s="177"/>
+      <c r="G5" s="177"/>
+      <c r="H5" s="177"/>
+      <c r="I5" s="177"/>
+      <c r="J5" s="177"/>
+      <c r="K5" s="175"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="105" customHeight="1">
       <c r="A6" s="6" t="s">
@@ -5627,14 +5627,14 @@
       <c r="C6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="169"/>
-      <c r="E6" s="170"/>
-      <c r="F6" s="170"/>
-      <c r="G6" s="170"/>
-      <c r="H6" s="170"/>
-      <c r="I6" s="170"/>
-      <c r="J6" s="170"/>
-      <c r="K6" s="168"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="177"/>
+      <c r="F6" s="177"/>
+      <c r="G6" s="177"/>
+      <c r="H6" s="177"/>
+      <c r="I6" s="177"/>
+      <c r="J6" s="177"/>
+      <c r="K6" s="175"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="105" customHeight="1">
       <c r="A7" s="6" t="s">
@@ -5646,14 +5646,14 @@
       <c r="C7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="169"/>
-      <c r="E7" s="170"/>
-      <c r="F7" s="170"/>
-      <c r="G7" s="170"/>
-      <c r="H7" s="170"/>
-      <c r="I7" s="170"/>
-      <c r="J7" s="170"/>
-      <c r="K7" s="168"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="177"/>
+      <c r="F7" s="177"/>
+      <c r="G7" s="177"/>
+      <c r="H7" s="177"/>
+      <c r="I7" s="177"/>
+      <c r="J7" s="177"/>
+      <c r="K7" s="175"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="120" customHeight="1">
       <c r="A8" s="6" t="s">
@@ -5665,14 +5665,14 @@
       <c r="C8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="169"/>
-      <c r="E8" s="170"/>
-      <c r="F8" s="170"/>
-      <c r="G8" s="170"/>
-      <c r="H8" s="170"/>
-      <c r="I8" s="170"/>
-      <c r="J8" s="170"/>
-      <c r="K8" s="168"/>
+      <c r="D8" s="176"/>
+      <c r="E8" s="177"/>
+      <c r="F8" s="177"/>
+      <c r="G8" s="177"/>
+      <c r="H8" s="177"/>
+      <c r="I8" s="177"/>
+      <c r="J8" s="177"/>
+      <c r="K8" s="175"/>
     </row>
     <row r="9" spans="1:11" s="3" customFormat="1" ht="135" customHeight="1">
       <c r="A9" s="6" t="s">
@@ -5684,14 +5684,14 @@
       <c r="C9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="169"/>
-      <c r="E9" s="170"/>
-      <c r="F9" s="170"/>
-      <c r="G9" s="170"/>
-      <c r="H9" s="170"/>
-      <c r="I9" s="170"/>
-      <c r="J9" s="170"/>
-      <c r="K9" s="168"/>
+      <c r="D9" s="176"/>
+      <c r="E9" s="177"/>
+      <c r="F9" s="177"/>
+      <c r="G9" s="177"/>
+      <c r="H9" s="177"/>
+      <c r="I9" s="177"/>
+      <c r="J9" s="177"/>
+      <c r="K9" s="175"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="135" customHeight="1">
       <c r="A10" s="6" t="s">
@@ -5703,16 +5703,16 @@
       <c r="C10" s="81" t="s">
         <v>353</v>
       </c>
-      <c r="D10" s="169"/>
-      <c r="E10" s="170"/>
-      <c r="F10" s="170"/>
-      <c r="G10" s="170"/>
-      <c r="H10" s="168"/>
+      <c r="D10" s="176"/>
+      <c r="E10" s="177"/>
+      <c r="F10" s="177"/>
+      <c r="G10" s="177"/>
+      <c r="H10" s="175"/>
       <c r="I10" s="125" t="s">
         <v>352</v>
       </c>
-      <c r="J10" s="169"/>
-      <c r="K10" s="168"/>
+      <c r="J10" s="176"/>
+      <c r="K10" s="175"/>
     </row>
     <row r="11" spans="1:11" s="3" customFormat="1" ht="135" customHeight="1">
       <c r="A11" s="6" t="s">
@@ -5724,14 +5724,14 @@
       <c r="C11" s="87" t="s">
         <v>356</v>
       </c>
-      <c r="D11" s="169"/>
-      <c r="E11" s="170"/>
-      <c r="F11" s="170"/>
-      <c r="G11" s="170"/>
-      <c r="H11" s="170"/>
-      <c r="I11" s="170"/>
-      <c r="J11" s="170"/>
-      <c r="K11" s="168"/>
+      <c r="D11" s="176"/>
+      <c r="E11" s="177"/>
+      <c r="F11" s="177"/>
+      <c r="G11" s="177"/>
+      <c r="H11" s="177"/>
+      <c r="I11" s="177"/>
+      <c r="J11" s="177"/>
+      <c r="K11" s="175"/>
     </row>
     <row r="12" spans="1:11" s="3" customFormat="1" ht="135" customHeight="1">
       <c r="A12" s="6" t="s">
@@ -5740,36 +5740,36 @@
       <c r="B12" s="82" t="s">
         <v>340</v>
       </c>
-      <c r="C12" s="174"/>
-      <c r="D12" s="170"/>
-      <c r="E12" s="170"/>
-      <c r="F12" s="170"/>
-      <c r="G12" s="170"/>
-      <c r="H12" s="168"/>
+      <c r="C12" s="181"/>
+      <c r="D12" s="177"/>
+      <c r="E12" s="177"/>
+      <c r="F12" s="177"/>
+      <c r="G12" s="177"/>
+      <c r="H12" s="175"/>
       <c r="I12" s="125" t="s">
         <v>342</v>
       </c>
-      <c r="J12" s="169"/>
-      <c r="K12" s="168"/>
+      <c r="J12" s="176"/>
+      <c r="K12" s="175"/>
     </row>
     <row r="13" spans="1:11" s="3" customFormat="1" ht="180" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="138" t="s">
-        <v>500</v>
-      </c>
-      <c r="D13" s="169"/>
-      <c r="E13" s="170"/>
-      <c r="F13" s="170"/>
-      <c r="G13" s="170"/>
-      <c r="H13" s="170"/>
-      <c r="I13" s="170"/>
-      <c r="J13" s="170"/>
-      <c r="K13" s="168"/>
+        <v>497</v>
+      </c>
+      <c r="D13" s="176"/>
+      <c r="E13" s="177"/>
+      <c r="F13" s="177"/>
+      <c r="G13" s="177"/>
+      <c r="H13" s="177"/>
+      <c r="I13" s="177"/>
+      <c r="J13" s="177"/>
+      <c r="K13" s="175"/>
     </row>
     <row r="14" spans="1:11" s="3" customFormat="1" ht="90" customHeight="1">
       <c r="A14" s="6" t="s">
@@ -5781,52 +5781,52 @@
       <c r="C14" s="131" t="s">
         <v>269</v>
       </c>
-      <c r="D14" s="169"/>
-      <c r="E14" s="170"/>
-      <c r="F14" s="170"/>
-      <c r="G14" s="170"/>
-      <c r="H14" s="170"/>
-      <c r="I14" s="170"/>
-      <c r="J14" s="170"/>
-      <c r="K14" s="168"/>
+      <c r="D14" s="176"/>
+      <c r="E14" s="177"/>
+      <c r="F14" s="177"/>
+      <c r="G14" s="177"/>
+      <c r="H14" s="177"/>
+      <c r="I14" s="177"/>
+      <c r="J14" s="177"/>
+      <c r="K14" s="175"/>
     </row>
     <row r="15" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B15" s="133" t="s">
-        <v>505</v>
-      </c>
-      <c r="C15" s="160" t="s">
-        <v>506</v>
-      </c>
-      <c r="D15" s="161"/>
-      <c r="E15" s="161"/>
-      <c r="F15" s="161"/>
-      <c r="G15" s="161"/>
-      <c r="H15" s="161"/>
-      <c r="I15" s="161"/>
-      <c r="J15" s="161"/>
-      <c r="K15" s="162"/>
+        <v>502</v>
+      </c>
+      <c r="C15" s="167" t="s">
+        <v>503</v>
+      </c>
+      <c r="D15" s="168"/>
+      <c r="E15" s="168"/>
+      <c r="F15" s="168"/>
+      <c r="G15" s="168"/>
+      <c r="H15" s="168"/>
+      <c r="I15" s="168"/>
+      <c r="J15" s="168"/>
+      <c r="K15" s="169"/>
     </row>
     <row r="16" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A16" s="6" t="s">
         <v>109</v>
       </c>
       <c r="B16" s="133" t="s">
-        <v>503</v>
-      </c>
-      <c r="C16" s="160" t="s">
-        <v>501</v>
-      </c>
-      <c r="D16" s="161"/>
-      <c r="E16" s="161"/>
-      <c r="F16" s="161"/>
-      <c r="G16" s="161"/>
-      <c r="H16" s="161"/>
-      <c r="I16" s="161"/>
-      <c r="J16" s="161"/>
-      <c r="K16" s="162"/>
+        <v>500</v>
+      </c>
+      <c r="C16" s="167" t="s">
+        <v>498</v>
+      </c>
+      <c r="D16" s="168"/>
+      <c r="E16" s="168"/>
+      <c r="F16" s="168"/>
+      <c r="G16" s="168"/>
+      <c r="H16" s="168"/>
+      <c r="I16" s="168"/>
+      <c r="J16" s="168"/>
+      <c r="K16" s="169"/>
     </row>
     <row r="17" spans="1:11" s="3" customFormat="1" ht="150" customHeight="1">
       <c r="A17" s="6" t="s">
@@ -5838,14 +5838,14 @@
       <c r="C17" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="169"/>
-      <c r="E17" s="170"/>
-      <c r="F17" s="170"/>
-      <c r="G17" s="170"/>
-      <c r="H17" s="170"/>
-      <c r="I17" s="170"/>
-      <c r="J17" s="170"/>
-      <c r="K17" s="168"/>
+      <c r="D17" s="176"/>
+      <c r="E17" s="177"/>
+      <c r="F17" s="177"/>
+      <c r="G17" s="177"/>
+      <c r="H17" s="177"/>
+      <c r="I17" s="177"/>
+      <c r="J17" s="177"/>
+      <c r="K17" s="175"/>
     </row>
     <row r="18" spans="1:11" s="3" customFormat="1" ht="60" customHeight="1">
       <c r="A18" s="6" t="s">
@@ -5857,14 +5857,14 @@
       <c r="C18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="169"/>
-      <c r="E18" s="170"/>
-      <c r="F18" s="170"/>
-      <c r="G18" s="170"/>
-      <c r="H18" s="170"/>
-      <c r="I18" s="170"/>
-      <c r="J18" s="170"/>
-      <c r="K18" s="168"/>
+      <c r="D18" s="176"/>
+      <c r="E18" s="177"/>
+      <c r="F18" s="177"/>
+      <c r="G18" s="177"/>
+      <c r="H18" s="177"/>
+      <c r="I18" s="177"/>
+      <c r="J18" s="177"/>
+      <c r="K18" s="175"/>
     </row>
     <row r="19" spans="1:11" s="3" customFormat="1" ht="60" customHeight="1">
       <c r="A19" s="6" t="s">
@@ -5876,14 +5876,14 @@
       <c r="C19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="169"/>
-      <c r="E19" s="170"/>
-      <c r="F19" s="170"/>
-      <c r="G19" s="170"/>
-      <c r="H19" s="170"/>
-      <c r="I19" s="170"/>
-      <c r="J19" s="170"/>
-      <c r="K19" s="168"/>
+      <c r="D19" s="176"/>
+      <c r="E19" s="177"/>
+      <c r="F19" s="177"/>
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177"/>
+      <c r="J19" s="177"/>
+      <c r="K19" s="175"/>
     </row>
     <row r="20" spans="1:11" s="3" customFormat="1" ht="60" customHeight="1">
       <c r="A20" s="6" t="s">
@@ -5895,14 +5895,14 @@
       <c r="C20" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="169"/>
-      <c r="E20" s="170"/>
-      <c r="F20" s="170"/>
-      <c r="G20" s="170"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="170"/>
-      <c r="J20" s="170"/>
-      <c r="K20" s="168"/>
+      <c r="D20" s="176"/>
+      <c r="E20" s="177"/>
+      <c r="F20" s="177"/>
+      <c r="G20" s="177"/>
+      <c r="H20" s="177"/>
+      <c r="I20" s="177"/>
+      <c r="J20" s="177"/>
+      <c r="K20" s="175"/>
     </row>
     <row r="21" spans="1:11" s="51" customFormat="1" ht="225" customHeight="1">
       <c r="A21" s="52" t="s">
@@ -5914,14 +5914,14 @@
       <c r="C21" s="49" t="s">
         <v>309</v>
       </c>
-      <c r="D21" s="169"/>
-      <c r="E21" s="170"/>
-      <c r="F21" s="170"/>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170"/>
-      <c r="J21" s="170"/>
-      <c r="K21" s="168"/>
+      <c r="D21" s="176"/>
+      <c r="E21" s="177"/>
+      <c r="F21" s="177"/>
+      <c r="G21" s="177"/>
+      <c r="H21" s="177"/>
+      <c r="I21" s="177"/>
+      <c r="J21" s="177"/>
+      <c r="K21" s="175"/>
     </row>
     <row r="22" spans="1:11" s="51" customFormat="1" ht="225" customHeight="1">
       <c r="A22" s="62" t="s">
@@ -5933,18 +5933,18 @@
       <c r="C22" s="50" t="s">
         <v>206</v>
       </c>
-      <c r="D22" s="165"/>
-      <c r="E22" s="166"/>
-      <c r="F22" s="166"/>
-      <c r="G22" s="167"/>
+      <c r="D22" s="172"/>
+      <c r="E22" s="173"/>
+      <c r="F22" s="173"/>
+      <c r="G22" s="174"/>
       <c r="H22" s="19" t="s">
         <v>207</v>
       </c>
       <c r="I22" s="124" t="s">
-        <v>461</v>
-      </c>
-      <c r="J22" s="165"/>
-      <c r="K22" s="168"/>
+        <v>460</v>
+      </c>
+      <c r="J22" s="172"/>
+      <c r="K22" s="175"/>
     </row>
     <row r="23" spans="1:11" s="51" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="75" t="s">
@@ -5953,16 +5953,16 @@
       <c r="B23" s="71" t="s">
         <v>303</v>
       </c>
-      <c r="C23" s="160" t="s">
+      <c r="C23" s="167" t="s">
         <v>302</v>
       </c>
-      <c r="D23" s="161"/>
-      <c r="E23" s="161"/>
-      <c r="F23" s="161"/>
-      <c r="G23" s="161"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="161"/>
-      <c r="J23" s="162"/>
+      <c r="D23" s="168"/>
+      <c r="E23" s="168"/>
+      <c r="F23" s="168"/>
+      <c r="G23" s="168"/>
+      <c r="H23" s="168"/>
+      <c r="I23" s="168"/>
+      <c r="J23" s="169"/>
       <c r="K23" s="67"/>
     </row>
     <row r="24" spans="1:11" ht="60">
@@ -5972,16 +5972,16 @@
       <c r="B24" s="55" t="s">
         <v>270</v>
       </c>
-      <c r="C24" s="157" t="s">
+      <c r="C24" s="164" t="s">
         <v>271</v>
       </c>
-      <c r="D24" s="158"/>
-      <c r="E24" s="158"/>
-      <c r="F24" s="158"/>
-      <c r="G24" s="158"/>
-      <c r="H24" s="158"/>
-      <c r="I24" s="158"/>
-      <c r="J24" s="159"/>
+      <c r="D24" s="165"/>
+      <c r="E24" s="165"/>
+      <c r="F24" s="165"/>
+      <c r="G24" s="165"/>
+      <c r="H24" s="165"/>
+      <c r="I24" s="165"/>
+      <c r="J24" s="166"/>
       <c r="K24" s="64"/>
     </row>
   </sheetData>
@@ -6015,10 +6015,10 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="L42" sqref="L42"/>
+      <selection pane="bottomLeft" activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6034,10 +6034,10 @@
   <sheetData>
     <row r="1" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="18" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>373</v>
@@ -6064,10 +6064,10 @@
         <v>247</v>
       </c>
       <c r="K1" s="61" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="L1" s="61" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="16" customFormat="1" ht="30" customHeight="1">
@@ -6077,67 +6077,67 @@
       <c r="B2" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="221" t="s">
+      <c r="C2" s="222" t="s">
         <v>158</v>
       </c>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
-      <c r="G2" s="222"/>
-      <c r="H2" s="222"/>
-      <c r="I2" s="222"/>
-      <c r="J2" s="223"/>
-      <c r="K2" s="233"/>
-      <c r="L2" s="234"/>
+      <c r="D2" s="223"/>
+      <c r="E2" s="223"/>
+      <c r="F2" s="223"/>
+      <c r="G2" s="223"/>
+      <c r="H2" s="223"/>
+      <c r="I2" s="223"/>
+      <c r="J2" s="224"/>
+      <c r="K2" s="234"/>
+      <c r="L2" s="235"/>
     </row>
     <row r="3" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="155" t="s">
+      <c r="A3" s="162" t="s">
         <v>157</v>
       </c>
-      <c r="B3" s="163" t="s">
+      <c r="B3" s="170" t="s">
         <v>224</v>
       </c>
-      <c r="C3" s="160" t="s">
+      <c r="C3" s="167" t="s">
         <v>272</v>
       </c>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161"/>
-      <c r="F3" s="161"/>
-      <c r="G3" s="161"/>
-      <c r="H3" s="161"/>
-      <c r="I3" s="161"/>
-      <c r="J3" s="161"/>
-      <c r="K3" s="161"/>
-      <c r="L3" s="162"/>
+      <c r="D3" s="168"/>
+      <c r="E3" s="168"/>
+      <c r="F3" s="168"/>
+      <c r="G3" s="168"/>
+      <c r="H3" s="168"/>
+      <c r="I3" s="168"/>
+      <c r="J3" s="168"/>
+      <c r="K3" s="168"/>
+      <c r="L3" s="169"/>
     </row>
     <row r="4" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A4" s="175"/>
-      <c r="B4" s="176"/>
-      <c r="C4" s="160" t="s">
-        <v>481</v>
-      </c>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
-      <c r="H4" s="161"/>
-      <c r="I4" s="161"/>
-      <c r="J4" s="161"/>
-      <c r="K4" s="161"/>
-      <c r="L4" s="162"/>
+      <c r="A4" s="246"/>
+      <c r="B4" s="185"/>
+      <c r="C4" s="167" t="s">
+        <v>538</v>
+      </c>
+      <c r="D4" s="168"/>
+      <c r="E4" s="168"/>
+      <c r="F4" s="168"/>
+      <c r="G4" s="168"/>
+      <c r="H4" s="168"/>
+      <c r="I4" s="168"/>
+      <c r="J4" s="168"/>
+      <c r="K4" s="168"/>
+      <c r="L4" s="169"/>
     </row>
     <row r="5" spans="1:12" s="16" customFormat="1" ht="180">
-      <c r="A5" s="156"/>
-      <c r="B5" s="164"/>
+      <c r="A5" s="163"/>
+      <c r="B5" s="171"/>
       <c r="C5" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="D5" s="177" t="s">
-        <v>375</v>
-      </c>
-      <c r="E5" s="177"/>
-      <c r="F5" s="177"/>
-      <c r="G5" s="177"/>
+      <c r="D5" s="236" t="s">
+        <v>374</v>
+      </c>
+      <c r="E5" s="236"/>
+      <c r="F5" s="236"/>
+      <c r="G5" s="236"/>
       <c r="H5" s="38" t="s">
         <v>155</v>
       </c>
@@ -6146,7 +6146,7 @@
       </c>
       <c r="J5" s="56"/>
       <c r="K5" s="46" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="L5" s="46" t="s">
         <v>310</v>
@@ -6159,19 +6159,19 @@
       <c r="B6" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C6" s="160" t="s">
+      <c r="C6" s="167" t="s">
         <v>152</v>
       </c>
-      <c r="D6" s="161"/>
-      <c r="E6" s="161"/>
-      <c r="F6" s="161"/>
-      <c r="G6" s="161"/>
-      <c r="H6" s="161"/>
-      <c r="I6" s="161"/>
-      <c r="J6" s="162"/>
+      <c r="D6" s="168"/>
+      <c r="E6" s="168"/>
+      <c r="F6" s="168"/>
+      <c r="G6" s="168"/>
+      <c r="H6" s="168"/>
+      <c r="I6" s="168"/>
+      <c r="J6" s="169"/>
       <c r="K6" s="113"/>
       <c r="L6" s="85" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="16" customFormat="1" ht="90">
@@ -6182,22 +6182,22 @@
         <v>223</v>
       </c>
       <c r="C7" s="27"/>
-      <c r="D7" s="177" t="s">
+      <c r="D7" s="236" t="s">
         <v>151</v>
       </c>
-      <c r="E7" s="177"/>
-      <c r="F7" s="177"/>
-      <c r="G7" s="177"/>
+      <c r="E7" s="236"/>
+      <c r="F7" s="236"/>
+      <c r="G7" s="236"/>
       <c r="H7" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="I7" s="231"/>
-      <c r="J7" s="232"/>
+      <c r="I7" s="232"/>
+      <c r="J7" s="233"/>
       <c r="K7" s="46" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="L7" s="46" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="16" customFormat="1" ht="105" customHeight="1">
@@ -6207,16 +6207,16 @@
       <c r="B8" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="C8" s="179" t="s">
+      <c r="C8" s="237" t="s">
         <v>147</v>
       </c>
-      <c r="D8" s="180"/>
-      <c r="E8" s="180"/>
-      <c r="F8" s="180"/>
-      <c r="G8" s="180"/>
-      <c r="H8" s="180"/>
-      <c r="I8" s="180"/>
-      <c r="J8" s="181"/>
+      <c r="D8" s="238"/>
+      <c r="E8" s="238"/>
+      <c r="F8" s="238"/>
+      <c r="G8" s="238"/>
+      <c r="H8" s="238"/>
+      <c r="I8" s="238"/>
+      <c r="J8" s="239"/>
       <c r="K8" s="113"/>
       <c r="L8" s="85" t="s">
         <v>147</v>
@@ -6229,18 +6229,18 @@
       <c r="B9" s="48" t="s">
         <v>222</v>
       </c>
-      <c r="C9" s="162" t="s">
+      <c r="C9" s="169" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="177"/>
-      <c r="E9" s="177"/>
-      <c r="F9" s="177"/>
-      <c r="G9" s="177"/>
-      <c r="H9" s="177"/>
-      <c r="I9" s="177"/>
-      <c r="J9" s="177"/>
-      <c r="K9" s="177"/>
-      <c r="L9" s="177"/>
+      <c r="D9" s="236"/>
+      <c r="E9" s="236"/>
+      <c r="F9" s="236"/>
+      <c r="G9" s="236"/>
+      <c r="H9" s="236"/>
+      <c r="I9" s="236"/>
+      <c r="J9" s="236"/>
+      <c r="K9" s="236"/>
+      <c r="L9" s="236"/>
     </row>
     <row r="10" spans="1:12" ht="105" customHeight="1">
       <c r="A10" s="30" t="s">
@@ -6249,19 +6249,19 @@
       <c r="B10" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="C10" s="179" t="s">
+      <c r="C10" s="237" t="s">
         <v>143</v>
       </c>
-      <c r="D10" s="180"/>
-      <c r="E10" s="180"/>
-      <c r="F10" s="180"/>
-      <c r="G10" s="180"/>
-      <c r="H10" s="180"/>
-      <c r="I10" s="180"/>
-      <c r="J10" s="181"/>
+      <c r="D10" s="238"/>
+      <c r="E10" s="238"/>
+      <c r="F10" s="238"/>
+      <c r="G10" s="238"/>
+      <c r="H10" s="238"/>
+      <c r="I10" s="238"/>
+      <c r="J10" s="239"/>
       <c r="K10" s="84"/>
       <c r="L10" s="85" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="120" customHeight="1">
@@ -6271,21 +6271,21 @@
       <c r="B11" s="48" t="s">
         <v>225</v>
       </c>
-      <c r="C11" s="160" t="s">
+      <c r="C11" s="167" t="s">
         <v>313</v>
       </c>
-      <c r="D11" s="161"/>
-      <c r="E11" s="161"/>
-      <c r="F11" s="161"/>
-      <c r="G11" s="161"/>
-      <c r="H11" s="162"/>
-      <c r="I11" s="184"/>
-      <c r="J11" s="185"/>
+      <c r="D11" s="168"/>
+      <c r="E11" s="168"/>
+      <c r="F11" s="168"/>
+      <c r="G11" s="168"/>
+      <c r="H11" s="169"/>
+      <c r="I11" s="240"/>
+      <c r="J11" s="218"/>
       <c r="K11" s="77" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="L11" s="46" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="120" customHeight="1">
@@ -6293,19 +6293,19 @@
         <v>314</v>
       </c>
       <c r="B12" s="74"/>
-      <c r="C12" s="188"/>
-      <c r="D12" s="189"/>
-      <c r="E12" s="189"/>
-      <c r="F12" s="189"/>
-      <c r="G12" s="189"/>
-      <c r="H12" s="189"/>
-      <c r="I12" s="166"/>
-      <c r="J12" s="167"/>
+      <c r="C12" s="248"/>
+      <c r="D12" s="249"/>
+      <c r="E12" s="249"/>
+      <c r="F12" s="249"/>
+      <c r="G12" s="249"/>
+      <c r="H12" s="249"/>
+      <c r="I12" s="173"/>
+      <c r="J12" s="174"/>
       <c r="K12" s="41" t="s">
         <v>315</v>
       </c>
       <c r="L12" s="41" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="180" customHeight="1">
@@ -6335,8 +6335,8 @@
       <c r="J13" s="42" t="s">
         <v>349</v>
       </c>
-      <c r="K13" s="224"/>
-      <c r="L13" s="225"/>
+      <c r="K13" s="225"/>
+      <c r="L13" s="226"/>
     </row>
     <row r="14" spans="1:12" ht="135">
       <c r="A14" s="13" t="s">
@@ -6348,19 +6348,19 @@
       <c r="C14" s="12" t="s">
         <v>337</v>
       </c>
-      <c r="D14" s="165"/>
-      <c r="E14" s="170"/>
-      <c r="F14" s="166"/>
-      <c r="G14" s="166"/>
-      <c r="H14" s="166"/>
+      <c r="D14" s="172"/>
+      <c r="E14" s="177"/>
+      <c r="F14" s="173"/>
+      <c r="G14" s="173"/>
+      <c r="H14" s="173"/>
       <c r="I14" s="42" t="s">
         <v>343</v>
       </c>
       <c r="J14" s="42" t="s">
         <v>250</v>
       </c>
-      <c r="K14" s="226"/>
-      <c r="L14" s="227"/>
+      <c r="K14" s="227"/>
+      <c r="L14" s="228"/>
     </row>
     <row r="15" spans="1:12" ht="135">
       <c r="A15" s="13" t="s">
@@ -6376,7 +6376,7 @@
         <v>137</v>
       </c>
       <c r="E15" s="99" t="s">
-        <v>374</v>
+        <v>537</v>
       </c>
       <c r="F15" s="19" t="s">
         <v>136</v>
@@ -6393,21 +6393,21 @@
       <c r="J15" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="K15" s="226"/>
-      <c r="L15" s="227"/>
+      <c r="K15" s="227"/>
+      <c r="L15" s="228"/>
     </row>
     <row r="16" spans="1:12" ht="150" customHeight="1">
-      <c r="A16" s="178" t="s">
+      <c r="A16" s="247" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="190" t="s">
+      <c r="B16" s="209" t="s">
         <v>133</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>308</v>
       </c>
-      <c r="D16" s="182"/>
-      <c r="E16" s="183"/>
+      <c r="D16" s="211"/>
+      <c r="E16" s="212"/>
       <c r="F16" s="28" t="s">
         <v>307</v>
       </c>
@@ -6421,37 +6421,37 @@
       <c r="J16" s="44" t="s">
         <v>212</v>
       </c>
-      <c r="K16" s="226"/>
-      <c r="L16" s="227"/>
+      <c r="K16" s="227"/>
+      <c r="L16" s="228"/>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1">
-      <c r="A17" s="178"/>
-      <c r="B17" s="190"/>
-      <c r="C17" s="160" t="s">
+      <c r="A17" s="247"/>
+      <c r="B17" s="209"/>
+      <c r="C17" s="167" t="s">
         <v>132</v>
       </c>
-      <c r="D17" s="161"/>
-      <c r="E17" s="161"/>
-      <c r="F17" s="161"/>
-      <c r="G17" s="161"/>
-      <c r="H17" s="186"/>
-      <c r="I17" s="186"/>
-      <c r="J17" s="187"/>
-      <c r="K17" s="226"/>
-      <c r="L17" s="227"/>
+      <c r="D17" s="168"/>
+      <c r="E17" s="168"/>
+      <c r="F17" s="168"/>
+      <c r="G17" s="168"/>
+      <c r="H17" s="206"/>
+      <c r="I17" s="206"/>
+      <c r="J17" s="191"/>
+      <c r="K17" s="227"/>
+      <c r="L17" s="228"/>
     </row>
     <row r="18" spans="1:13" ht="135" customHeight="1">
-      <c r="A18" s="178" t="s">
+      <c r="A18" s="247" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="190" t="s">
+      <c r="B18" s="209" t="s">
         <v>131</v>
       </c>
       <c r="C18" s="91" t="s">
         <v>305</v>
       </c>
-      <c r="D18" s="182"/>
-      <c r="E18" s="183"/>
+      <c r="D18" s="211"/>
+      <c r="E18" s="212"/>
       <c r="F18" s="92" t="s">
         <v>306</v>
       </c>
@@ -6465,64 +6465,64 @@
       <c r="J18" s="44" t="s">
         <v>213</v>
       </c>
-      <c r="K18" s="228"/>
-      <c r="L18" s="229"/>
+      <c r="K18" s="229"/>
+      <c r="L18" s="230"/>
     </row>
     <row r="19" spans="1:13" ht="15" customHeight="1">
-      <c r="A19" s="178"/>
+      <c r="A19" s="247"/>
       <c r="B19" s="210"/>
-      <c r="C19" s="230" t="s">
+      <c r="C19" s="231" t="s">
         <v>130</v>
       </c>
-      <c r="D19" s="161"/>
-      <c r="E19" s="161"/>
-      <c r="F19" s="161"/>
-      <c r="G19" s="161"/>
-      <c r="H19" s="161"/>
-      <c r="I19" s="161"/>
-      <c r="J19" s="161"/>
-      <c r="K19" s="161"/>
-      <c r="L19" s="162"/>
+      <c r="D19" s="168"/>
+      <c r="E19" s="168"/>
+      <c r="F19" s="168"/>
+      <c r="G19" s="168"/>
+      <c r="H19" s="168"/>
+      <c r="I19" s="168"/>
+      <c r="J19" s="168"/>
+      <c r="K19" s="168"/>
+      <c r="L19" s="169"/>
     </row>
     <row r="20" spans="1:13" ht="15" customHeight="1">
-      <c r="A20" s="155" t="s">
+      <c r="A20" s="162" t="s">
         <v>267</v>
       </c>
-      <c r="B20" s="249" t="s">
+      <c r="B20" s="241" t="s">
         <v>268</v>
       </c>
-      <c r="C20" s="230" t="s">
-        <v>534</v>
-      </c>
-      <c r="D20" s="161"/>
-      <c r="E20" s="161"/>
-      <c r="F20" s="161"/>
-      <c r="G20" s="161"/>
-      <c r="H20" s="161"/>
-      <c r="I20" s="161"/>
-      <c r="J20" s="161"/>
-      <c r="K20" s="161"/>
-      <c r="L20" s="161"/>
-      <c r="M20" s="282"/>
+      <c r="C20" s="231" t="s">
+        <v>531</v>
+      </c>
+      <c r="D20" s="168"/>
+      <c r="E20" s="168"/>
+      <c r="F20" s="168"/>
+      <c r="G20" s="168"/>
+      <c r="H20" s="168"/>
+      <c r="I20" s="168"/>
+      <c r="J20" s="168"/>
+      <c r="K20" s="168"/>
+      <c r="L20" s="168"/>
+      <c r="M20" s="161"/>
     </row>
     <row r="21" spans="1:13" ht="105" customHeight="1">
-      <c r="A21" s="156"/>
-      <c r="B21" s="258"/>
-      <c r="C21" s="278" t="s">
-        <v>537</v>
-      </c>
-      <c r="D21" s="279"/>
-      <c r="E21" s="279"/>
-      <c r="F21" s="279"/>
-      <c r="G21" s="279"/>
-      <c r="H21" s="279"/>
-      <c r="I21" s="279"/>
-      <c r="J21" s="280"/>
+      <c r="A21" s="163"/>
+      <c r="B21" s="242"/>
+      <c r="C21" s="243" t="s">
+        <v>534</v>
+      </c>
+      <c r="D21" s="244"/>
+      <c r="E21" s="244"/>
+      <c r="F21" s="244"/>
+      <c r="G21" s="244"/>
+      <c r="H21" s="244"/>
+      <c r="I21" s="244"/>
+      <c r="J21" s="245"/>
       <c r="K21" s="44" t="s">
-        <v>536</v>
-      </c>
-      <c r="L21" s="281" t="s">
-        <v>535</v>
+        <v>533</v>
+      </c>
+      <c r="L21" s="160" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="105" customHeight="1">
@@ -6532,78 +6532,78 @@
       <c r="B22" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C22" s="160" t="s">
+      <c r="C22" s="167" t="s">
         <v>237</v>
       </c>
-      <c r="D22" s="161"/>
-      <c r="E22" s="161"/>
-      <c r="F22" s="161"/>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161"/>
-      <c r="J22" s="162"/>
+      <c r="D22" s="168"/>
+      <c r="E22" s="168"/>
+      <c r="F22" s="168"/>
+      <c r="G22" s="168"/>
+      <c r="H22" s="168"/>
+      <c r="I22" s="168"/>
+      <c r="J22" s="169"/>
       <c r="K22" s="43" t="s">
         <v>311</v>
       </c>
       <c r="L22" s="46" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="90" customHeight="1">
-      <c r="A23" s="192" t="s">
-        <v>388</v>
-      </c>
-      <c r="B23" s="163" t="s">
-        <v>393</v>
-      </c>
-      <c r="C23" s="160" t="s">
-        <v>390</v>
-      </c>
-      <c r="D23" s="161"/>
-      <c r="E23" s="161"/>
-      <c r="F23" s="161"/>
-      <c r="G23" s="161"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="161"/>
-      <c r="J23" s="162"/>
-      <c r="K23" s="187" t="s">
+      <c r="A23" s="186" t="s">
+        <v>387</v>
+      </c>
+      <c r="B23" s="170" t="s">
         <v>392</v>
       </c>
-      <c r="L23" s="187" t="s">
-        <v>409</v>
+      <c r="C23" s="167" t="s">
+        <v>389</v>
+      </c>
+      <c r="D23" s="168"/>
+      <c r="E23" s="168"/>
+      <c r="F23" s="168"/>
+      <c r="G23" s="168"/>
+      <c r="H23" s="168"/>
+      <c r="I23" s="168"/>
+      <c r="J23" s="169"/>
+      <c r="K23" s="191" t="s">
+        <v>391</v>
+      </c>
+      <c r="L23" s="191" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15" customHeight="1">
-      <c r="A24" s="193"/>
-      <c r="B24" s="176"/>
-      <c r="C24" s="160" t="s">
-        <v>389</v>
-      </c>
-      <c r="D24" s="161"/>
-      <c r="E24" s="161"/>
-      <c r="F24" s="161"/>
-      <c r="G24" s="161"/>
-      <c r="H24" s="161"/>
-      <c r="I24" s="161"/>
-      <c r="J24" s="162"/>
-      <c r="K24" s="197"/>
-      <c r="L24" s="197"/>
+      <c r="A24" s="187"/>
+      <c r="B24" s="185"/>
+      <c r="C24" s="167" t="s">
+        <v>388</v>
+      </c>
+      <c r="D24" s="168"/>
+      <c r="E24" s="168"/>
+      <c r="F24" s="168"/>
+      <c r="G24" s="168"/>
+      <c r="H24" s="168"/>
+      <c r="I24" s="168"/>
+      <c r="J24" s="169"/>
+      <c r="K24" s="192"/>
+      <c r="L24" s="192"/>
     </row>
     <row r="25" spans="1:13" ht="45" customHeight="1">
-      <c r="A25" s="194"/>
-      <c r="B25" s="164"/>
-      <c r="C25" s="160" t="s">
-        <v>391</v>
-      </c>
-      <c r="D25" s="161"/>
-      <c r="E25" s="161"/>
-      <c r="F25" s="161"/>
-      <c r="G25" s="161"/>
-      <c r="H25" s="161"/>
-      <c r="I25" s="161"/>
-      <c r="J25" s="162"/>
-      <c r="K25" s="198"/>
-      <c r="L25" s="198"/>
+      <c r="A25" s="188"/>
+      <c r="B25" s="171"/>
+      <c r="C25" s="167" t="s">
+        <v>390</v>
+      </c>
+      <c r="D25" s="168"/>
+      <c r="E25" s="168"/>
+      <c r="F25" s="168"/>
+      <c r="G25" s="168"/>
+      <c r="H25" s="168"/>
+      <c r="I25" s="168"/>
+      <c r="J25" s="169"/>
+      <c r="K25" s="193"/>
+      <c r="L25" s="193"/>
     </row>
     <row r="26" spans="1:13" ht="30" customHeight="1">
       <c r="A26" s="13" t="s">
@@ -6612,18 +6612,18 @@
       <c r="B26" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="C26" s="195" t="s">
+      <c r="C26" s="189" t="s">
         <v>125</v>
       </c>
-      <c r="D26" s="196"/>
-      <c r="E26" s="196"/>
-      <c r="F26" s="196"/>
-      <c r="G26" s="196"/>
-      <c r="H26" s="196"/>
-      <c r="I26" s="196"/>
-      <c r="J26" s="196"/>
-      <c r="K26" s="196"/>
-      <c r="L26" s="196"/>
+      <c r="D26" s="190"/>
+      <c r="E26" s="190"/>
+      <c r="F26" s="190"/>
+      <c r="G26" s="190"/>
+      <c r="H26" s="190"/>
+      <c r="I26" s="190"/>
+      <c r="J26" s="190"/>
+      <c r="K26" s="190"/>
+      <c r="L26" s="190"/>
     </row>
     <row r="27" spans="1:13" ht="30" customHeight="1">
       <c r="A27" s="10" t="s">
@@ -6632,18 +6632,18 @@
       <c r="B27" s="101" t="s">
         <v>123</v>
       </c>
-      <c r="C27" s="195" t="s">
+      <c r="C27" s="189" t="s">
         <v>122</v>
       </c>
-      <c r="D27" s="196"/>
-      <c r="E27" s="196"/>
-      <c r="F27" s="196"/>
-      <c r="G27" s="196"/>
-      <c r="H27" s="196"/>
-      <c r="I27" s="196"/>
-      <c r="J27" s="196"/>
-      <c r="K27" s="196"/>
-      <c r="L27" s="196"/>
+      <c r="D27" s="190"/>
+      <c r="E27" s="190"/>
+      <c r="F27" s="190"/>
+      <c r="G27" s="190"/>
+      <c r="H27" s="190"/>
+      <c r="I27" s="190"/>
+      <c r="J27" s="190"/>
+      <c r="K27" s="190"/>
+      <c r="L27" s="190"/>
     </row>
     <row r="28" spans="1:13" ht="30" customHeight="1">
       <c r="A28" s="10" t="s">
@@ -6652,18 +6652,18 @@
       <c r="B28" s="101" t="s">
         <v>173</v>
       </c>
-      <c r="C28" s="195" t="s">
+      <c r="C28" s="189" t="s">
         <v>174</v>
       </c>
-      <c r="D28" s="196"/>
-      <c r="E28" s="196"/>
-      <c r="F28" s="196"/>
-      <c r="G28" s="196"/>
-      <c r="H28" s="196"/>
-      <c r="I28" s="196"/>
-      <c r="J28" s="196"/>
-      <c r="K28" s="196"/>
-      <c r="L28" s="196"/>
+      <c r="D28" s="190"/>
+      <c r="E28" s="190"/>
+      <c r="F28" s="190"/>
+      <c r="G28" s="190"/>
+      <c r="H28" s="190"/>
+      <c r="I28" s="190"/>
+      <c r="J28" s="190"/>
+      <c r="K28" s="190"/>
+      <c r="L28" s="190"/>
     </row>
     <row r="29" spans="1:13" ht="30" customHeight="1">
       <c r="A29" s="10" t="s">
@@ -6672,18 +6672,18 @@
       <c r="B29" s="101" t="s">
         <v>120</v>
       </c>
-      <c r="C29" s="195" t="s">
+      <c r="C29" s="189" t="s">
         <v>119</v>
       </c>
-      <c r="D29" s="196"/>
-      <c r="E29" s="196"/>
-      <c r="F29" s="196"/>
-      <c r="G29" s="196"/>
-      <c r="H29" s="196"/>
-      <c r="I29" s="196"/>
-      <c r="J29" s="196"/>
-      <c r="K29" s="196"/>
-      <c r="L29" s="196"/>
+      <c r="D29" s="190"/>
+      <c r="E29" s="190"/>
+      <c r="F29" s="190"/>
+      <c r="G29" s="190"/>
+      <c r="H29" s="190"/>
+      <c r="I29" s="190"/>
+      <c r="J29" s="190"/>
+      <c r="K29" s="190"/>
+      <c r="L29" s="190"/>
     </row>
     <row r="30" spans="1:13" ht="30" customHeight="1">
       <c r="A30" s="10" t="s">
@@ -6692,18 +6692,18 @@
       <c r="B30" s="101" t="s">
         <v>176</v>
       </c>
-      <c r="C30" s="195" t="s">
+      <c r="C30" s="189" t="s">
         <v>177</v>
       </c>
-      <c r="D30" s="196"/>
-      <c r="E30" s="196"/>
-      <c r="F30" s="196"/>
-      <c r="G30" s="196"/>
-      <c r="H30" s="196"/>
-      <c r="I30" s="196"/>
-      <c r="J30" s="196"/>
-      <c r="K30" s="196"/>
-      <c r="L30" s="196"/>
+      <c r="D30" s="190"/>
+      <c r="E30" s="190"/>
+      <c r="F30" s="190"/>
+      <c r="G30" s="190"/>
+      <c r="H30" s="190"/>
+      <c r="I30" s="190"/>
+      <c r="J30" s="190"/>
+      <c r="K30" s="190"/>
+      <c r="L30" s="190"/>
     </row>
     <row r="31" spans="1:13" ht="30" customHeight="1">
       <c r="A31" s="10" t="s">
@@ -6712,18 +6712,18 @@
       <c r="B31" s="101" t="s">
         <v>117</v>
       </c>
-      <c r="C31" s="195" t="s">
+      <c r="C31" s="189" t="s">
         <v>116</v>
       </c>
-      <c r="D31" s="196"/>
-      <c r="E31" s="196"/>
-      <c r="F31" s="196"/>
-      <c r="G31" s="196"/>
-      <c r="H31" s="196"/>
-      <c r="I31" s="196"/>
-      <c r="J31" s="196"/>
-      <c r="K31" s="196"/>
-      <c r="L31" s="196"/>
+      <c r="D31" s="190"/>
+      <c r="E31" s="190"/>
+      <c r="F31" s="190"/>
+      <c r="G31" s="190"/>
+      <c r="H31" s="190"/>
+      <c r="I31" s="190"/>
+      <c r="J31" s="190"/>
+      <c r="K31" s="190"/>
+      <c r="L31" s="190"/>
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1">
       <c r="A32" s="10" t="s">
@@ -6732,38 +6732,38 @@
       <c r="B32" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="C32" s="195" t="s">
+      <c r="C32" s="189" t="s">
         <v>113</v>
       </c>
-      <c r="D32" s="196"/>
-      <c r="E32" s="196"/>
-      <c r="F32" s="196"/>
-      <c r="G32" s="196"/>
-      <c r="H32" s="196"/>
-      <c r="I32" s="196"/>
-      <c r="J32" s="196"/>
-      <c r="K32" s="196"/>
-      <c r="L32" s="196"/>
+      <c r="D32" s="190"/>
+      <c r="E32" s="190"/>
+      <c r="F32" s="190"/>
+      <c r="G32" s="190"/>
+      <c r="H32" s="190"/>
+      <c r="I32" s="190"/>
+      <c r="J32" s="190"/>
+      <c r="K32" s="190"/>
+      <c r="L32" s="190"/>
     </row>
     <row r="33" spans="1:13" ht="75" customHeight="1">
-      <c r="A33" s="276" t="s">
+      <c r="A33" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="B33" s="277" t="s">
+      <c r="B33" s="159" t="s">
         <v>111</v>
       </c>
       <c r="C33" s="151" t="s">
         <v>179</v>
       </c>
-      <c r="D33" s="268"/>
+      <c r="D33" s="156"/>
       <c r="E33" s="152" t="s">
         <v>110</v>
       </c>
       <c r="F33" s="153" t="s">
         <v>180</v>
       </c>
-      <c r="G33" s="182"/>
-      <c r="H33" s="183"/>
+      <c r="G33" s="211"/>
+      <c r="H33" s="212"/>
       <c r="I33" s="152" t="s">
         <v>324</v>
       </c>
@@ -6774,67 +6774,67 @@
         <v>211</v>
       </c>
       <c r="L33" s="42" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="75" customHeight="1">
-      <c r="A34" s="275" t="s">
+      <c r="A34" s="157" t="s">
+        <v>524</v>
+      </c>
+      <c r="B34" s="154" t="s">
+        <v>525</v>
+      </c>
+      <c r="C34" s="192" t="s">
+        <v>529</v>
+      </c>
+      <c r="D34" s="197"/>
+      <c r="E34" s="197"/>
+      <c r="F34" s="197"/>
+      <c r="G34" s="197"/>
+      <c r="H34" s="197"/>
+      <c r="I34" s="197"/>
+      <c r="J34" s="99" t="s">
+        <v>528</v>
+      </c>
+      <c r="K34" s="119" t="s">
         <v>527</v>
       </c>
-      <c r="B34" s="154" t="s">
-        <v>528</v>
-      </c>
-      <c r="C34" s="197" t="s">
-        <v>532</v>
-      </c>
-      <c r="D34" s="274"/>
-      <c r="E34" s="274"/>
-      <c r="F34" s="274"/>
-      <c r="G34" s="274"/>
-      <c r="H34" s="274"/>
-      <c r="I34" s="274"/>
-      <c r="J34" s="99" t="s">
-        <v>531</v>
-      </c>
-      <c r="K34" s="119" t="s">
-        <v>530</v>
-      </c>
-      <c r="L34" s="267" t="s">
-        <v>529</v>
+      <c r="L34" s="155" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="35" spans="1:13" s="68" customFormat="1" ht="15" customHeight="1">
-      <c r="A35" s="269" t="s">
+      <c r="A35" s="182" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="270" t="s">
+      <c r="B35" s="184" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="271" t="s">
-        <v>402</v>
-      </c>
-      <c r="D35" s="272"/>
-      <c r="E35" s="272"/>
-      <c r="F35" s="272"/>
-      <c r="G35" s="272"/>
-      <c r="H35" s="272"/>
-      <c r="I35" s="272"/>
-      <c r="J35" s="272"/>
-      <c r="K35" s="272"/>
-      <c r="L35" s="273"/>
+      <c r="C35" s="194" t="s">
+        <v>401</v>
+      </c>
+      <c r="D35" s="195"/>
+      <c r="E35" s="195"/>
+      <c r="F35" s="195"/>
+      <c r="G35" s="195"/>
+      <c r="H35" s="195"/>
+      <c r="I35" s="195"/>
+      <c r="J35" s="195"/>
+      <c r="K35" s="195"/>
+      <c r="L35" s="196"/>
     </row>
     <row r="36" spans="1:13" ht="345" customHeight="1">
-      <c r="A36" s="191"/>
-      <c r="B36" s="176"/>
+      <c r="A36" s="183"/>
+      <c r="B36" s="185"/>
       <c r="C36" s="114" t="s">
         <v>229</v>
       </c>
       <c r="D36" s="99" t="s">
-        <v>401</v>
-      </c>
-      <c r="E36" s="169"/>
-      <c r="F36" s="170"/>
-      <c r="G36" s="168"/>
+        <v>400</v>
+      </c>
+      <c r="E36" s="176"/>
+      <c r="F36" s="177"/>
+      <c r="G36" s="175"/>
       <c r="H36" s="115" t="s">
         <v>230</v>
       </c>
@@ -6848,7 +6848,7 @@
         <v>261</v>
       </c>
       <c r="L36" s="42" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="45" customHeight="1">
@@ -6856,20 +6856,20 @@
         <v>109</v>
       </c>
       <c r="B37" s="130" t="s">
-        <v>502</v>
-      </c>
-      <c r="C37" s="205" t="s">
+        <v>499</v>
+      </c>
+      <c r="C37" s="204" t="s">
         <v>108</v>
       </c>
-      <c r="D37" s="207"/>
-      <c r="E37" s="207"/>
-      <c r="F37" s="207"/>
-      <c r="G37" s="207"/>
-      <c r="H37" s="207"/>
-      <c r="I37" s="207"/>
-      <c r="J37" s="207"/>
-      <c r="K37" s="207"/>
-      <c r="L37" s="198"/>
+      <c r="D37" s="205"/>
+      <c r="E37" s="205"/>
+      <c r="F37" s="205"/>
+      <c r="G37" s="205"/>
+      <c r="H37" s="205"/>
+      <c r="I37" s="205"/>
+      <c r="J37" s="205"/>
+      <c r="K37" s="205"/>
+      <c r="L37" s="193"/>
     </row>
     <row r="38" spans="1:13" ht="45" customHeight="1">
       <c r="A38" s="129" t="s">
@@ -6878,41 +6878,41 @@
       <c r="B38" s="130" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="204" t="s">
-        <v>455</v>
-      </c>
-      <c r="D38" s="186"/>
-      <c r="E38" s="186"/>
-      <c r="F38" s="186"/>
-      <c r="G38" s="186"/>
-      <c r="H38" s="186"/>
-      <c r="I38" s="186"/>
-      <c r="J38" s="186"/>
-      <c r="K38" s="186"/>
-      <c r="L38" s="187"/>
+      <c r="C38" s="203" t="s">
+        <v>454</v>
+      </c>
+      <c r="D38" s="206"/>
+      <c r="E38" s="206"/>
+      <c r="F38" s="206"/>
+      <c r="G38" s="206"/>
+      <c r="H38" s="206"/>
+      <c r="I38" s="206"/>
+      <c r="J38" s="206"/>
+      <c r="K38" s="206"/>
+      <c r="L38" s="191"/>
     </row>
     <row r="39" spans="1:13" ht="60" customHeight="1">
       <c r="A39" s="127" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B39" s="128" t="s">
-        <v>508</v>
-      </c>
-      <c r="C39" s="160" t="s">
-        <v>454</v>
-      </c>
-      <c r="D39" s="161"/>
-      <c r="E39" s="161"/>
-      <c r="F39" s="161"/>
-      <c r="G39" s="161"/>
-      <c r="H39" s="161"/>
-      <c r="I39" s="161"/>
-      <c r="J39" s="162"/>
+        <v>505</v>
+      </c>
+      <c r="C39" s="167" t="s">
+        <v>453</v>
+      </c>
+      <c r="D39" s="168"/>
+      <c r="E39" s="168"/>
+      <c r="F39" s="168"/>
+      <c r="G39" s="168"/>
+      <c r="H39" s="168"/>
+      <c r="I39" s="168"/>
+      <c r="J39" s="169"/>
       <c r="K39" s="122" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="L39" s="122" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="105" customHeight="1">
@@ -6925,22 +6925,22 @@
       <c r="C40" s="37" t="s">
         <v>345</v>
       </c>
-      <c r="D40" s="182"/>
-      <c r="E40" s="183"/>
+      <c r="D40" s="211"/>
+      <c r="E40" s="212"/>
       <c r="F40" s="29" t="s">
         <v>103</v>
       </c>
       <c r="G40" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="H40" s="211"/>
+      <c r="H40" s="213"/>
       <c r="I40" s="80" t="s">
         <v>344</v>
       </c>
-      <c r="J40" s="208"/>
-      <c r="K40" s="209"/>
+      <c r="J40" s="207"/>
+      <c r="K40" s="208"/>
       <c r="L40" s="103" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="90">
@@ -6960,12 +6960,12 @@
         <v>97</v>
       </c>
       <c r="F41" s="23" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="G41" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="H41" s="212"/>
+      <c r="H41" s="214"/>
       <c r="I41" s="83" t="s">
         <v>327</v>
       </c>
@@ -6985,18 +6985,18 @@
       <c r="C42" s="215" t="s">
         <v>189</v>
       </c>
-      <c r="D42" s="203"/>
-      <c r="E42" s="203"/>
-      <c r="F42" s="203"/>
-      <c r="G42" s="203"/>
-      <c r="H42" s="195"/>
+      <c r="D42" s="202"/>
+      <c r="E42" s="202"/>
+      <c r="F42" s="202"/>
+      <c r="G42" s="202"/>
+      <c r="H42" s="189"/>
       <c r="I42" s="217"/>
-      <c r="J42" s="185"/>
+      <c r="J42" s="218"/>
       <c r="K42" s="77" t="s">
         <v>216</v>
       </c>
       <c r="L42" s="103" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="75" customHeight="1">
@@ -7009,18 +7009,18 @@
       <c r="C43" s="215" t="s">
         <v>220</v>
       </c>
-      <c r="D43" s="203"/>
-      <c r="E43" s="203"/>
-      <c r="F43" s="203"/>
-      <c r="G43" s="203"/>
-      <c r="H43" s="195"/>
-      <c r="I43" s="169"/>
-      <c r="J43" s="168"/>
+      <c r="D43" s="202"/>
+      <c r="E43" s="202"/>
+      <c r="F43" s="202"/>
+      <c r="G43" s="202"/>
+      <c r="H43" s="189"/>
+      <c r="I43" s="176"/>
+      <c r="J43" s="175"/>
       <c r="K43" s="77" t="s">
         <v>219</v>
       </c>
       <c r="L43" s="103" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="120">
@@ -7030,14 +7030,14 @@
       <c r="B44" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="C44" s="203" t="s">
+      <c r="C44" s="202" t="s">
         <v>186</v>
       </c>
-      <c r="D44" s="203"/>
-      <c r="E44" s="203"/>
-      <c r="F44" s="203"/>
-      <c r="G44" s="203"/>
-      <c r="H44" s="203"/>
+      <c r="D44" s="202"/>
+      <c r="E44" s="202"/>
+      <c r="F44" s="202"/>
+      <c r="G44" s="202"/>
+      <c r="H44" s="202"/>
       <c r="I44" s="44" t="s">
         <v>323</v>
       </c>
@@ -7046,7 +7046,7 @@
         <v>252</v>
       </c>
       <c r="L44" s="42" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="300" customHeight="1">
@@ -7063,24 +7063,24 @@
         <v>359</v>
       </c>
       <c r="E45" s="32" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F45" s="32" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G45" s="32" t="s">
         <v>92</v>
       </c>
       <c r="H45" s="79" t="s">
-        <v>420</v>
-      </c>
-      <c r="I45" s="169"/>
-      <c r="J45" s="168"/>
+        <v>419</v>
+      </c>
+      <c r="I45" s="176"/>
+      <c r="J45" s="175"/>
       <c r="K45" s="42" t="s">
         <v>236</v>
       </c>
       <c r="L45" s="42" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="285">
@@ -7095,22 +7095,22 @@
       </c>
       <c r="D46" s="45"/>
       <c r="E46" s="100" t="s">
+        <v>416</v>
+      </c>
+      <c r="F46" s="19" t="s">
         <v>417</v>
       </c>
-      <c r="F46" s="19" t="s">
+      <c r="G46" s="19" t="s">
         <v>418</v>
       </c>
-      <c r="G46" s="19" t="s">
-        <v>419</v>
-      </c>
-      <c r="H46" s="169"/>
-      <c r="I46" s="170"/>
-      <c r="J46" s="168"/>
+      <c r="H46" s="176"/>
+      <c r="I46" s="177"/>
+      <c r="J46" s="175"/>
       <c r="K46" s="42" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="L46" s="42" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="240">
@@ -7120,15 +7120,15 @@
       <c r="B47" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="C47" s="219"/>
-      <c r="D47" s="170"/>
+      <c r="C47" s="220"/>
+      <c r="D47" s="177"/>
       <c r="E47" s="44" t="s">
         <v>232</v>
       </c>
-      <c r="F47" s="169"/>
-      <c r="G47" s="170"/>
-      <c r="H47" s="170"/>
-      <c r="I47" s="168"/>
+      <c r="F47" s="176"/>
+      <c r="G47" s="177"/>
+      <c r="H47" s="177"/>
+      <c r="I47" s="175"/>
       <c r="J47" s="42" t="s">
         <v>231</v>
       </c>
@@ -7147,10 +7147,10 @@
       <c r="C48" s="35" t="s">
         <v>320</v>
       </c>
-      <c r="D48" s="165"/>
-      <c r="E48" s="166"/>
-      <c r="F48" s="166"/>
-      <c r="G48" s="167"/>
+      <c r="D48" s="172"/>
+      <c r="E48" s="173"/>
+      <c r="F48" s="173"/>
+      <c r="G48" s="174"/>
       <c r="H48" s="19" t="s">
         <v>178</v>
       </c>
@@ -7164,29 +7164,29 @@
         <v>253</v>
       </c>
       <c r="L48" s="102" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="M48" s="7"/>
     </row>
     <row r="49" spans="1:12" ht="210" customHeight="1">
-      <c r="A49" s="199" t="s">
+      <c r="A49" s="198" t="s">
         <v>84</v>
       </c>
-      <c r="B49" s="201" t="s">
+      <c r="B49" s="200" t="s">
         <v>83</v>
       </c>
       <c r="C49" s="215" t="s">
         <v>319</v>
       </c>
-      <c r="D49" s="203"/>
+      <c r="D49" s="202"/>
       <c r="E49" s="44" t="s">
         <v>321</v>
       </c>
-      <c r="F49" s="203" t="s">
+      <c r="F49" s="202" t="s">
         <v>318</v>
       </c>
-      <c r="G49" s="203"/>
-      <c r="H49" s="195"/>
+      <c r="G49" s="202"/>
+      <c r="H49" s="189"/>
       <c r="I49" s="42" t="s">
         <v>325</v>
       </c>
@@ -7199,44 +7199,44 @@
       <c r="L49" s="11"/>
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1">
-      <c r="A50" s="200"/>
-      <c r="B50" s="202"/>
-      <c r="C50" s="160" t="s">
+      <c r="A50" s="199"/>
+      <c r="B50" s="201"/>
+      <c r="C50" s="167" t="s">
         <v>82</v>
       </c>
-      <c r="D50" s="161"/>
-      <c r="E50" s="161"/>
-      <c r="F50" s="161"/>
-      <c r="G50" s="161"/>
-      <c r="H50" s="161"/>
-      <c r="I50" s="161"/>
-      <c r="J50" s="161"/>
-      <c r="K50" s="161"/>
-      <c r="L50" s="162"/>
+      <c r="D50" s="168"/>
+      <c r="E50" s="168"/>
+      <c r="F50" s="168"/>
+      <c r="G50" s="168"/>
+      <c r="H50" s="168"/>
+      <c r="I50" s="168"/>
+      <c r="J50" s="168"/>
+      <c r="K50" s="168"/>
+      <c r="L50" s="169"/>
     </row>
     <row r="51" spans="1:12" ht="15" customHeight="1">
-      <c r="A51" s="199" t="s">
+      <c r="A51" s="198" t="s">
         <v>190</v>
       </c>
-      <c r="B51" s="201" t="s">
+      <c r="B51" s="200" t="s">
         <v>198</v>
       </c>
-      <c r="C51" s="205" t="s">
+      <c r="C51" s="204" t="s">
         <v>192</v>
       </c>
-      <c r="D51" s="207"/>
-      <c r="E51" s="207"/>
-      <c r="F51" s="207"/>
-      <c r="G51" s="207"/>
-      <c r="H51" s="207"/>
-      <c r="I51" s="207"/>
-      <c r="J51" s="207"/>
-      <c r="K51" s="207"/>
-      <c r="L51" s="198"/>
+      <c r="D51" s="205"/>
+      <c r="E51" s="205"/>
+      <c r="F51" s="205"/>
+      <c r="G51" s="205"/>
+      <c r="H51" s="205"/>
+      <c r="I51" s="205"/>
+      <c r="J51" s="205"/>
+      <c r="K51" s="205"/>
+      <c r="L51" s="193"/>
     </row>
     <row r="52" spans="1:12" ht="285" customHeight="1">
-      <c r="A52" s="200"/>
-      <c r="B52" s="205"/>
+      <c r="A52" s="199"/>
+      <c r="B52" s="204"/>
       <c r="C52" s="37" t="s">
         <v>193</v>
       </c>
@@ -7258,12 +7258,12 @@
       <c r="I52" s="44" t="s">
         <v>329</v>
       </c>
-      <c r="J52" s="211"/>
+      <c r="J52" s="213"/>
       <c r="K52" s="42" t="s">
         <v>228</v>
       </c>
       <c r="L52" s="42" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="352.5" customHeight="1">
@@ -7294,12 +7294,12 @@
       <c r="I53" s="44" t="s">
         <v>331</v>
       </c>
-      <c r="J53" s="212"/>
+      <c r="J53" s="214"/>
       <c r="K53" s="42" t="s">
         <v>330</v>
       </c>
       <c r="L53" s="42" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="135" customHeight="1">
@@ -7316,7 +7316,7 @@
         <v>78</v>
       </c>
       <c r="E54" s="32" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F54" s="32" t="s">
         <v>77</v>
@@ -7335,32 +7335,32 @@
         <v>256</v>
       </c>
       <c r="L54" s="36" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="30" customHeight="1">
-      <c r="A55" s="199" t="s">
+      <c r="A55" s="198" t="s">
         <v>75</v>
       </c>
-      <c r="B55" s="204" t="s">
+      <c r="B55" s="203" t="s">
         <v>74</v>
       </c>
-      <c r="C55" s="218" t="s">
-        <v>427</v>
-      </c>
-      <c r="D55" s="196"/>
-      <c r="E55" s="196"/>
-      <c r="F55" s="196"/>
-      <c r="G55" s="196"/>
-      <c r="H55" s="196"/>
-      <c r="I55" s="196"/>
-      <c r="J55" s="196"/>
-      <c r="K55" s="196"/>
-      <c r="L55" s="196"/>
+      <c r="C55" s="219" t="s">
+        <v>426</v>
+      </c>
+      <c r="D55" s="190"/>
+      <c r="E55" s="190"/>
+      <c r="F55" s="190"/>
+      <c r="G55" s="190"/>
+      <c r="H55" s="190"/>
+      <c r="I55" s="190"/>
+      <c r="J55" s="190"/>
+      <c r="K55" s="190"/>
+      <c r="L55" s="190"/>
     </row>
     <row r="56" spans="1:12" ht="195" customHeight="1">
-      <c r="A56" s="200"/>
-      <c r="B56" s="202"/>
+      <c r="A56" s="199"/>
+      <c r="B56" s="201"/>
       <c r="C56" s="114" t="s">
         <v>241</v>
       </c>
@@ -7385,45 +7385,45 @@
       </c>
       <c r="K56" s="117"/>
       <c r="L56" s="119" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="30" customHeight="1">
-      <c r="A57" s="199" t="s">
+      <c r="A57" s="198" t="s">
         <v>73</v>
       </c>
-      <c r="B57" s="204" t="s">
+      <c r="B57" s="203" t="s">
         <v>72</v>
       </c>
-      <c r="C57" s="218" t="s">
-        <v>428</v>
-      </c>
-      <c r="D57" s="196"/>
-      <c r="E57" s="196"/>
-      <c r="F57" s="196"/>
-      <c r="G57" s="196"/>
-      <c r="H57" s="196"/>
-      <c r="I57" s="196"/>
-      <c r="J57" s="196"/>
-      <c r="K57" s="196"/>
-      <c r="L57" s="196"/>
+      <c r="C57" s="219" t="s">
+        <v>427</v>
+      </c>
+      <c r="D57" s="190"/>
+      <c r="E57" s="190"/>
+      <c r="F57" s="190"/>
+      <c r="G57" s="190"/>
+      <c r="H57" s="190"/>
+      <c r="I57" s="190"/>
+      <c r="J57" s="190"/>
+      <c r="K57" s="190"/>
+      <c r="L57" s="190"/>
     </row>
     <row r="58" spans="1:12" ht="326.25" customHeight="1">
-      <c r="A58" s="200"/>
-      <c r="B58" s="202"/>
+      <c r="A58" s="199"/>
+      <c r="B58" s="201"/>
       <c r="C58" s="120" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="D58" s="14"/>
       <c r="E58" s="139" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="F58" s="139" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="G58" s="14"/>
       <c r="H58" s="36" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="I58" s="109"/>
       <c r="J58" s="118"/>
@@ -7431,7 +7431,7 @@
         <v>238</v>
       </c>
       <c r="L58" s="97" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="195" customHeight="1">
@@ -7459,7 +7459,7 @@
       <c r="H59" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="I59" s="220"/>
+      <c r="I59" s="221"/>
       <c r="J59" s="42" t="s">
         <v>258</v>
       </c>
@@ -7467,7 +7467,7 @@
         <v>257</v>
       </c>
       <c r="L59" s="42" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="105" customHeight="1">
@@ -7495,7 +7495,7 @@
       <c r="H60" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="I60" s="212"/>
+      <c r="I60" s="214"/>
       <c r="J60" s="42" t="s">
         <v>260</v>
       </c>
@@ -7503,7 +7503,7 @@
         <v>259</v>
       </c>
       <c r="L60" s="42" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="360">
@@ -7522,15 +7522,15 @@
       <c r="E61" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="F61" s="165"/>
-      <c r="G61" s="167"/>
+      <c r="F61" s="172"/>
+      <c r="G61" s="174"/>
       <c r="H61" s="25" t="s">
         <v>181</v>
       </c>
       <c r="I61" s="78" t="s">
         <v>333</v>
       </c>
-      <c r="J61" s="211"/>
+      <c r="J61" s="213"/>
       <c r="K61" s="8" t="s">
         <v>334</v>
       </c>
@@ -7564,27 +7564,43 @@
       <c r="I62" s="44" t="s">
         <v>341</v>
       </c>
-      <c r="J62" s="212"/>
+      <c r="J62" s="214"/>
       <c r="K62" s="42" t="s">
         <v>262</v>
       </c>
       <c r="L62" s="42" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="B20:B21"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="C20:L20"/>
     <mergeCell ref="C3:L3"/>
     <mergeCell ref="C9:L9"/>
+    <mergeCell ref="C21:J21"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="B16:B17"/>
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="K13:L18"/>
     <mergeCell ref="C19:L19"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="C4:L4"/>
     <mergeCell ref="K2:L2"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="C8:J8"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="I11:J12"/>
+    <mergeCell ref="C17:J17"/>
     <mergeCell ref="J61:J62"/>
     <mergeCell ref="J52:J53"/>
     <mergeCell ref="C43:H43"/>
@@ -7601,7 +7617,6 @@
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="F49:H49"/>
     <mergeCell ref="I59:I60"/>
-    <mergeCell ref="C21:J21"/>
     <mergeCell ref="C37:L37"/>
     <mergeCell ref="C38:L38"/>
     <mergeCell ref="J40:K40"/>
@@ -7617,6 +7632,7 @@
     <mergeCell ref="C26:L26"/>
     <mergeCell ref="C27:L27"/>
     <mergeCell ref="C28:L28"/>
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="B57:B58"/>
     <mergeCell ref="A57:A58"/>
     <mergeCell ref="A55:A56"/>
@@ -7643,22 +7659,6 @@
     <mergeCell ref="C32:L32"/>
     <mergeCell ref="C35:L35"/>
     <mergeCell ref="C34:I34"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C8:J8"/>
-    <mergeCell ref="C10:J10"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="I11:J12"/>
-    <mergeCell ref="C17:J17"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7670,10 +7670,10 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:XFB56"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="I45" sqref="I45"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7689,13 +7689,13 @@
   <sheetData>
     <row r="1" spans="1:14" s="16" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="59" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B1" s="60" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C1" s="140" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D1" s="60" t="s">
         <v>373</v>
@@ -7725,464 +7725,464 @@
         <v>248</v>
       </c>
       <c r="M1" s="60" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="261" t="s">
+      <c r="A2" s="275" t="s">
+        <v>393</v>
+      </c>
+      <c r="B2" s="273" t="s">
         <v>394</v>
-      </c>
-      <c r="B2" s="259" t="s">
-        <v>395</v>
       </c>
       <c r="C2" s="141">
         <v>1</v>
       </c>
-      <c r="D2" s="255" t="s">
-        <v>396</v>
-      </c>
-      <c r="E2" s="255"/>
-      <c r="F2" s="255"/>
-      <c r="G2" s="255"/>
-      <c r="H2" s="255"/>
-      <c r="I2" s="255"/>
-      <c r="J2" s="255"/>
-      <c r="K2" s="255"/>
-      <c r="L2" s="255"/>
-      <c r="M2" s="256"/>
+      <c r="D2" s="270" t="s">
+        <v>395</v>
+      </c>
+      <c r="E2" s="270"/>
+      <c r="F2" s="270"/>
+      <c r="G2" s="270"/>
+      <c r="H2" s="270"/>
+      <c r="I2" s="270"/>
+      <c r="J2" s="270"/>
+      <c r="K2" s="270"/>
+      <c r="L2" s="270"/>
+      <c r="M2" s="271"/>
     </row>
     <row r="3" spans="1:14" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="175"/>
-      <c r="B3" s="250"/>
+      <c r="A3" s="246"/>
+      <c r="B3" s="265"/>
       <c r="C3" s="142">
         <v>2</v>
       </c>
-      <c r="D3" s="257" t="s">
-        <v>491</v>
-      </c>
-      <c r="E3" s="257"/>
-      <c r="F3" s="257"/>
-      <c r="G3" s="257"/>
-      <c r="H3" s="257"/>
-      <c r="I3" s="257"/>
-      <c r="J3" s="257"/>
-      <c r="K3" s="257"/>
-      <c r="L3" s="257"/>
-      <c r="M3" s="257"/>
+      <c r="D3" s="272" t="s">
+        <v>539</v>
+      </c>
+      <c r="E3" s="272"/>
+      <c r="F3" s="272"/>
+      <c r="G3" s="272"/>
+      <c r="H3" s="272"/>
+      <c r="I3" s="272"/>
+      <c r="J3" s="272"/>
+      <c r="K3" s="272"/>
+      <c r="L3" s="272"/>
+      <c r="M3" s="272"/>
       <c r="N3" s="86"/>
     </row>
     <row r="4" spans="1:14" s="16" customFormat="1" ht="120" customHeight="1">
-      <c r="A4" s="175"/>
-      <c r="B4" s="250"/>
+      <c r="A4" s="246"/>
+      <c r="B4" s="265"/>
       <c r="C4" s="142">
         <v>3</v>
       </c>
       <c r="D4" s="107" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E4" s="94" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="F4" s="94" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G4" s="44" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H4" s="112" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I4" s="46"/>
       <c r="J4" s="107" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K4" s="46"/>
       <c r="L4" s="94" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="M4" s="94" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="90" customHeight="1">
-      <c r="A5" s="262"/>
-      <c r="B5" s="260"/>
+      <c r="A5" s="276"/>
+      <c r="B5" s="274"/>
       <c r="C5" s="148">
         <v>4</v>
       </c>
-      <c r="D5" s="206"/>
-      <c r="E5" s="206"/>
-      <c r="F5" s="206"/>
-      <c r="G5" s="206"/>
-      <c r="H5" s="206"/>
-      <c r="I5" s="206"/>
-      <c r="J5" s="206"/>
-      <c r="K5" s="206"/>
-      <c r="L5" s="183"/>
+      <c r="D5" s="257"/>
+      <c r="E5" s="257"/>
+      <c r="F5" s="257"/>
+      <c r="G5" s="257"/>
+      <c r="H5" s="257"/>
+      <c r="I5" s="257"/>
+      <c r="J5" s="257"/>
+      <c r="K5" s="257"/>
+      <c r="L5" s="212"/>
       <c r="M5" s="44" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A6" s="175" t="s">
+      <c r="A6" s="246" t="s">
         <v>171</v>
       </c>
-      <c r="B6" s="250" t="s">
+      <c r="B6" s="265" t="s">
         <v>263</v>
       </c>
       <c r="C6" s="149">
         <v>1</v>
       </c>
-      <c r="D6" s="243" t="s">
+      <c r="D6" s="259" t="s">
         <v>287</v>
       </c>
-      <c r="E6" s="243"/>
-      <c r="F6" s="243"/>
-      <c r="G6" s="243"/>
-      <c r="H6" s="243"/>
-      <c r="I6" s="243"/>
-      <c r="J6" s="243"/>
-      <c r="K6" s="243"/>
-      <c r="L6" s="243"/>
-      <c r="M6" s="244"/>
+      <c r="E6" s="259"/>
+      <c r="F6" s="259"/>
+      <c r="G6" s="259"/>
+      <c r="H6" s="259"/>
+      <c r="I6" s="259"/>
+      <c r="J6" s="259"/>
+      <c r="K6" s="259"/>
+      <c r="L6" s="259"/>
+      <c r="M6" s="260"/>
     </row>
     <row r="7" spans="1:14" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A7" s="175"/>
-      <c r="B7" s="250"/>
+      <c r="A7" s="246"/>
+      <c r="B7" s="265"/>
       <c r="C7" s="142">
         <v>2</v>
       </c>
-      <c r="D7" s="245" t="s">
-        <v>490</v>
-      </c>
-      <c r="E7" s="245"/>
-      <c r="F7" s="245"/>
-      <c r="G7" s="245"/>
-      <c r="H7" s="245"/>
-      <c r="I7" s="245"/>
-      <c r="J7" s="245"/>
-      <c r="K7" s="245"/>
-      <c r="L7" s="245"/>
-      <c r="M7" s="246"/>
+      <c r="D7" s="261" t="s">
+        <v>488</v>
+      </c>
+      <c r="E7" s="261"/>
+      <c r="F7" s="261"/>
+      <c r="G7" s="261"/>
+      <c r="H7" s="261"/>
+      <c r="I7" s="261"/>
+      <c r="J7" s="261"/>
+      <c r="K7" s="261"/>
+      <c r="L7" s="261"/>
+      <c r="M7" s="262"/>
     </row>
     <row r="8" spans="1:14" s="16" customFormat="1" ht="105" customHeight="1">
-      <c r="A8" s="175"/>
-      <c r="B8" s="250"/>
+      <c r="A8" s="246"/>
+      <c r="B8" s="265"/>
       <c r="C8" s="142">
         <v>3</v>
       </c>
       <c r="D8" s="107" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E8" s="134" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="F8" s="126" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G8" s="112" t="s">
         <v>361</v>
       </c>
       <c r="H8" s="112" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="I8" s="112"/>
       <c r="J8" s="111" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="K8" s="112"/>
       <c r="L8" s="110" t="s">
         <v>297</v>
       </c>
       <c r="M8" s="123" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="75" customHeight="1">
-      <c r="A9" s="262"/>
-      <c r="B9" s="260"/>
+      <c r="A9" s="276"/>
+      <c r="B9" s="274"/>
       <c r="C9" s="143">
         <v>4</v>
       </c>
-      <c r="D9" s="206"/>
-      <c r="E9" s="183"/>
+      <c r="D9" s="257"/>
+      <c r="E9" s="212"/>
       <c r="F9" s="106" t="s">
         <v>366</v>
       </c>
-      <c r="G9" s="182"/>
-      <c r="H9" s="206"/>
-      <c r="I9" s="206"/>
-      <c r="J9" s="206"/>
-      <c r="K9" s="206"/>
-      <c r="L9" s="206"/>
-      <c r="M9" s="183"/>
+      <c r="G9" s="211"/>
+      <c r="H9" s="257"/>
+      <c r="I9" s="257"/>
+      <c r="J9" s="257"/>
+      <c r="K9" s="257"/>
+      <c r="L9" s="257"/>
+      <c r="M9" s="212"/>
     </row>
     <row r="10" spans="1:14" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A10" s="263" t="s">
+      <c r="A10" s="277" t="s">
         <v>170</v>
       </c>
-      <c r="B10" s="264" t="s">
+      <c r="B10" s="278" t="s">
         <v>264</v>
       </c>
       <c r="C10" s="149">
         <v>1</v>
       </c>
-      <c r="D10" s="243" t="s">
+      <c r="D10" s="259" t="s">
         <v>286</v>
       </c>
-      <c r="E10" s="243"/>
-      <c r="F10" s="243"/>
-      <c r="G10" s="243"/>
-      <c r="H10" s="243"/>
-      <c r="I10" s="243"/>
-      <c r="J10" s="243"/>
-      <c r="K10" s="243"/>
-      <c r="L10" s="243"/>
-      <c r="M10" s="244"/>
+      <c r="E10" s="259"/>
+      <c r="F10" s="259"/>
+      <c r="G10" s="259"/>
+      <c r="H10" s="259"/>
+      <c r="I10" s="259"/>
+      <c r="J10" s="259"/>
+      <c r="K10" s="259"/>
+      <c r="L10" s="259"/>
+      <c r="M10" s="260"/>
     </row>
     <row r="11" spans="1:14" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="175"/>
-      <c r="B11" s="250"/>
+      <c r="A11" s="246"/>
+      <c r="B11" s="265"/>
       <c r="C11" s="142">
         <v>2</v>
       </c>
-      <c r="D11" s="245" t="s">
-        <v>492</v>
-      </c>
-      <c r="E11" s="245"/>
-      <c r="F11" s="245"/>
-      <c r="G11" s="245"/>
-      <c r="H11" s="245"/>
-      <c r="I11" s="245"/>
-      <c r="J11" s="245"/>
-      <c r="K11" s="245"/>
-      <c r="L11" s="245"/>
-      <c r="M11" s="246"/>
+      <c r="D11" s="261" t="s">
+        <v>489</v>
+      </c>
+      <c r="E11" s="261"/>
+      <c r="F11" s="261"/>
+      <c r="G11" s="261"/>
+      <c r="H11" s="261"/>
+      <c r="I11" s="261"/>
+      <c r="J11" s="261"/>
+      <c r="K11" s="261"/>
+      <c r="L11" s="261"/>
+      <c r="M11" s="262"/>
     </row>
     <row r="12" spans="1:14" s="16" customFormat="1" ht="105" customHeight="1">
-      <c r="A12" s="175"/>
-      <c r="B12" s="250"/>
+      <c r="A12" s="246"/>
+      <c r="B12" s="265"/>
       <c r="C12" s="142">
         <v>3</v>
       </c>
       <c r="D12" s="90" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E12" s="134" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="F12" s="46" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G12" s="44" t="s">
         <v>360</v>
       </c>
       <c r="H12" s="112" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="I12" s="94"/>
       <c r="J12" s="111" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K12" s="110"/>
       <c r="L12" s="110" t="s">
         <v>296</v>
       </c>
       <c r="M12" s="123" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="90" customHeight="1">
-      <c r="A13" s="156"/>
-      <c r="B13" s="258"/>
+      <c r="A13" s="163"/>
+      <c r="B13" s="242"/>
       <c r="C13" s="143">
         <v>4</v>
       </c>
-      <c r="D13" s="206"/>
-      <c r="E13" s="206"/>
-      <c r="F13" s="206"/>
-      <c r="G13" s="206"/>
-      <c r="H13" s="183"/>
+      <c r="D13" s="257"/>
+      <c r="E13" s="257"/>
+      <c r="F13" s="257"/>
+      <c r="G13" s="257"/>
+      <c r="H13" s="212"/>
       <c r="I13" s="97" t="s">
         <v>367</v>
       </c>
-      <c r="J13" s="182"/>
-      <c r="K13" s="206"/>
-      <c r="L13" s="206"/>
-      <c r="M13" s="183"/>
+      <c r="J13" s="211"/>
+      <c r="K13" s="257"/>
+      <c r="L13" s="257"/>
+      <c r="M13" s="212"/>
     </row>
     <row r="14" spans="1:14" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A14" s="155" t="s">
+      <c r="A14" s="162" t="s">
         <v>169</v>
       </c>
-      <c r="B14" s="249" t="s">
+      <c r="B14" s="241" t="s">
         <v>265</v>
       </c>
       <c r="C14" s="149">
         <v>1</v>
       </c>
-      <c r="D14" s="243" t="s">
+      <c r="D14" s="259" t="s">
         <v>285</v>
       </c>
-      <c r="E14" s="243"/>
-      <c r="F14" s="243"/>
-      <c r="G14" s="243"/>
-      <c r="H14" s="243"/>
-      <c r="I14" s="243"/>
-      <c r="J14" s="243"/>
-      <c r="K14" s="243"/>
-      <c r="L14" s="243"/>
-      <c r="M14" s="244"/>
+      <c r="E14" s="259"/>
+      <c r="F14" s="259"/>
+      <c r="G14" s="259"/>
+      <c r="H14" s="259"/>
+      <c r="I14" s="259"/>
+      <c r="J14" s="259"/>
+      <c r="K14" s="259"/>
+      <c r="L14" s="259"/>
+      <c r="M14" s="260"/>
     </row>
     <row r="15" spans="1:14" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A15" s="175"/>
-      <c r="B15" s="250"/>
+      <c r="A15" s="246"/>
+      <c r="B15" s="265"/>
       <c r="C15" s="142">
         <v>2</v>
       </c>
-      <c r="D15" s="245" t="s">
-        <v>493</v>
-      </c>
-      <c r="E15" s="245"/>
-      <c r="F15" s="245"/>
-      <c r="G15" s="245"/>
-      <c r="H15" s="245"/>
-      <c r="I15" s="245"/>
-      <c r="J15" s="245"/>
-      <c r="K15" s="245"/>
-      <c r="L15" s="245"/>
-      <c r="M15" s="246"/>
+      <c r="D15" s="261" t="s">
+        <v>490</v>
+      </c>
+      <c r="E15" s="261"/>
+      <c r="F15" s="261"/>
+      <c r="G15" s="261"/>
+      <c r="H15" s="261"/>
+      <c r="I15" s="261"/>
+      <c r="J15" s="261"/>
+      <c r="K15" s="261"/>
+      <c r="L15" s="261"/>
+      <c r="M15" s="262"/>
     </row>
     <row r="16" spans="1:14" s="16" customFormat="1" ht="105" customHeight="1">
-      <c r="A16" s="175"/>
-      <c r="B16" s="250"/>
+      <c r="A16" s="246"/>
+      <c r="B16" s="265"/>
       <c r="C16" s="142">
         <v>3</v>
       </c>
       <c r="D16" s="90" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E16" s="134" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="F16" s="46" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G16" s="44" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H16" s="112" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I16" s="110"/>
       <c r="J16" s="111" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="K16" s="110"/>
       <c r="L16" s="110" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M16" s="123" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="17" spans="1:16382" ht="75" customHeight="1">
-      <c r="A17" s="156"/>
-      <c r="B17" s="258"/>
+      <c r="A17" s="163"/>
+      <c r="B17" s="242"/>
       <c r="C17" s="143">
         <v>4</v>
       </c>
-      <c r="D17" s="206"/>
-      <c r="E17" s="206"/>
-      <c r="F17" s="183"/>
+      <c r="D17" s="257"/>
+      <c r="E17" s="257"/>
+      <c r="F17" s="212"/>
       <c r="G17" s="97" t="s">
         <v>316</v>
       </c>
-      <c r="H17" s="182"/>
-      <c r="I17" s="206"/>
-      <c r="J17" s="206"/>
-      <c r="K17" s="206"/>
-      <c r="L17" s="206"/>
-      <c r="M17" s="183"/>
+      <c r="H17" s="211"/>
+      <c r="I17" s="257"/>
+      <c r="J17" s="257"/>
+      <c r="K17" s="257"/>
+      <c r="L17" s="257"/>
+      <c r="M17" s="212"/>
     </row>
     <row r="18" spans="1:16382" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A18" s="155" t="s">
+      <c r="A18" s="162" t="s">
         <v>168</v>
       </c>
-      <c r="B18" s="249" t="s">
+      <c r="B18" s="241" t="s">
         <v>266</v>
       </c>
       <c r="C18" s="149">
         <v>1</v>
       </c>
-      <c r="D18" s="243" t="s">
-        <v>437</v>
-      </c>
-      <c r="E18" s="243"/>
-      <c r="F18" s="243"/>
-      <c r="G18" s="243"/>
-      <c r="H18" s="243"/>
-      <c r="I18" s="243"/>
-      <c r="J18" s="243"/>
-      <c r="K18" s="243"/>
-      <c r="L18" s="243"/>
-      <c r="M18" s="244"/>
+      <c r="D18" s="259" t="s">
+        <v>436</v>
+      </c>
+      <c r="E18" s="259"/>
+      <c r="F18" s="259"/>
+      <c r="G18" s="259"/>
+      <c r="H18" s="259"/>
+      <c r="I18" s="259"/>
+      <c r="J18" s="259"/>
+      <c r="K18" s="259"/>
+      <c r="L18" s="259"/>
+      <c r="M18" s="260"/>
     </row>
     <row r="19" spans="1:16382" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A19" s="175"/>
-      <c r="B19" s="250"/>
+      <c r="A19" s="246"/>
+      <c r="B19" s="265"/>
       <c r="C19" s="142">
         <v>2</v>
       </c>
-      <c r="D19" s="245" t="s">
-        <v>494</v>
-      </c>
-      <c r="E19" s="245"/>
-      <c r="F19" s="245"/>
-      <c r="G19" s="245"/>
-      <c r="H19" s="245"/>
-      <c r="I19" s="245"/>
-      <c r="J19" s="245"/>
-      <c r="K19" s="245"/>
-      <c r="L19" s="245"/>
-      <c r="M19" s="246"/>
+      <c r="D19" s="261" t="s">
+        <v>491</v>
+      </c>
+      <c r="E19" s="261"/>
+      <c r="F19" s="261"/>
+      <c r="G19" s="261"/>
+      <c r="H19" s="261"/>
+      <c r="I19" s="261"/>
+      <c r="J19" s="261"/>
+      <c r="K19" s="261"/>
+      <c r="L19" s="261"/>
+      <c r="M19" s="262"/>
     </row>
     <row r="20" spans="1:16382" s="16" customFormat="1" ht="105" customHeight="1">
-      <c r="A20" s="175"/>
-      <c r="B20" s="250"/>
+      <c r="A20" s="246"/>
+      <c r="B20" s="265"/>
       <c r="C20" s="142">
         <v>3</v>
       </c>
       <c r="D20" s="90" t="s">
+        <v>428</v>
+      </c>
+      <c r="E20" s="134" t="s">
+        <v>511</v>
+      </c>
+      <c r="F20" s="110" t="s">
+        <v>467</v>
+      </c>
+      <c r="G20" s="110" t="s">
         <v>429</v>
       </c>
-      <c r="E20" s="134" t="s">
-        <v>514</v>
-      </c>
-      <c r="F20" s="110" t="s">
-        <v>468</v>
-      </c>
-      <c r="G20" s="110" t="s">
-        <v>430</v>
-      </c>
       <c r="H20" s="112" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I20" s="110"/>
       <c r="J20" s="111" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K20" s="110"/>
       <c r="L20" s="110" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="M20" s="123" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="21" spans="1:16382" s="65" customFormat="1" ht="60" customHeight="1">
-      <c r="A21" s="254"/>
-      <c r="B21" s="251"/>
+      <c r="A21" s="269"/>
+      <c r="B21" s="266"/>
       <c r="C21" s="143">
         <v>4</v>
       </c>
@@ -8190,14 +8190,14 @@
       <c r="E21" s="121" t="s">
         <v>365</v>
       </c>
-      <c r="F21" s="213"/>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214"/>
-      <c r="J21" s="214"/>
-      <c r="K21" s="214"/>
-      <c r="L21" s="214"/>
-      <c r="M21" s="266"/>
+      <c r="F21" s="280"/>
+      <c r="G21" s="281"/>
+      <c r="H21" s="281"/>
+      <c r="I21" s="281"/>
+      <c r="J21" s="281"/>
+      <c r="K21" s="281"/>
+      <c r="L21" s="281"/>
+      <c r="M21" s="282"/>
       <c r="N21" s="68"/>
       <c r="O21" s="68"/>
       <c r="P21" s="68"/>
@@ -24569,365 +24569,365 @@
       <c r="XFB21" s="68"/>
     </row>
     <row r="22" spans="1:16382" s="66" customFormat="1" ht="15" customHeight="1">
-      <c r="A22" s="253" t="s">
+      <c r="A22" s="268" t="s">
         <v>167</v>
       </c>
-      <c r="B22" s="252" t="s">
-        <v>445</v>
+      <c r="B22" s="267" t="s">
+        <v>444</v>
       </c>
       <c r="C22" s="149">
         <v>1</v>
       </c>
-      <c r="D22" s="245" t="s">
+      <c r="D22" s="261" t="s">
         <v>284</v>
       </c>
-      <c r="E22" s="245"/>
-      <c r="F22" s="245"/>
-      <c r="G22" s="245"/>
-      <c r="H22" s="245"/>
-      <c r="I22" s="245"/>
-      <c r="J22" s="245"/>
-      <c r="K22" s="245"/>
-      <c r="L22" s="245"/>
-      <c r="M22" s="246"/>
+      <c r="E22" s="261"/>
+      <c r="F22" s="261"/>
+      <c r="G22" s="261"/>
+      <c r="H22" s="261"/>
+      <c r="I22" s="261"/>
+      <c r="J22" s="261"/>
+      <c r="K22" s="261"/>
+      <c r="L22" s="261"/>
+      <c r="M22" s="262"/>
     </row>
     <row r="23" spans="1:16382" s="66" customFormat="1" ht="15" customHeight="1">
-      <c r="A23" s="239"/>
-      <c r="B23" s="176"/>
+      <c r="A23" s="254"/>
+      <c r="B23" s="185"/>
       <c r="C23" s="142">
         <v>2</v>
       </c>
-      <c r="D23" s="245" t="s">
-        <v>495</v>
-      </c>
-      <c r="E23" s="245"/>
-      <c r="F23" s="245"/>
-      <c r="G23" s="245"/>
-      <c r="H23" s="245"/>
-      <c r="I23" s="245"/>
-      <c r="J23" s="245"/>
-      <c r="K23" s="245"/>
-      <c r="L23" s="245"/>
-      <c r="M23" s="246"/>
+      <c r="D23" s="261" t="s">
+        <v>492</v>
+      </c>
+      <c r="E23" s="261"/>
+      <c r="F23" s="261"/>
+      <c r="G23" s="261"/>
+      <c r="H23" s="261"/>
+      <c r="I23" s="261"/>
+      <c r="J23" s="261"/>
+      <c r="K23" s="261"/>
+      <c r="L23" s="261"/>
+      <c r="M23" s="262"/>
     </row>
     <row r="24" spans="1:16382" s="66" customFormat="1" ht="105" customHeight="1">
-      <c r="A24" s="239"/>
-      <c r="B24" s="176"/>
+      <c r="A24" s="254"/>
+      <c r="B24" s="185"/>
       <c r="C24" s="142">
         <v>3</v>
       </c>
       <c r="D24" s="93" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E24" s="134"/>
       <c r="F24" s="110" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G24" s="110" t="s">
         <v>364</v>
       </c>
       <c r="H24" s="110" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="I24" s="110"/>
       <c r="J24" s="111" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="K24" s="110"/>
       <c r="L24" s="110" t="s">
         <v>295</v>
       </c>
       <c r="M24" s="123" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="25" spans="1:16382" s="68" customFormat="1" ht="90" customHeight="1">
-      <c r="A25" s="242"/>
-      <c r="B25" s="164"/>
+      <c r="A25" s="258"/>
+      <c r="B25" s="171"/>
       <c r="C25" s="143">
         <v>4</v>
       </c>
       <c r="D25" s="96" t="s">
         <v>368</v>
       </c>
-      <c r="E25" s="182"/>
-      <c r="F25" s="206"/>
-      <c r="G25" s="206"/>
-      <c r="H25" s="206"/>
-      <c r="I25" s="206"/>
-      <c r="J25" s="206"/>
-      <c r="K25" s="206"/>
-      <c r="L25" s="206"/>
-      <c r="M25" s="183"/>
+      <c r="E25" s="211"/>
+      <c r="F25" s="257"/>
+      <c r="G25" s="257"/>
+      <c r="H25" s="257"/>
+      <c r="I25" s="257"/>
+      <c r="J25" s="257"/>
+      <c r="K25" s="257"/>
+      <c r="L25" s="257"/>
+      <c r="M25" s="212"/>
     </row>
     <row r="26" spans="1:16382" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A26" s="241" t="s">
+      <c r="A26" s="256" t="s">
         <v>166</v>
       </c>
-      <c r="B26" s="163" t="s">
-        <v>446</v>
+      <c r="B26" s="170" t="s">
+        <v>445</v>
       </c>
       <c r="C26" s="149">
         <v>1</v>
       </c>
-      <c r="D26" s="243" t="s">
+      <c r="D26" s="259" t="s">
         <v>283</v>
       </c>
-      <c r="E26" s="243"/>
-      <c r="F26" s="243"/>
-      <c r="G26" s="243"/>
-      <c r="H26" s="243"/>
-      <c r="I26" s="243"/>
-      <c r="J26" s="243"/>
-      <c r="K26" s="243"/>
-      <c r="L26" s="243"/>
-      <c r="M26" s="244"/>
+      <c r="E26" s="259"/>
+      <c r="F26" s="259"/>
+      <c r="G26" s="259"/>
+      <c r="H26" s="259"/>
+      <c r="I26" s="259"/>
+      <c r="J26" s="259"/>
+      <c r="K26" s="259"/>
+      <c r="L26" s="259"/>
+      <c r="M26" s="260"/>
     </row>
     <row r="27" spans="1:16382" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A27" s="239"/>
-      <c r="B27" s="176"/>
+      <c r="A27" s="254"/>
+      <c r="B27" s="185"/>
       <c r="C27" s="142">
         <v>2</v>
       </c>
-      <c r="D27" s="245" t="s">
-        <v>496</v>
-      </c>
-      <c r="E27" s="245"/>
-      <c r="F27" s="245"/>
-      <c r="G27" s="245"/>
-      <c r="H27" s="245"/>
-      <c r="I27" s="245"/>
-      <c r="J27" s="245"/>
-      <c r="K27" s="245"/>
-      <c r="L27" s="245"/>
-      <c r="M27" s="246"/>
+      <c r="D27" s="261" t="s">
+        <v>493</v>
+      </c>
+      <c r="E27" s="261"/>
+      <c r="F27" s="261"/>
+      <c r="G27" s="261"/>
+      <c r="H27" s="261"/>
+      <c r="I27" s="261"/>
+      <c r="J27" s="261"/>
+      <c r="K27" s="261"/>
+      <c r="L27" s="261"/>
+      <c r="M27" s="262"/>
     </row>
     <row r="28" spans="1:16382" s="16" customFormat="1" ht="105" customHeight="1">
-      <c r="A28" s="239"/>
-      <c r="B28" s="176"/>
+      <c r="A28" s="254"/>
+      <c r="B28" s="185"/>
       <c r="C28" s="142">
         <v>3</v>
       </c>
       <c r="D28" s="93" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E28" s="94"/>
       <c r="F28" s="110" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G28" s="94" t="s">
         <v>363</v>
       </c>
       <c r="H28" s="126" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="I28" s="110"/>
       <c r="J28" s="110" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="K28" s="110"/>
       <c r="L28" s="110"/>
       <c r="M28" s="123" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="29" spans="1:16382" ht="60" customHeight="1">
-      <c r="A29" s="242"/>
-      <c r="B29" s="164"/>
+      <c r="A29" s="258"/>
+      <c r="B29" s="171"/>
       <c r="C29" s="143">
         <v>4</v>
       </c>
-      <c r="D29" s="206"/>
-      <c r="E29" s="206"/>
-      <c r="F29" s="206"/>
-      <c r="G29" s="183"/>
+      <c r="D29" s="257"/>
+      <c r="E29" s="257"/>
+      <c r="F29" s="257"/>
+      <c r="G29" s="212"/>
       <c r="H29" s="88" t="s">
         <v>300</v>
       </c>
-      <c r="I29" s="182"/>
-      <c r="J29" s="206"/>
-      <c r="K29" s="206"/>
-      <c r="L29" s="206"/>
-      <c r="M29" s="183"/>
+      <c r="I29" s="211"/>
+      <c r="J29" s="257"/>
+      <c r="K29" s="257"/>
+      <c r="L29" s="257"/>
+      <c r="M29" s="212"/>
     </row>
     <row r="30" spans="1:16382" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A30" s="241" t="s">
+      <c r="A30" s="256" t="s">
         <v>273</v>
       </c>
-      <c r="B30" s="163" t="s">
-        <v>447</v>
+      <c r="B30" s="170" t="s">
+        <v>446</v>
       </c>
       <c r="C30" s="149">
         <v>1</v>
       </c>
-      <c r="D30" s="243" t="s">
+      <c r="D30" s="259" t="s">
         <v>293</v>
       </c>
-      <c r="E30" s="243"/>
-      <c r="F30" s="243"/>
-      <c r="G30" s="243"/>
-      <c r="H30" s="243"/>
-      <c r="I30" s="243"/>
-      <c r="J30" s="243"/>
-      <c r="K30" s="243"/>
-      <c r="L30" s="243"/>
-      <c r="M30" s="244"/>
+      <c r="E30" s="259"/>
+      <c r="F30" s="259"/>
+      <c r="G30" s="259"/>
+      <c r="H30" s="259"/>
+      <c r="I30" s="259"/>
+      <c r="J30" s="259"/>
+      <c r="K30" s="259"/>
+      <c r="L30" s="259"/>
+      <c r="M30" s="260"/>
     </row>
     <row r="31" spans="1:16382" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A31" s="239"/>
-      <c r="B31" s="176"/>
+      <c r="A31" s="254"/>
+      <c r="B31" s="185"/>
       <c r="C31" s="142">
         <v>2</v>
       </c>
-      <c r="D31" s="245" t="s">
-        <v>497</v>
-      </c>
-      <c r="E31" s="245"/>
-      <c r="F31" s="245"/>
-      <c r="G31" s="245"/>
-      <c r="H31" s="245"/>
-      <c r="I31" s="245"/>
-      <c r="J31" s="245"/>
-      <c r="K31" s="245"/>
-      <c r="L31" s="245"/>
-      <c r="M31" s="246"/>
+      <c r="D31" s="261" t="s">
+        <v>494</v>
+      </c>
+      <c r="E31" s="261"/>
+      <c r="F31" s="261"/>
+      <c r="G31" s="261"/>
+      <c r="H31" s="261"/>
+      <c r="I31" s="261"/>
+      <c r="J31" s="261"/>
+      <c r="K31" s="261"/>
+      <c r="L31" s="261"/>
+      <c r="M31" s="262"/>
     </row>
     <row r="32" spans="1:16382" ht="105" customHeight="1">
-      <c r="A32" s="239"/>
-      <c r="B32" s="176"/>
+      <c r="A32" s="254"/>
+      <c r="B32" s="185"/>
       <c r="C32" s="142">
         <v>3</v>
       </c>
       <c r="D32" s="93" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E32" s="44"/>
       <c r="F32" s="110" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G32" s="44" t="s">
         <v>362</v>
       </c>
       <c r="H32" s="126" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="I32" s="44"/>
       <c r="J32" s="94" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K32" s="44"/>
       <c r="L32" s="79" t="s">
         <v>298</v>
       </c>
       <c r="M32" s="123" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="33" spans="1:13" s="16" customFormat="1" ht="45" customHeight="1">
-      <c r="A33" s="239"/>
-      <c r="B33" s="176"/>
+      <c r="A33" s="254"/>
+      <c r="B33" s="185"/>
       <c r="C33" s="143">
         <v>4</v>
       </c>
-      <c r="D33" s="206"/>
-      <c r="E33" s="206"/>
-      <c r="F33" s="206"/>
-      <c r="G33" s="206"/>
-      <c r="H33" s="206"/>
-      <c r="I33" s="206"/>
-      <c r="J33" s="206"/>
-      <c r="K33" s="183"/>
+      <c r="D33" s="257"/>
+      <c r="E33" s="257"/>
+      <c r="F33" s="257"/>
+      <c r="G33" s="257"/>
+      <c r="H33" s="257"/>
+      <c r="I33" s="257"/>
+      <c r="J33" s="257"/>
+      <c r="K33" s="212"/>
       <c r="L33" s="46" t="s">
         <v>358</v>
       </c>
       <c r="M33" s="57"/>
     </row>
     <row r="34" spans="1:13" ht="15" customHeight="1">
-      <c r="A34" s="238" t="s">
+      <c r="A34" s="253" t="s">
         <v>165</v>
       </c>
-      <c r="B34" s="201" t="s">
-        <v>448</v>
+      <c r="B34" s="200" t="s">
+        <v>447</v>
       </c>
       <c r="C34" s="149">
         <v>1</v>
       </c>
-      <c r="D34" s="243" t="s">
+      <c r="D34" s="259" t="s">
         <v>282</v>
       </c>
-      <c r="E34" s="243"/>
-      <c r="F34" s="243"/>
-      <c r="G34" s="243"/>
-      <c r="H34" s="243"/>
-      <c r="I34" s="243"/>
-      <c r="J34" s="243"/>
-      <c r="K34" s="243"/>
-      <c r="L34" s="243"/>
-      <c r="M34" s="244"/>
+      <c r="E34" s="259"/>
+      <c r="F34" s="259"/>
+      <c r="G34" s="259"/>
+      <c r="H34" s="259"/>
+      <c r="I34" s="259"/>
+      <c r="J34" s="259"/>
+      <c r="K34" s="259"/>
+      <c r="L34" s="259"/>
+      <c r="M34" s="260"/>
     </row>
     <row r="35" spans="1:13" ht="15" customHeight="1">
-      <c r="A35" s="239"/>
-      <c r="B35" s="176"/>
+      <c r="A35" s="254"/>
+      <c r="B35" s="185"/>
       <c r="C35" s="142">
         <v>2</v>
       </c>
-      <c r="D35" s="245" t="s">
-        <v>498</v>
-      </c>
-      <c r="E35" s="245"/>
-      <c r="F35" s="245"/>
-      <c r="G35" s="245"/>
-      <c r="H35" s="245"/>
-      <c r="I35" s="245"/>
-      <c r="J35" s="245"/>
-      <c r="K35" s="245"/>
-      <c r="L35" s="245"/>
-      <c r="M35" s="246"/>
+      <c r="D35" s="261" t="s">
+        <v>495</v>
+      </c>
+      <c r="E35" s="261"/>
+      <c r="F35" s="261"/>
+      <c r="G35" s="261"/>
+      <c r="H35" s="261"/>
+      <c r="I35" s="261"/>
+      <c r="J35" s="261"/>
+      <c r="K35" s="261"/>
+      <c r="L35" s="261"/>
+      <c r="M35" s="262"/>
     </row>
     <row r="36" spans="1:13" ht="105" customHeight="1">
-      <c r="A36" s="239"/>
-      <c r="B36" s="176"/>
+      <c r="A36" s="254"/>
+      <c r="B36" s="185"/>
       <c r="C36" s="142">
         <v>3</v>
       </c>
       <c r="D36" s="93" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E36" s="94"/>
       <c r="F36" s="110" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G36" s="94" t="s">
         <v>372</v>
       </c>
       <c r="H36" s="94" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="I36" s="94"/>
       <c r="J36" s="94" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="K36" s="94"/>
       <c r="L36" s="110" t="s">
         <v>299</v>
       </c>
       <c r="M36" s="123" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="37" spans="1:13" s="16" customFormat="1" ht="45" customHeight="1">
-      <c r="A37" s="242"/>
-      <c r="B37" s="164"/>
+      <c r="A37" s="258"/>
+      <c r="B37" s="171"/>
       <c r="C37" s="143">
         <v>4</v>
       </c>
-      <c r="D37" s="206"/>
-      <c r="E37" s="206"/>
-      <c r="F37" s="206"/>
-      <c r="G37" s="206"/>
-      <c r="H37" s="206"/>
-      <c r="I37" s="206"/>
-      <c r="J37" s="183"/>
+      <c r="D37" s="257"/>
+      <c r="E37" s="257"/>
+      <c r="F37" s="257"/>
+      <c r="G37" s="257"/>
+      <c r="H37" s="257"/>
+      <c r="I37" s="257"/>
+      <c r="J37" s="212"/>
       <c r="K37" s="88" t="s">
         <v>357</v>
       </c>
@@ -24935,31 +24935,31 @@
       <c r="M37" s="108"/>
     </row>
     <row r="38" spans="1:13" s="68" customFormat="1" ht="15" customHeight="1">
-      <c r="A38" s="241" t="s">
+      <c r="A38" s="256" t="s">
         <v>164</v>
       </c>
-      <c r="B38" s="163" t="s">
+      <c r="B38" s="170" t="s">
         <v>275</v>
       </c>
       <c r="C38" s="142">
         <v>1</v>
       </c>
-      <c r="D38" s="247" t="s">
+      <c r="D38" s="263" t="s">
         <v>278</v>
       </c>
-      <c r="E38" s="248"/>
-      <c r="F38" s="248"/>
-      <c r="G38" s="248"/>
-      <c r="H38" s="248"/>
-      <c r="I38" s="248"/>
-      <c r="J38" s="248"/>
-      <c r="K38" s="248"/>
-      <c r="L38" s="248"/>
-      <c r="M38" s="248"/>
+      <c r="E38" s="264"/>
+      <c r="F38" s="264"/>
+      <c r="G38" s="264"/>
+      <c r="H38" s="264"/>
+      <c r="I38" s="264"/>
+      <c r="J38" s="264"/>
+      <c r="K38" s="264"/>
+      <c r="L38" s="264"/>
+      <c r="M38" s="264"/>
     </row>
     <row r="39" spans="1:13" s="66" customFormat="1" ht="120" customHeight="1">
-      <c r="A39" s="240"/>
-      <c r="B39" s="202"/>
+      <c r="A39" s="255"/>
+      <c r="B39" s="201"/>
       <c r="C39" s="142">
         <v>4</v>
       </c>
@@ -24971,7 +24971,7 @@
       </c>
       <c r="F39" s="99"/>
       <c r="G39" s="99" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H39" s="67"/>
       <c r="I39" s="67"/>
@@ -24981,31 +24981,31 @@
       <c r="M39" s="67"/>
     </row>
     <row r="40" spans="1:13" s="68" customFormat="1" ht="15" customHeight="1">
-      <c r="A40" s="238" t="s">
+      <c r="A40" s="253" t="s">
         <v>163</v>
       </c>
-      <c r="B40" s="201" t="s">
+      <c r="B40" s="200" t="s">
         <v>274</v>
       </c>
       <c r="C40" s="144">
         <v>1</v>
       </c>
-      <c r="D40" s="244" t="s">
+      <c r="D40" s="260" t="s">
         <v>279</v>
       </c>
-      <c r="E40" s="265"/>
-      <c r="F40" s="265"/>
-      <c r="G40" s="265"/>
-      <c r="H40" s="265"/>
-      <c r="I40" s="265"/>
-      <c r="J40" s="265"/>
-      <c r="K40" s="265"/>
-      <c r="L40" s="265"/>
-      <c r="M40" s="265"/>
+      <c r="E40" s="279"/>
+      <c r="F40" s="279"/>
+      <c r="G40" s="279"/>
+      <c r="H40" s="279"/>
+      <c r="I40" s="279"/>
+      <c r="J40" s="279"/>
+      <c r="K40" s="279"/>
+      <c r="L40" s="279"/>
+      <c r="M40" s="279"/>
     </row>
     <row r="41" spans="1:13" s="16" customFormat="1" ht="150" customHeight="1">
-      <c r="A41" s="240"/>
-      <c r="B41" s="202"/>
+      <c r="A41" s="255"/>
+      <c r="B41" s="201"/>
       <c r="C41" s="142">
         <v>4</v>
       </c>
@@ -25017,7 +25017,7 @@
       </c>
       <c r="F41" s="99"/>
       <c r="G41" s="99" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H41" s="67"/>
       <c r="I41" s="67"/>
@@ -25027,31 +25027,31 @@
       <c r="M41" s="67"/>
     </row>
     <row r="42" spans="1:13" s="68" customFormat="1" ht="15" customHeight="1">
-      <c r="A42" s="238" t="s">
+      <c r="A42" s="253" t="s">
         <v>162</v>
       </c>
-      <c r="B42" s="201" t="s">
+      <c r="B42" s="200" t="s">
         <v>276</v>
       </c>
       <c r="C42" s="144">
         <v>1</v>
       </c>
-      <c r="D42" s="244" t="s">
+      <c r="D42" s="260" t="s">
         <v>280</v>
       </c>
-      <c r="E42" s="265"/>
-      <c r="F42" s="265"/>
-      <c r="G42" s="265"/>
-      <c r="H42" s="265"/>
-      <c r="I42" s="265"/>
-      <c r="J42" s="265"/>
-      <c r="K42" s="265"/>
-      <c r="L42" s="265"/>
-      <c r="M42" s="265"/>
+      <c r="E42" s="279"/>
+      <c r="F42" s="279"/>
+      <c r="G42" s="279"/>
+      <c r="H42" s="279"/>
+      <c r="I42" s="279"/>
+      <c r="J42" s="279"/>
+      <c r="K42" s="279"/>
+      <c r="L42" s="279"/>
+      <c r="M42" s="279"/>
     </row>
     <row r="43" spans="1:13" s="98" customFormat="1" ht="225" customHeight="1">
-      <c r="A43" s="239"/>
-      <c r="B43" s="202"/>
+      <c r="A43" s="254"/>
+      <c r="B43" s="201"/>
       <c r="C43" s="150">
         <v>4</v>
       </c>
@@ -25063,7 +25063,7 @@
       </c>
       <c r="F43" s="99"/>
       <c r="G43" s="99" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H43" s="67"/>
       <c r="I43" s="67"/>
@@ -25073,54 +25073,54 @@
       <c r="M43" s="67"/>
     </row>
     <row r="44" spans="1:13" s="68" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A44" s="235" t="s">
+      <c r="A44" s="250" t="s">
         <v>161</v>
       </c>
-      <c r="B44" s="176" t="s">
+      <c r="B44" s="185" t="s">
         <v>277</v>
       </c>
       <c r="C44" s="142">
         <v>1</v>
       </c>
-      <c r="D44" s="244" t="s">
+      <c r="D44" s="260" t="s">
         <v>281</v>
       </c>
-      <c r="E44" s="265"/>
-      <c r="F44" s="265"/>
-      <c r="G44" s="265"/>
-      <c r="H44" s="265"/>
-      <c r="I44" s="265"/>
-      <c r="J44" s="265"/>
-      <c r="K44" s="265"/>
-      <c r="L44" s="265"/>
-      <c r="M44" s="265"/>
+      <c r="E44" s="279"/>
+      <c r="F44" s="279"/>
+      <c r="G44" s="279"/>
+      <c r="H44" s="279"/>
+      <c r="I44" s="279"/>
+      <c r="J44" s="279"/>
+      <c r="K44" s="279"/>
+      <c r="L44" s="279"/>
+      <c r="M44" s="279"/>
     </row>
     <row r="45" spans="1:13" ht="300" customHeight="1">
-      <c r="A45" s="236"/>
-      <c r="B45" s="237"/>
+      <c r="A45" s="251"/>
+      <c r="B45" s="252"/>
       <c r="C45" s="145">
         <v>4</v>
       </c>
       <c r="D45" s="70" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="E45" s="72" t="s">
         <v>294</v>
       </c>
       <c r="F45" s="72" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G45" s="72" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="H45" s="72" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="I45" s="70" t="s">
         <v>291</v>
       </c>
       <c r="J45" s="70" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="K45" s="64" t="s">
         <v>317</v>
@@ -25129,7 +25129,7 @@
         <v>292</v>
       </c>
       <c r="M45" s="70" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="46" spans="1:13">

</xml_diff>